<commit_message>
FIX: função que detecta falso positivo e negativo
</commit_message>
<xml_diff>
--- a/storage/app/public/GRR_BASICO.xlsx
+++ b/storage/app/public/GRR_BASICO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" state="visible" r:id="rId3"/>
@@ -16261,8 +16261,8 @@
   </sheetPr>
   <dimension ref="A1:AN930"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL20" activeCellId="0" sqref="AL20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X34" activeCellId="0" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16996,75 +16996,75 @@
         <v/>
       </c>
       <c r="K13" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K13="","",IF('Data Entry'!K13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L13" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L13="","",IF('Data Entry'!L13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M13" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M13="","",IF('Data Entry'!M13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N13" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N13="","",IF('Data Entry'!N13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O13" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O13="","",IF('Data Entry'!O13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P13" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P13="","",IF('Data Entry'!P13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q13="","",IF('Data Entry'!Q13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R13" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R13="","",IF('Data Entry'!R13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S13" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S13="","",IF('Data Entry'!S13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T13" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T13="","",IF('Data Entry'!T13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U13" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U13="","",IF('Data Entry'!U13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V13" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V13="","",IF('Data Entry'!V13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W13" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W13="","",IF('Data Entry'!W13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X13" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X13="","",IF('Data Entry'!X13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y13" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y13="","",IF('Data Entry'!Y13='Data Entry'!$D13,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K13="","",IF('Data Entry'!K13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L13="","",IF('Data Entry'!L13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M13="","",IF('Data Entry'!M13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N13="","",IF('Data Entry'!N13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O13="","",IF('Data Entry'!O13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P13="","",IF('Data Entry'!P13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q13="","",IF('Data Entry'!Q13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R13="","",IF('Data Entry'!R13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S13="","",IF('Data Entry'!S13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T13="","",IF('Data Entry'!T13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U13="","",IF('Data Entry'!U13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V13="","",IF('Data Entry'!V13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W13="","",IF('Data Entry'!W13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X13="","",IF('Data Entry'!X13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y13="","",IF('Data Entry'!Y13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z13" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z13="","",IF('Data Entry'!Z13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA13" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA13="","",IF('Data Entry'!AA13='Data Entry'!$D13,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB13" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB13="","",IF('Data Entry'!AB13='Data Entry'!$D13,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z13="","",IF('Data Entry'!Z13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA13="","",IF('Data Entry'!AA13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB13" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB13="","",IF('Data Entry'!AB13='Data Entry'!$D13,1,IF('Data Entry'!$D13="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC13" s="99" t="str">
@@ -17124,75 +17124,75 @@
         <v/>
       </c>
       <c r="K14" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K14="","",IF('Data Entry'!K14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L14" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L14="","",IF('Data Entry'!L14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M14" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M14="","",IF('Data Entry'!M14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N14" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N14="","",IF('Data Entry'!N14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O14" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O14="","",IF('Data Entry'!O14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P14" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P14="","",IF('Data Entry'!P14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q14="","",IF('Data Entry'!Q14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R14" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R14="","",IF('Data Entry'!R14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S14" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S14="","",IF('Data Entry'!S14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T14" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T14="","",IF('Data Entry'!T14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U14" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U14="","",IF('Data Entry'!U14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V14" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V14="","",IF('Data Entry'!V14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W14" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W14="","",IF('Data Entry'!W14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X14" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X14="","",IF('Data Entry'!X14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y14" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y14="","",IF('Data Entry'!Y14='Data Entry'!$D14,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K14="","",IF('Data Entry'!K14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L14="","",IF('Data Entry'!L14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M14="","",IF('Data Entry'!M14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N14="","",IF('Data Entry'!N14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O14="","",IF('Data Entry'!O14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P14="","",IF('Data Entry'!P14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q14="","",IF('Data Entry'!Q14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R14="","",IF('Data Entry'!R14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S14="","",IF('Data Entry'!S14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T14="","",IF('Data Entry'!T14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U14="","",IF('Data Entry'!U14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V14="","",IF('Data Entry'!V14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W14="","",IF('Data Entry'!W14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X14="","",IF('Data Entry'!X14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y14="","",IF('Data Entry'!Y14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z14" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z14="","",IF('Data Entry'!Z14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA14" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA14="","",IF('Data Entry'!AA14='Data Entry'!$D14,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB14" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB14="","",IF('Data Entry'!AB14='Data Entry'!$D14,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z14="","",IF('Data Entry'!Z14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA14="","",IF('Data Entry'!AA14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB14" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB14="","",IF('Data Entry'!AB14='Data Entry'!$D14,1,IF('Data Entry'!$D14="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC14" s="99" t="str">
@@ -17252,75 +17252,75 @@
         <v/>
       </c>
       <c r="K15" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K15="","",IF('Data Entry'!K15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L15" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L15="","",IF('Data Entry'!L15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M15" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M15="","",IF('Data Entry'!M15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N15" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N15="","",IF('Data Entry'!N15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O15" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O15="","",IF('Data Entry'!O15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P15" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P15="","",IF('Data Entry'!P15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q15="","",IF('Data Entry'!Q15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R15" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R15="","",IF('Data Entry'!R15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S15" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S15="","",IF('Data Entry'!S15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T15" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T15="","",IF('Data Entry'!T15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U15" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U15="","",IF('Data Entry'!U15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V15" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V15="","",IF('Data Entry'!V15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W15" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W15="","",IF('Data Entry'!W15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X15" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X15="","",IF('Data Entry'!X15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y15" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y15="","",IF('Data Entry'!Y15='Data Entry'!$D15,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K15="","",IF('Data Entry'!K15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L15="","",IF('Data Entry'!L15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M15="","",IF('Data Entry'!M15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N15="","",IF('Data Entry'!N15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O15="","",IF('Data Entry'!O15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P15="","",IF('Data Entry'!P15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q15="","",IF('Data Entry'!Q15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R15="","",IF('Data Entry'!R15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S15="","",IF('Data Entry'!S15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T15="","",IF('Data Entry'!T15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U15="","",IF('Data Entry'!U15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V15="","",IF('Data Entry'!V15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W15="","",IF('Data Entry'!W15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X15="","",IF('Data Entry'!X15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y15="","",IF('Data Entry'!Y15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z15" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z15="","",IF('Data Entry'!Z15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA15" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA15="","",IF('Data Entry'!AA15='Data Entry'!$D15,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB15" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB15="","",IF('Data Entry'!AB15='Data Entry'!$D15,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z15="","",IF('Data Entry'!Z15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA15="","",IF('Data Entry'!AA15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB15" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB15="","",IF('Data Entry'!AB15='Data Entry'!$D15,1,IF('Data Entry'!$D15="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC15" s="99" t="str">
@@ -17380,75 +17380,75 @@
         <v/>
       </c>
       <c r="K16" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K16="","",IF('Data Entry'!K16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L16" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L16="","",IF('Data Entry'!L16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M16" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M16="","",IF('Data Entry'!M16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N16" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N16="","",IF('Data Entry'!N16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O16" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O16="","",IF('Data Entry'!O16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P16" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P16="","",IF('Data Entry'!P16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q16="","",IF('Data Entry'!Q16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R16" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R16="","",IF('Data Entry'!R16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S16" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S16="","",IF('Data Entry'!S16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T16" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T16="","",IF('Data Entry'!T16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U16" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U16="","",IF('Data Entry'!U16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V16" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V16="","",IF('Data Entry'!V16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W16" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W16="","",IF('Data Entry'!W16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X16" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X16="","",IF('Data Entry'!X16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y16" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y16="","",IF('Data Entry'!Y16='Data Entry'!$D16,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K16="","",IF('Data Entry'!K16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L16="","",IF('Data Entry'!L16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M16="","",IF('Data Entry'!M16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N16="","",IF('Data Entry'!N16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O16="","",IF('Data Entry'!O16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P16="","",IF('Data Entry'!P16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q16="","",IF('Data Entry'!Q16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R16="","",IF('Data Entry'!R16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S16="","",IF('Data Entry'!S16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T16="","",IF('Data Entry'!T16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U16="","",IF('Data Entry'!U16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V16="","",IF('Data Entry'!V16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W16="","",IF('Data Entry'!W16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X16="","",IF('Data Entry'!X16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y16="","",IF('Data Entry'!Y16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z16" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z16="","",IF('Data Entry'!Z16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA16" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA16="","",IF('Data Entry'!AA16='Data Entry'!$D16,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB16" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB16="","",IF('Data Entry'!AB16='Data Entry'!$D16,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z16="","",IF('Data Entry'!Z16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA16="","",IF('Data Entry'!AA16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB16" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB16="","",IF('Data Entry'!AB16='Data Entry'!$D16,1,IF('Data Entry'!$D16="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC16" s="99" t="str">
@@ -17508,75 +17508,75 @@
         <v/>
       </c>
       <c r="K17" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K17="","",IF('Data Entry'!K17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L17" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L17="","",IF('Data Entry'!L17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M17" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M17="","",IF('Data Entry'!M17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N17" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N17="","",IF('Data Entry'!N17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O17" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O17="","",IF('Data Entry'!O17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P17" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P17="","",IF('Data Entry'!P17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q17="","",IF('Data Entry'!Q17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R17" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R17="","",IF('Data Entry'!R17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S17" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S17="","",IF('Data Entry'!S17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T17" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T17="","",IF('Data Entry'!T17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U17" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U17="","",IF('Data Entry'!U17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V17" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V17="","",IF('Data Entry'!V17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W17" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W17="","",IF('Data Entry'!W17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X17" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X17="","",IF('Data Entry'!X17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y17" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y17="","",IF('Data Entry'!Y17='Data Entry'!$D17,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K17="","",IF('Data Entry'!K17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L17="","",IF('Data Entry'!L17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M17="","",IF('Data Entry'!M17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N17="","",IF('Data Entry'!N17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O17="","",IF('Data Entry'!O17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P17="","",IF('Data Entry'!P17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q17="","",IF('Data Entry'!Q17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R17="","",IF('Data Entry'!R17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S17="","",IF('Data Entry'!S17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T17="","",IF('Data Entry'!T17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U17="","",IF('Data Entry'!U17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V17="","",IF('Data Entry'!V17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W17="","",IF('Data Entry'!W17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X17="","",IF('Data Entry'!X17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y17="","",IF('Data Entry'!Y17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z17" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z17="","",IF('Data Entry'!Z17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA17" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA17="","",IF('Data Entry'!AA17='Data Entry'!$D17,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB17" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB17="","",IF('Data Entry'!AB17='Data Entry'!$D17,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z17="","",IF('Data Entry'!Z17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA17="","",IF('Data Entry'!AA17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB17" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB17="","",IF('Data Entry'!AB17='Data Entry'!$D17,1,IF('Data Entry'!$D17="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC17" s="99" t="str">
@@ -17636,75 +17636,75 @@
         <v/>
       </c>
       <c r="K18" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K18="","",IF('Data Entry'!K18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L18" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L18="","",IF('Data Entry'!L18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M18" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M18="","",IF('Data Entry'!M18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N18" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N18="","",IF('Data Entry'!N18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O18" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O18="","",IF('Data Entry'!O18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P18" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P18="","",IF('Data Entry'!P18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q18="","",IF('Data Entry'!Q18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R18" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R18="","",IF('Data Entry'!R18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S18" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S18="","",IF('Data Entry'!S18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T18" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T18="","",IF('Data Entry'!T18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U18" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U18="","",IF('Data Entry'!U18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V18" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V18="","",IF('Data Entry'!V18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W18" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W18="","",IF('Data Entry'!W18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X18" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X18="","",IF('Data Entry'!X18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y18" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y18="","",IF('Data Entry'!Y18='Data Entry'!$D18,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K18="","",IF('Data Entry'!K18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L18="","",IF('Data Entry'!L18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M18="","",IF('Data Entry'!M18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N18="","",IF('Data Entry'!N18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O18="","",IF('Data Entry'!O18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P18="","",IF('Data Entry'!P18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q18="","",IF('Data Entry'!Q18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R18="","",IF('Data Entry'!R18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S18="","",IF('Data Entry'!S18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T18="","",IF('Data Entry'!T18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U18="","",IF('Data Entry'!U18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V18="","",IF('Data Entry'!V18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W18="","",IF('Data Entry'!W18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X18="","",IF('Data Entry'!X18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y18="","",IF('Data Entry'!Y18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z18" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z18="","",IF('Data Entry'!Z18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA18" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA18="","",IF('Data Entry'!AA18='Data Entry'!$D18,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB18" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB18="","",IF('Data Entry'!AB18='Data Entry'!$D18,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z18="","",IF('Data Entry'!Z18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA18="","",IF('Data Entry'!AA18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB18" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB18="","",IF('Data Entry'!AB18='Data Entry'!$D18,1,IF('Data Entry'!$D18="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC18" s="99" t="str">
@@ -17764,75 +17764,75 @@
         <v/>
       </c>
       <c r="K19" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K19="","",IF('Data Entry'!K19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L19" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L19="","",IF('Data Entry'!L19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M19" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M19="","",IF('Data Entry'!M19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N19" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N19="","",IF('Data Entry'!N19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O19" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O19="","",IF('Data Entry'!O19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P19" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P19="","",IF('Data Entry'!P19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q19="","",IF('Data Entry'!Q19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R19" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R19="","",IF('Data Entry'!R19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S19" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S19="","",IF('Data Entry'!S19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T19" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T19="","",IF('Data Entry'!T19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U19" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U19="","",IF('Data Entry'!U19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V19" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V19="","",IF('Data Entry'!V19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W19" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W19="","",IF('Data Entry'!W19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X19" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X19="","",IF('Data Entry'!X19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y19" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y19="","",IF('Data Entry'!Y19='Data Entry'!$D19,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K19="","",IF('Data Entry'!K19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L19="","",IF('Data Entry'!L19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M19="","",IF('Data Entry'!M19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N19="","",IF('Data Entry'!N19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O19="","",IF('Data Entry'!O19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P19="","",IF('Data Entry'!P19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q19="","",IF('Data Entry'!Q19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R19="","",IF('Data Entry'!R19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S19="","",IF('Data Entry'!S19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T19="","",IF('Data Entry'!T19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U19="","",IF('Data Entry'!U19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V19="","",IF('Data Entry'!V19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W19="","",IF('Data Entry'!W19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X19="","",IF('Data Entry'!X19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y19="","",IF('Data Entry'!Y19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z19" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z19="","",IF('Data Entry'!Z19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA19" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA19="","",IF('Data Entry'!AA19='Data Entry'!$D19,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB19" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB19="","",IF('Data Entry'!AB19='Data Entry'!$D19,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z19="","",IF('Data Entry'!Z19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA19="","",IF('Data Entry'!AA19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB19" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB19="","",IF('Data Entry'!AB19='Data Entry'!$D19,1,IF('Data Entry'!$D19="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC19" s="99" t="str">
@@ -17892,75 +17892,75 @@
         <v/>
       </c>
       <c r="K20" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K20="","",IF('Data Entry'!K20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L20" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L20="","",IF('Data Entry'!L20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M20" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M20="","",IF('Data Entry'!M20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N20" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N20="","",IF('Data Entry'!N20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O20" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O20="","",IF('Data Entry'!O20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P20" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P20="","",IF('Data Entry'!P20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q20="","",IF('Data Entry'!Q20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R20" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R20="","",IF('Data Entry'!R20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S20" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S20="","",IF('Data Entry'!S20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T20" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T20="","",IF('Data Entry'!T20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U20" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U20="","",IF('Data Entry'!U20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V20" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V20="","",IF('Data Entry'!V20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W20" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W20="","",IF('Data Entry'!W20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X20" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X20="","",IF('Data Entry'!X20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y20" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y20="","",IF('Data Entry'!Y20='Data Entry'!$D20,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K20="","",IF('Data Entry'!K20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L20="","",IF('Data Entry'!L20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M20="","",IF('Data Entry'!M20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N20="","",IF('Data Entry'!N20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O20="","",IF('Data Entry'!O20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P20="","",IF('Data Entry'!P20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q20="","",IF('Data Entry'!Q20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R20="","",IF('Data Entry'!R20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S20="","",IF('Data Entry'!S20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T20="","",IF('Data Entry'!T20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U20="","",IF('Data Entry'!U20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V20="","",IF('Data Entry'!V20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W20="","",IF('Data Entry'!W20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X20="","",IF('Data Entry'!X20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y20="","",IF('Data Entry'!Y20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z20" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z20="","",IF('Data Entry'!Z20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA20" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA20="","",IF('Data Entry'!AA20='Data Entry'!$D20,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB20" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB20="","",IF('Data Entry'!AB20='Data Entry'!$D20,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z20="","",IF('Data Entry'!Z20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA20="","",IF('Data Entry'!AA20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB20" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB20="","",IF('Data Entry'!AB20='Data Entry'!$D20,1,IF('Data Entry'!$D20="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC20" s="99" t="str">
@@ -18020,75 +18020,75 @@
         <v/>
       </c>
       <c r="K21" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K21="","",IF('Data Entry'!K21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L21" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L21="","",IF('Data Entry'!L21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M21" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M21="","",IF('Data Entry'!M21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N21" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N21="","",IF('Data Entry'!N21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O21" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O21="","",IF('Data Entry'!O21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P21" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P21="","",IF('Data Entry'!P21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q21="","",IF('Data Entry'!Q21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R21" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R21="","",IF('Data Entry'!R21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S21" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S21="","",IF('Data Entry'!S21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T21" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T21="","",IF('Data Entry'!T21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U21" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U21="","",IF('Data Entry'!U21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V21" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V21="","",IF('Data Entry'!V21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W21" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W21="","",IF('Data Entry'!W21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X21" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X21="","",IF('Data Entry'!X21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y21" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y21="","",IF('Data Entry'!Y21='Data Entry'!$D21,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K21="","",IF('Data Entry'!K21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L21="","",IF('Data Entry'!L21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M21="","",IF('Data Entry'!M21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N21="","",IF('Data Entry'!N21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O21="","",IF('Data Entry'!O21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P21="","",IF('Data Entry'!P21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q21="","",IF('Data Entry'!Q21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R21="","",IF('Data Entry'!R21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S21="","",IF('Data Entry'!S21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T21="","",IF('Data Entry'!T21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U21="","",IF('Data Entry'!U21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V21="","",IF('Data Entry'!V21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W21="","",IF('Data Entry'!W21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X21="","",IF('Data Entry'!X21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y21="","",IF('Data Entry'!Y21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z21" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z21="","",IF('Data Entry'!Z21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA21" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA21="","",IF('Data Entry'!AA21='Data Entry'!$D21,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB21" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB21="","",IF('Data Entry'!AB21='Data Entry'!$D21,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z21="","",IF('Data Entry'!Z21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA21="","",IF('Data Entry'!AA21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB21" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB21="","",IF('Data Entry'!AB21='Data Entry'!$D21,1,IF('Data Entry'!$D21="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC21" s="99" t="str">
@@ -18148,75 +18148,75 @@
         <v/>
       </c>
       <c r="K22" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K22="","",IF('Data Entry'!K22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L22" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L22="","",IF('Data Entry'!L22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M22" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M22="","",IF('Data Entry'!M22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N22" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N22="","",IF('Data Entry'!N22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O22" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O22="","",IF('Data Entry'!O22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P22" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P22="","",IF('Data Entry'!P22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q22="","",IF('Data Entry'!Q22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R22" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R22="","",IF('Data Entry'!R22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S22" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S22="","",IF('Data Entry'!S22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T22" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T22="","",IF('Data Entry'!T22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U22" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U22="","",IF('Data Entry'!U22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V22" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V22="","",IF('Data Entry'!V22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W22" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W22="","",IF('Data Entry'!W22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X22" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X22="","",IF('Data Entry'!X22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y22" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y22="","",IF('Data Entry'!Y22='Data Entry'!$D22,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K22="","",IF('Data Entry'!K22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L22="","",IF('Data Entry'!L22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M22="","",IF('Data Entry'!M22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N22="","",IF('Data Entry'!N22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O22="","",IF('Data Entry'!O22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P22="","",IF('Data Entry'!P22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q22="","",IF('Data Entry'!Q22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R22="","",IF('Data Entry'!R22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S22="","",IF('Data Entry'!S22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T22="","",IF('Data Entry'!T22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U22="","",IF('Data Entry'!U22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V22="","",IF('Data Entry'!V22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W22="","",IF('Data Entry'!W22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X22="","",IF('Data Entry'!X22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y22="","",IF('Data Entry'!Y22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z22" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z22="","",IF('Data Entry'!Z22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA22" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA22="","",IF('Data Entry'!AA22='Data Entry'!$D22,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB22" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB22="","",IF('Data Entry'!AB22='Data Entry'!$D22,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z22="","",IF('Data Entry'!Z22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA22="","",IF('Data Entry'!AA22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB22" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB22="","",IF('Data Entry'!AB22='Data Entry'!$D22,1,IF('Data Entry'!$D22="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC22" s="99" t="str">
@@ -18276,75 +18276,75 @@
         <v/>
       </c>
       <c r="K23" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K23="","",IF('Data Entry'!K23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L23" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L23="","",IF('Data Entry'!L23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M23" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M23="","",IF('Data Entry'!M23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N23" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N23="","",IF('Data Entry'!N23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O23" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O23="","",IF('Data Entry'!O23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P23" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P23="","",IF('Data Entry'!P23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q23="","",IF('Data Entry'!Q23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R23" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R23="","",IF('Data Entry'!R23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S23" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S23="","",IF('Data Entry'!S23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T23" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T23="","",IF('Data Entry'!T23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U23" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U23="","",IF('Data Entry'!U23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V23" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V23="","",IF('Data Entry'!V23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W23" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W23="","",IF('Data Entry'!W23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X23" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X23="","",IF('Data Entry'!X23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y23" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y23="","",IF('Data Entry'!Y23='Data Entry'!$D23,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K23="","",IF('Data Entry'!K23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L23="","",IF('Data Entry'!L23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M23="","",IF('Data Entry'!M23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N23="","",IF('Data Entry'!N23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O23="","",IF('Data Entry'!O23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P23="","",IF('Data Entry'!P23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q23="","",IF('Data Entry'!Q23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R23="","",IF('Data Entry'!R23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S23="","",IF('Data Entry'!S23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T23="","",IF('Data Entry'!T23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U23="","",IF('Data Entry'!U23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V23="","",IF('Data Entry'!V23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W23="","",IF('Data Entry'!W23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X23="","",IF('Data Entry'!X23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y23="","",IF('Data Entry'!Y23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z23" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z23="","",IF('Data Entry'!Z23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA23" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA23="","",IF('Data Entry'!AA23='Data Entry'!$D23,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB23" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB23="","",IF('Data Entry'!AB23='Data Entry'!$D23,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z23="","",IF('Data Entry'!Z23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA23="","",IF('Data Entry'!AA23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB23" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB23="","",IF('Data Entry'!AB23='Data Entry'!$D23,1,IF('Data Entry'!$D23="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC23" s="99" t="str">
@@ -18404,75 +18404,75 @@
         <v/>
       </c>
       <c r="K24" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K24="","",IF('Data Entry'!K24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L24" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L24="","",IF('Data Entry'!L24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M24" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M24="","",IF('Data Entry'!M24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N24" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N24="","",IF('Data Entry'!N24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O24" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O24="","",IF('Data Entry'!O24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P24" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P24="","",IF('Data Entry'!P24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q24="","",IF('Data Entry'!Q24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R24" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R24="","",IF('Data Entry'!R24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S24" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S24="","",IF('Data Entry'!S24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T24" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T24="","",IF('Data Entry'!T24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U24" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U24="","",IF('Data Entry'!U24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V24" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V24="","",IF('Data Entry'!V24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W24" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W24="","",IF('Data Entry'!W24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X24" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X24="","",IF('Data Entry'!X24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y24" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y24="","",IF('Data Entry'!Y24='Data Entry'!$D24,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K24="","",IF('Data Entry'!K24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L24="","",IF('Data Entry'!L24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M24="","",IF('Data Entry'!M24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N24="","",IF('Data Entry'!N24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O24="","",IF('Data Entry'!O24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P24="","",IF('Data Entry'!P24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q24="","",IF('Data Entry'!Q24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R24="","",IF('Data Entry'!R24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S24="","",IF('Data Entry'!S24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T24="","",IF('Data Entry'!T24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U24="","",IF('Data Entry'!U24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V24="","",IF('Data Entry'!V24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W24="","",IF('Data Entry'!W24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X24="","",IF('Data Entry'!X24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y24="","",IF('Data Entry'!Y24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z24" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z24="","",IF('Data Entry'!Z24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA24" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA24="","",IF('Data Entry'!AA24='Data Entry'!$D24,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB24" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB24="","",IF('Data Entry'!AB24='Data Entry'!$D24,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z24="","",IF('Data Entry'!Z24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA24="","",IF('Data Entry'!AA24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB24" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB24="","",IF('Data Entry'!AB24='Data Entry'!$D24,1,IF('Data Entry'!$D24="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC24" s="99" t="str">
@@ -18532,75 +18532,75 @@
         <v/>
       </c>
       <c r="K25" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K25="","",IF('Data Entry'!K25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L25" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L25="","",IF('Data Entry'!L25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M25" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M25="","",IF('Data Entry'!M25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N25" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N25="","",IF('Data Entry'!N25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O25" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O25="","",IF('Data Entry'!O25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P25" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P25="","",IF('Data Entry'!P25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q25="","",IF('Data Entry'!Q25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R25" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R25="","",IF('Data Entry'!R25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S25" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S25="","",IF('Data Entry'!S25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T25" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T25="","",IF('Data Entry'!T25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U25" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U25="","",IF('Data Entry'!U25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V25" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V25="","",IF('Data Entry'!V25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W25" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W25="","",IF('Data Entry'!W25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X25" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X25="","",IF('Data Entry'!X25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y25" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y25="","",IF('Data Entry'!Y25='Data Entry'!$D25,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K25="","",IF('Data Entry'!K25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L25="","",IF('Data Entry'!L25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M25="","",IF('Data Entry'!M25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N25="","",IF('Data Entry'!N25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O25="","",IF('Data Entry'!O25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P25="","",IF('Data Entry'!P25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q25="","",IF('Data Entry'!Q25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R25="","",IF('Data Entry'!R25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S25="","",IF('Data Entry'!S25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T25="","",IF('Data Entry'!T25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U25="","",IF('Data Entry'!U25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V25="","",IF('Data Entry'!V25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W25="","",IF('Data Entry'!W25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X25="","",IF('Data Entry'!X25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y25="","",IF('Data Entry'!Y25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z25" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z25="","",IF('Data Entry'!Z25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA25" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA25="","",IF('Data Entry'!AA25='Data Entry'!$D25,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB25" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB25="","",IF('Data Entry'!AB25='Data Entry'!$D25,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z25="","",IF('Data Entry'!Z25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA25="","",IF('Data Entry'!AA25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB25" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB25="","",IF('Data Entry'!AB25='Data Entry'!$D25,1,IF('Data Entry'!$D25="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC25" s="99" t="str">
@@ -18660,75 +18660,75 @@
         <v/>
       </c>
       <c r="K26" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K26="","",IF('Data Entry'!K26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L26" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L26="","",IF('Data Entry'!L26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M26" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M26="","",IF('Data Entry'!M26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N26" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N26="","",IF('Data Entry'!N26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O26" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O26="","",IF('Data Entry'!O26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P26" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P26="","",IF('Data Entry'!P26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q26="","",IF('Data Entry'!Q26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R26" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R26="","",IF('Data Entry'!R26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S26" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S26="","",IF('Data Entry'!S26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T26" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T26="","",IF('Data Entry'!T26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U26" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U26="","",IF('Data Entry'!U26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V26" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V26="","",IF('Data Entry'!V26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W26" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W26="","",IF('Data Entry'!W26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X26" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X26="","",IF('Data Entry'!X26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y26" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y26="","",IF('Data Entry'!Y26='Data Entry'!$D26,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K26="","",IF('Data Entry'!K26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L26="","",IF('Data Entry'!L26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M26="","",IF('Data Entry'!M26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N26="","",IF('Data Entry'!N26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O26="","",IF('Data Entry'!O26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P26="","",IF('Data Entry'!P26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q26="","",IF('Data Entry'!Q26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R26="","",IF('Data Entry'!R26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S26="","",IF('Data Entry'!S26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T26="","",IF('Data Entry'!T26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U26="","",IF('Data Entry'!U26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V26="","",IF('Data Entry'!V26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W26="","",IF('Data Entry'!W26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X26="","",IF('Data Entry'!X26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y26="","",IF('Data Entry'!Y26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z26" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z26="","",IF('Data Entry'!Z26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA26" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA26="","",IF('Data Entry'!AA26='Data Entry'!$D26,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB26" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB26="","",IF('Data Entry'!AB26='Data Entry'!$D26,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z26="","",IF('Data Entry'!Z26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA26="","",IF('Data Entry'!AA26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB26" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB26="","",IF('Data Entry'!AB26='Data Entry'!$D26,1,IF('Data Entry'!$D26="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC26" s="99" t="str">
@@ -18788,75 +18788,75 @@
         <v/>
       </c>
       <c r="K27" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K27="","",IF('Data Entry'!K27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L27" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L27="","",IF('Data Entry'!L27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M27" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M27="","",IF('Data Entry'!M27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N27" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N27="","",IF('Data Entry'!N27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O27" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O27="","",IF('Data Entry'!O27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P27" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P27="","",IF('Data Entry'!P27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q27="","",IF('Data Entry'!Q27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R27" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R27="","",IF('Data Entry'!R27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S27" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S27="","",IF('Data Entry'!S27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T27" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T27="","",IF('Data Entry'!T27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U27" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U27="","",IF('Data Entry'!U27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V27" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V27="","",IF('Data Entry'!V27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W27" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W27="","",IF('Data Entry'!W27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X27" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X27="","",IF('Data Entry'!X27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y27" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y27="","",IF('Data Entry'!Y27='Data Entry'!$D27,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K27="","",IF('Data Entry'!K27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L27="","",IF('Data Entry'!L27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M27="","",IF('Data Entry'!M27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N27="","",IF('Data Entry'!N27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O27="","",IF('Data Entry'!O27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P27="","",IF('Data Entry'!P27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q27="","",IF('Data Entry'!Q27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R27="","",IF('Data Entry'!R27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S27="","",IF('Data Entry'!S27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T27="","",IF('Data Entry'!T27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U27="","",IF('Data Entry'!U27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V27="","",IF('Data Entry'!V27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W27="","",IF('Data Entry'!W27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X27="","",IF('Data Entry'!X27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y27="","",IF('Data Entry'!Y27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z27" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z27="","",IF('Data Entry'!Z27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA27" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA27="","",IF('Data Entry'!AA27='Data Entry'!$D27,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB27" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB27="","",IF('Data Entry'!AB27='Data Entry'!$D27,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z27="","",IF('Data Entry'!Z27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA27="","",IF('Data Entry'!AA27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB27" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB27="","",IF('Data Entry'!AB27='Data Entry'!$D27,1,IF('Data Entry'!$D27="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC27" s="99" t="str">
@@ -18916,75 +18916,75 @@
         <v/>
       </c>
       <c r="K28" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K28="","",IF('Data Entry'!K28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L28" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L28="","",IF('Data Entry'!L28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M28" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M28="","",IF('Data Entry'!M28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N28" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N28="","",IF('Data Entry'!N28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O28" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O28="","",IF('Data Entry'!O28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P28" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P28="","",IF('Data Entry'!P28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q28="","",IF('Data Entry'!Q28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R28" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R28="","",IF('Data Entry'!R28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S28" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S28="","",IF('Data Entry'!S28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T28" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T28="","",IF('Data Entry'!T28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U28" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U28="","",IF('Data Entry'!U28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V28" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V28="","",IF('Data Entry'!V28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W28" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W28="","",IF('Data Entry'!W28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X28" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X28="","",IF('Data Entry'!X28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y28" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y28="","",IF('Data Entry'!Y28='Data Entry'!$D28,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K28="","",IF('Data Entry'!K28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L28="","",IF('Data Entry'!L28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M28="","",IF('Data Entry'!M28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N28="","",IF('Data Entry'!N28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O28="","",IF('Data Entry'!O28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P28="","",IF('Data Entry'!P28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q28="","",IF('Data Entry'!Q28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R28="","",IF('Data Entry'!R28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S28="","",IF('Data Entry'!S28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T28="","",IF('Data Entry'!T28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U28="","",IF('Data Entry'!U28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V28="","",IF('Data Entry'!V28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W28="","",IF('Data Entry'!W28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X28="","",IF('Data Entry'!X28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y28="","",IF('Data Entry'!Y28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z28" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z28="","",IF('Data Entry'!Z28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA28" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA28="","",IF('Data Entry'!AA28='Data Entry'!$D28,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB28" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB28="","",IF('Data Entry'!AB28='Data Entry'!$D28,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z28="","",IF('Data Entry'!Z28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA28="","",IF('Data Entry'!AA28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB28" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB28="","",IF('Data Entry'!AB28='Data Entry'!$D28,1,IF('Data Entry'!$D28="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC28" s="99" t="str">
@@ -19044,75 +19044,75 @@
         <v/>
       </c>
       <c r="K29" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K29="","",IF('Data Entry'!K29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L29" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L29="","",IF('Data Entry'!L29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M29" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M29="","",IF('Data Entry'!M29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N29" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N29="","",IF('Data Entry'!N29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O29" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O29="","",IF('Data Entry'!O29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P29" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P29="","",IF('Data Entry'!P29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q29="","",IF('Data Entry'!Q29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R29" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R29="","",IF('Data Entry'!R29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S29" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S29="","",IF('Data Entry'!S29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T29" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T29="","",IF('Data Entry'!T29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U29" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U29="","",IF('Data Entry'!U29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V29" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V29="","",IF('Data Entry'!V29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W29" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W29="","",IF('Data Entry'!W29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X29" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X29="","",IF('Data Entry'!X29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y29" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y29="","",IF('Data Entry'!Y29='Data Entry'!$D29,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K29="","",IF('Data Entry'!K29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L29="","",IF('Data Entry'!L29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M29="","",IF('Data Entry'!M29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N29="","",IF('Data Entry'!N29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O29="","",IF('Data Entry'!O29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P29="","",IF('Data Entry'!P29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q29="","",IF('Data Entry'!Q29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R29="","",IF('Data Entry'!R29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S29="","",IF('Data Entry'!S29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T29="","",IF('Data Entry'!T29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U29="","",IF('Data Entry'!U29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V29="","",IF('Data Entry'!V29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W29="","",IF('Data Entry'!W29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X29="","",IF('Data Entry'!X29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y29="","",IF('Data Entry'!Y29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z29" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z29="","",IF('Data Entry'!Z29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA29" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA29="","",IF('Data Entry'!AA29='Data Entry'!$D29,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB29" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB29="","",IF('Data Entry'!AB29='Data Entry'!$D29,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z29="","",IF('Data Entry'!Z29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA29="","",IF('Data Entry'!AA29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB29" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB29="","",IF('Data Entry'!AB29='Data Entry'!$D29,1,IF('Data Entry'!$D29="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC29" s="99" t="str">
@@ -19172,75 +19172,75 @@
         <v/>
       </c>
       <c r="K30" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K30="","",IF('Data Entry'!K30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L30" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L30="","",IF('Data Entry'!L30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M30" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M30="","",IF('Data Entry'!M30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N30" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N30="","",IF('Data Entry'!N30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O30" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O30="","",IF('Data Entry'!O30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P30" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P30="","",IF('Data Entry'!P30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q30="","",IF('Data Entry'!Q30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R30" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R30="","",IF('Data Entry'!R30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S30" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S30="","",IF('Data Entry'!S30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T30" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T30="","",IF('Data Entry'!T30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U30" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U30="","",IF('Data Entry'!U30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V30" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V30="","",IF('Data Entry'!V30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W30" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W30="","",IF('Data Entry'!W30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X30" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X30="","",IF('Data Entry'!X30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y30" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y30="","",IF('Data Entry'!Y30='Data Entry'!$D30,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K30="","",IF('Data Entry'!K30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L30="","",IF('Data Entry'!L30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M30="","",IF('Data Entry'!M30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N30="","",IF('Data Entry'!N30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O30="","",IF('Data Entry'!O30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P30="","",IF('Data Entry'!P30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q30="","",IF('Data Entry'!Q30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R30="","",IF('Data Entry'!R30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S30="","",IF('Data Entry'!S30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T30="","",IF('Data Entry'!T30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U30="","",IF('Data Entry'!U30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V30="","",IF('Data Entry'!V30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W30="","",IF('Data Entry'!W30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X30="","",IF('Data Entry'!X30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y30="","",IF('Data Entry'!Y30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z30" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z30="","",IF('Data Entry'!Z30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA30" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA30="","",IF('Data Entry'!AA30='Data Entry'!$D30,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB30" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB30="","",IF('Data Entry'!AB30='Data Entry'!$D30,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z30="","",IF('Data Entry'!Z30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA30="","",IF('Data Entry'!AA30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB30" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB30="","",IF('Data Entry'!AB30='Data Entry'!$D30,1,IF('Data Entry'!$D30="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC30" s="99" t="str">
@@ -19300,75 +19300,75 @@
         <v/>
       </c>
       <c r="K31" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K31="","",IF('Data Entry'!K31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L31" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L31="","",IF('Data Entry'!L31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M31" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M31="","",IF('Data Entry'!M31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N31" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N31="","",IF('Data Entry'!N31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O31" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O31="","",IF('Data Entry'!O31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P31" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P31="","",IF('Data Entry'!P31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q31="","",IF('Data Entry'!Q31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R31" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R31="","",IF('Data Entry'!R31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S31" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S31="","",IF('Data Entry'!S31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T31" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T31="","",IF('Data Entry'!T31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U31" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U31="","",IF('Data Entry'!U31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V31" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V31="","",IF('Data Entry'!V31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W31" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W31="","",IF('Data Entry'!W31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X31" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X31="","",IF('Data Entry'!X31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y31" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y31="","",IF('Data Entry'!Y31='Data Entry'!$D31,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K31="","",IF('Data Entry'!K31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L31="","",IF('Data Entry'!L31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M31="","",IF('Data Entry'!M31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N31="","",IF('Data Entry'!N31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O31="","",IF('Data Entry'!O31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P31="","",IF('Data Entry'!P31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q31="","",IF('Data Entry'!Q31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R31="","",IF('Data Entry'!R31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S31="","",IF('Data Entry'!S31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T31="","",IF('Data Entry'!T31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U31="","",IF('Data Entry'!U31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V31="","",IF('Data Entry'!V31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W31="","",IF('Data Entry'!W31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X31="","",IF('Data Entry'!X31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y31="","",IF('Data Entry'!Y31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z31" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z31="","",IF('Data Entry'!Z31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA31" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA31="","",IF('Data Entry'!AA31='Data Entry'!$D31,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB31" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB31="","",IF('Data Entry'!AB31='Data Entry'!$D31,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z31="","",IF('Data Entry'!Z31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA31="","",IF('Data Entry'!AA31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB31" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB31="","",IF('Data Entry'!AB31='Data Entry'!$D31,1,IF('Data Entry'!$D31="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC31" s="99" t="str">
@@ -19428,75 +19428,75 @@
         <v/>
       </c>
       <c r="K32" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K32="","",IF('Data Entry'!K32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L32" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L32="","",IF('Data Entry'!L32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M32" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M32="","",IF('Data Entry'!M32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N32" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N32="","",IF('Data Entry'!N32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O32" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O32="","",IF('Data Entry'!O32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P32" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P32="","",IF('Data Entry'!P32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q32="","",IF('Data Entry'!Q32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R32" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R32="","",IF('Data Entry'!R32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S32" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S32="","",IF('Data Entry'!S32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T32" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T32="","",IF('Data Entry'!T32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U32" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U32="","",IF('Data Entry'!U32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V32" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V32="","",IF('Data Entry'!V32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W32" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W32="","",IF('Data Entry'!W32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X32" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X32="","",IF('Data Entry'!X32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y32" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y32="","",IF('Data Entry'!Y32='Data Entry'!$D32,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K32="","",IF('Data Entry'!K32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L32="","",IF('Data Entry'!L32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M32="","",IF('Data Entry'!M32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N32="","",IF('Data Entry'!N32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O32="","",IF('Data Entry'!O32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P32="","",IF('Data Entry'!P32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q32="","",IF('Data Entry'!Q32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R32="","",IF('Data Entry'!R32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S32="","",IF('Data Entry'!S32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T32="","",IF('Data Entry'!T32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U32="","",IF('Data Entry'!U32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V32="","",IF('Data Entry'!V32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W32="","",IF('Data Entry'!W32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X32="","",IF('Data Entry'!X32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y32="","",IF('Data Entry'!Y32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z32" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z32="","",IF('Data Entry'!Z32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA32" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA32="","",IF('Data Entry'!AA32='Data Entry'!$D32,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB32" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB32="","",IF('Data Entry'!AB32='Data Entry'!$D32,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z32="","",IF('Data Entry'!Z32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA32="","",IF('Data Entry'!AA32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB32" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB32="","",IF('Data Entry'!AB32='Data Entry'!$D32,1,IF('Data Entry'!$D32="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC32" s="99" t="str">
@@ -19556,75 +19556,75 @@
         <v/>
       </c>
       <c r="K33" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K33="","",IF('Data Entry'!K33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L33" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L33="","",IF('Data Entry'!L33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M33" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M33="","",IF('Data Entry'!M33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N33" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N33="","",IF('Data Entry'!N33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O33" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O33="","",IF('Data Entry'!O33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P33" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P33="","",IF('Data Entry'!P33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q33" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q33="","",IF('Data Entry'!Q33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R33" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R33="","",IF('Data Entry'!R33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S33" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S33="","",IF('Data Entry'!S33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T33" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T33="","",IF('Data Entry'!T33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U33" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U33="","",IF('Data Entry'!U33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V33" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V33="","",IF('Data Entry'!V33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W33" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W33="","",IF('Data Entry'!W33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X33" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X33="","",IF('Data Entry'!X33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y33" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y33="","",IF('Data Entry'!Y33='Data Entry'!$D33,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K33="","",IF('Data Entry'!K33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L33="","",IF('Data Entry'!L33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M33="","",IF('Data Entry'!M33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N33="","",IF('Data Entry'!N33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O33="","",IF('Data Entry'!O33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P33="","",IF('Data Entry'!P33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q33="","",IF('Data Entry'!Q33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R33="","",IF('Data Entry'!R33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S33="","",IF('Data Entry'!S33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T33="","",IF('Data Entry'!T33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U33="","",IF('Data Entry'!U33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V33="","",IF('Data Entry'!V33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W33="","",IF('Data Entry'!W33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X33="","",IF('Data Entry'!X33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y33="","",IF('Data Entry'!Y33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z33" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z33="","",IF('Data Entry'!Z33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA33" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA33="","",IF('Data Entry'!AA33='Data Entry'!$D33,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB33" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB33="","",IF('Data Entry'!AB33='Data Entry'!$D33,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z33="","",IF('Data Entry'!Z33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA33="","",IF('Data Entry'!AA33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB33" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB33="","",IF('Data Entry'!AB33='Data Entry'!$D33,1,IF('Data Entry'!$D33="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC33" s="99" t="str">
@@ -19684,75 +19684,75 @@
         <v/>
       </c>
       <c r="K34" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K34="","",IF('Data Entry'!K34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L34" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L34="","",IF('Data Entry'!L34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M34" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M34="","",IF('Data Entry'!M34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N34" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N34="","",IF('Data Entry'!N34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O34" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O34="","",IF('Data Entry'!O34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P34" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P34="","",IF('Data Entry'!P34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q34="","",IF('Data Entry'!Q34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R34" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R34="","",IF('Data Entry'!R34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S34" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S34="","",IF('Data Entry'!S34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T34" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T34="","",IF('Data Entry'!T34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U34" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U34="","",IF('Data Entry'!U34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V34" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V34="","",IF('Data Entry'!V34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W34" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W34="","",IF('Data Entry'!W34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X34" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X34="","",IF('Data Entry'!X34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y34" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y34="","",IF('Data Entry'!Y34='Data Entry'!$D34,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K34="","",IF('Data Entry'!K34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L34="","",IF('Data Entry'!L34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M34="","",IF('Data Entry'!M34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N34="","",IF('Data Entry'!N34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O34="","",IF('Data Entry'!O34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P34="","",IF('Data Entry'!P34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q34="","",IF('Data Entry'!Q34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R34="","",IF('Data Entry'!R34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S34="","",IF('Data Entry'!S34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T34="","",IF('Data Entry'!T34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U34="","",IF('Data Entry'!U34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V34="","",IF('Data Entry'!V34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W34="","",IF('Data Entry'!W34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X34="","",IF('Data Entry'!X34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y34="","",IF('Data Entry'!Y34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z34" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z34="","",IF('Data Entry'!Z34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA34" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA34="","",IF('Data Entry'!AA34='Data Entry'!$D34,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB34" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB34="","",IF('Data Entry'!AB34='Data Entry'!$D34,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z34="","",IF('Data Entry'!Z34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA34="","",IF('Data Entry'!AA34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB34" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB34="","",IF('Data Entry'!AB34='Data Entry'!$D34,1,IF('Data Entry'!$D34="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC34" s="99" t="str">
@@ -19812,75 +19812,75 @@
         <v/>
       </c>
       <c r="K35" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K35="","",IF('Data Entry'!K35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L35" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L35="","",IF('Data Entry'!L35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M35" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M35="","",IF('Data Entry'!M35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N35" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N35="","",IF('Data Entry'!N35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O35" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O35="","",IF('Data Entry'!O35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P35" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P35="","",IF('Data Entry'!P35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q35="","",IF('Data Entry'!Q35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R35" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R35="","",IF('Data Entry'!R35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S35" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S35="","",IF('Data Entry'!S35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T35" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T35="","",IF('Data Entry'!T35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U35" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U35="","",IF('Data Entry'!U35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V35" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V35="","",IF('Data Entry'!V35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W35" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W35="","",IF('Data Entry'!W35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X35" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X35="","",IF('Data Entry'!X35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y35" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y35="","",IF('Data Entry'!Y35='Data Entry'!$D35,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K35="","",IF('Data Entry'!K35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L35="","",IF('Data Entry'!L35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M35="","",IF('Data Entry'!M35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N35="","",IF('Data Entry'!N35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O35="","",IF('Data Entry'!O35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P35="","",IF('Data Entry'!P35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q35="","",IF('Data Entry'!Q35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R35="","",IF('Data Entry'!R35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S35="","",IF('Data Entry'!S35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T35="","",IF('Data Entry'!T35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U35="","",IF('Data Entry'!U35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V35="","",IF('Data Entry'!V35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W35="","",IF('Data Entry'!W35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X35="","",IF('Data Entry'!X35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y35="","",IF('Data Entry'!Y35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z35" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z35="","",IF('Data Entry'!Z35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA35" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA35="","",IF('Data Entry'!AA35='Data Entry'!$D35,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB35" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB35="","",IF('Data Entry'!AB35='Data Entry'!$D35,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z35="","",IF('Data Entry'!Z35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA35="","",IF('Data Entry'!AA35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB35" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB35="","",IF('Data Entry'!AB35='Data Entry'!$D35,1,IF('Data Entry'!$D35="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC35" s="99" t="str">
@@ -19940,75 +19940,75 @@
         <v/>
       </c>
       <c r="K36" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K36="","",IF('Data Entry'!K36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L36" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L36="","",IF('Data Entry'!L36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M36" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M36="","",IF('Data Entry'!M36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N36" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N36="","",IF('Data Entry'!N36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O36" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O36="","",IF('Data Entry'!O36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P36" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P36="","",IF('Data Entry'!P36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q36="","",IF('Data Entry'!Q36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R36" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R36="","",IF('Data Entry'!R36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S36" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S36="","",IF('Data Entry'!S36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T36" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T36="","",IF('Data Entry'!T36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U36" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U36="","",IF('Data Entry'!U36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V36" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V36="","",IF('Data Entry'!V36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W36" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W36="","",IF('Data Entry'!W36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X36" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X36="","",IF('Data Entry'!X36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y36" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y36="","",IF('Data Entry'!Y36='Data Entry'!$D36,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K36="","",IF('Data Entry'!K36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L36="","",IF('Data Entry'!L36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M36="","",IF('Data Entry'!M36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N36="","",IF('Data Entry'!N36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O36="","",IF('Data Entry'!O36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P36="","",IF('Data Entry'!P36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q36="","",IF('Data Entry'!Q36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R36="","",IF('Data Entry'!R36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S36="","",IF('Data Entry'!S36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T36="","",IF('Data Entry'!T36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U36="","",IF('Data Entry'!U36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V36="","",IF('Data Entry'!V36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W36="","",IF('Data Entry'!W36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X36="","",IF('Data Entry'!X36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y36="","",IF('Data Entry'!Y36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z36" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z36="","",IF('Data Entry'!Z36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA36" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA36="","",IF('Data Entry'!AA36='Data Entry'!$D36,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB36" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB36="","",IF('Data Entry'!AB36='Data Entry'!$D36,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z36="","",IF('Data Entry'!Z36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA36="","",IF('Data Entry'!AA36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB36" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB36="","",IF('Data Entry'!AB36='Data Entry'!$D36,1,IF('Data Entry'!$D36="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC36" s="99" t="str">
@@ -20068,75 +20068,75 @@
         <v/>
       </c>
       <c r="K37" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K37="","",IF('Data Entry'!K37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L37" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L37="","",IF('Data Entry'!L37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M37" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M37="","",IF('Data Entry'!M37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N37" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N37="","",IF('Data Entry'!N37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O37" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O37="","",IF('Data Entry'!O37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P37" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P37="","",IF('Data Entry'!P37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q37="","",IF('Data Entry'!Q37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R37" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R37="","",IF('Data Entry'!R37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S37" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S37="","",IF('Data Entry'!S37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T37" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T37="","",IF('Data Entry'!T37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U37" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U37="","",IF('Data Entry'!U37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V37" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V37="","",IF('Data Entry'!V37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W37" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W37="","",IF('Data Entry'!W37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X37" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X37="","",IF('Data Entry'!X37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y37" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y37="","",IF('Data Entry'!Y37='Data Entry'!$D37,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K37="","",IF('Data Entry'!K37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L37="","",IF('Data Entry'!L37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M37="","",IF('Data Entry'!M37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N37="","",IF('Data Entry'!N37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O37="","",IF('Data Entry'!O37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P37="","",IF('Data Entry'!P37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q37="","",IF('Data Entry'!Q37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R37="","",IF('Data Entry'!R37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S37="","",IF('Data Entry'!S37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T37="","",IF('Data Entry'!T37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U37="","",IF('Data Entry'!U37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V37="","",IF('Data Entry'!V37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W37="","",IF('Data Entry'!W37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X37="","",IF('Data Entry'!X37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y37="","",IF('Data Entry'!Y37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z37" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z37="","",IF('Data Entry'!Z37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA37" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA37="","",IF('Data Entry'!AA37='Data Entry'!$D37,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB37" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB37="","",IF('Data Entry'!AB37='Data Entry'!$D37,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z37="","",IF('Data Entry'!Z37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA37="","",IF('Data Entry'!AA37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB37" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB37="","",IF('Data Entry'!AB37='Data Entry'!$D37,1,IF('Data Entry'!$D37="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC37" s="99" t="str">
@@ -20196,75 +20196,75 @@
         <v/>
       </c>
       <c r="K38" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K38="","",IF('Data Entry'!K38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L38" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L38="","",IF('Data Entry'!L38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M38" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M38="","",IF('Data Entry'!M38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N38" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N38="","",IF('Data Entry'!N38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O38" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O38="","",IF('Data Entry'!O38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P38" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P38="","",IF('Data Entry'!P38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q38="","",IF('Data Entry'!Q38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R38" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R38="","",IF('Data Entry'!R38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S38" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S38="","",IF('Data Entry'!S38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T38" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T38="","",IF('Data Entry'!T38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U38" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U38="","",IF('Data Entry'!U38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V38" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V38="","",IF('Data Entry'!V38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W38" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W38="","",IF('Data Entry'!W38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X38" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X38="","",IF('Data Entry'!X38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y38" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y38="","",IF('Data Entry'!Y38='Data Entry'!$D38,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K38="","",IF('Data Entry'!K38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L38="","",IF('Data Entry'!L38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M38="","",IF('Data Entry'!M38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N38="","",IF('Data Entry'!N38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O38="","",IF('Data Entry'!O38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P38="","",IF('Data Entry'!P38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q38="","",IF('Data Entry'!Q38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R38="","",IF('Data Entry'!R38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S38="","",IF('Data Entry'!S38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T38="","",IF('Data Entry'!T38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U38="","",IF('Data Entry'!U38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V38="","",IF('Data Entry'!V38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W38="","",IF('Data Entry'!W38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X38="","",IF('Data Entry'!X38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y38="","",IF('Data Entry'!Y38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z38" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z38="","",IF('Data Entry'!Z38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA38" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA38="","",IF('Data Entry'!AA38='Data Entry'!$D38,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB38" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB38="","",IF('Data Entry'!AB38='Data Entry'!$D38,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z38="","",IF('Data Entry'!Z38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA38="","",IF('Data Entry'!AA38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB38" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB38="","",IF('Data Entry'!AB38='Data Entry'!$D38,1,IF('Data Entry'!$D38="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC38" s="99" t="str">
@@ -20324,75 +20324,75 @@
         <v/>
       </c>
       <c r="K39" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K39="","",IF('Data Entry'!K39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L39" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L39="","",IF('Data Entry'!L39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M39" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M39="","",IF('Data Entry'!M39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N39" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N39="","",IF('Data Entry'!N39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O39" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O39="","",IF('Data Entry'!O39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P39" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P39="","",IF('Data Entry'!P39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q39" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q39="","",IF('Data Entry'!Q39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R39" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R39="","",IF('Data Entry'!R39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S39" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S39="","",IF('Data Entry'!S39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T39" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T39="","",IF('Data Entry'!T39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U39" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U39="","",IF('Data Entry'!U39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V39" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V39="","",IF('Data Entry'!V39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W39" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W39="","",IF('Data Entry'!W39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X39" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X39="","",IF('Data Entry'!X39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y39" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y39="","",IF('Data Entry'!Y39='Data Entry'!$D39,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K39="","",IF('Data Entry'!K39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L39="","",IF('Data Entry'!L39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M39="","",IF('Data Entry'!M39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N39="","",IF('Data Entry'!N39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O39="","",IF('Data Entry'!O39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P39="","",IF('Data Entry'!P39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q39="","",IF('Data Entry'!Q39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R39="","",IF('Data Entry'!R39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S39="","",IF('Data Entry'!S39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T39="","",IF('Data Entry'!T39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U39="","",IF('Data Entry'!U39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V39="","",IF('Data Entry'!V39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W39="","",IF('Data Entry'!W39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X39="","",IF('Data Entry'!X39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y39="","",IF('Data Entry'!Y39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z39" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z39="","",IF('Data Entry'!Z39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA39" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA39="","",IF('Data Entry'!AA39='Data Entry'!$D39,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB39" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB39="","",IF('Data Entry'!AB39='Data Entry'!$D39,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z39="","",IF('Data Entry'!Z39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA39="","",IF('Data Entry'!AA39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB39" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB39="","",IF('Data Entry'!AB39='Data Entry'!$D39,1,IF('Data Entry'!$D39="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC39" s="99" t="str">
@@ -20452,75 +20452,75 @@
         <v/>
       </c>
       <c r="K40" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K40="","",IF('Data Entry'!K40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L40" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L40="","",IF('Data Entry'!L40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M40" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M40="","",IF('Data Entry'!M40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N40" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N40="","",IF('Data Entry'!N40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O40" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O40="","",IF('Data Entry'!O40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P40" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P40="","",IF('Data Entry'!P40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q40="","",IF('Data Entry'!Q40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R40" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R40="","",IF('Data Entry'!R40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S40" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S40="","",IF('Data Entry'!S40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T40" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T40="","",IF('Data Entry'!T40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U40" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U40="","",IF('Data Entry'!U40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V40" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V40="","",IF('Data Entry'!V40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W40" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W40="","",IF('Data Entry'!W40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X40" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X40="","",IF('Data Entry'!X40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y40" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y40="","",IF('Data Entry'!Y40='Data Entry'!$D40,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K40="","",IF('Data Entry'!K40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L40="","",IF('Data Entry'!L40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M40="","",IF('Data Entry'!M40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N40="","",IF('Data Entry'!N40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O40="","",IF('Data Entry'!O40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P40="","",IF('Data Entry'!P40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q40="","",IF('Data Entry'!Q40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R40="","",IF('Data Entry'!R40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S40="","",IF('Data Entry'!S40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T40="","",IF('Data Entry'!T40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U40="","",IF('Data Entry'!U40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V40="","",IF('Data Entry'!V40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W40="","",IF('Data Entry'!W40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X40="","",IF('Data Entry'!X40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y40="","",IF('Data Entry'!Y40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z40" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z40="","",IF('Data Entry'!Z40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA40" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA40="","",IF('Data Entry'!AA40='Data Entry'!$D40,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB40" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB40="","",IF('Data Entry'!AB40='Data Entry'!$D40,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z40="","",IF('Data Entry'!Z40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA40="","",IF('Data Entry'!AA40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB40" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB40="","",IF('Data Entry'!AB40='Data Entry'!$D40,1,IF('Data Entry'!$D40="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC40" s="99" t="str">
@@ -20580,75 +20580,75 @@
         <v/>
       </c>
       <c r="K41" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K41="","",IF('Data Entry'!K41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L41" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L41="","",IF('Data Entry'!L41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M41" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M41="","",IF('Data Entry'!M41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N41" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N41="","",IF('Data Entry'!N41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O41" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O41="","",IF('Data Entry'!O41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P41" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P41="","",IF('Data Entry'!P41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q41="","",IF('Data Entry'!Q41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R41" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R41="","",IF('Data Entry'!R41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S41" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S41="","",IF('Data Entry'!S41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T41" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T41="","",IF('Data Entry'!T41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U41" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U41="","",IF('Data Entry'!U41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V41" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V41="","",IF('Data Entry'!V41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W41" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W41="","",IF('Data Entry'!W41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X41" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X41="","",IF('Data Entry'!X41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y41" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y41="","",IF('Data Entry'!Y41='Data Entry'!$D41,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K41="","",IF('Data Entry'!K41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L41="","",IF('Data Entry'!L41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M41="","",IF('Data Entry'!M41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N41="","",IF('Data Entry'!N41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O41="","",IF('Data Entry'!O41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P41="","",IF('Data Entry'!P41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q41="","",IF('Data Entry'!Q41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R41="","",IF('Data Entry'!R41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S41="","",IF('Data Entry'!S41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T41="","",IF('Data Entry'!T41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U41="","",IF('Data Entry'!U41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V41="","",IF('Data Entry'!V41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W41="","",IF('Data Entry'!W41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X41="","",IF('Data Entry'!X41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y41="","",IF('Data Entry'!Y41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z41" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z41="","",IF('Data Entry'!Z41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA41" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA41="","",IF('Data Entry'!AA41='Data Entry'!$D41,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB41" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB41="","",IF('Data Entry'!AB41='Data Entry'!$D41,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z41="","",IF('Data Entry'!Z41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA41="","",IF('Data Entry'!AA41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB41" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB41="","",IF('Data Entry'!AB41='Data Entry'!$D41,1,IF('Data Entry'!$D41="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC41" s="99" t="str">
@@ -20708,75 +20708,75 @@
         <v/>
       </c>
       <c r="K42" s="49" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!K42="","",IF('Data Entry'!K42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="L42" s="46" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!L42="","",IF('Data Entry'!L42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="M42" s="47" t="str">
-        <f aca="false">IF($K$11="","",IF('Data Entry'!M42="","",IF('Data Entry'!M42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="N42" s="45" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!N42="","",IF('Data Entry'!N42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="O42" s="46" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!O42="","",IF('Data Entry'!O42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="P42" s="48" t="str">
-        <f aca="false">IF($N$11="","",IF('Data Entry'!P42="","",IF('Data Entry'!P42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Q42="","",IF('Data Entry'!Q42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="R42" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!R42="","",IF('Data Entry'!R42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="S42" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!S42="","",IF('Data Entry'!S42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="T42" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!T42="","",IF('Data Entry'!T42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="U42" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!U42="","",IF('Data Entry'!U42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="V42" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!V42="","",IF('Data Entry'!V42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="W42" s="45" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!W42="","",IF('Data Entry'!W42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="X42" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!X42="","",IF('Data Entry'!X42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="Y42" s="48" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Y42="","",IF('Data Entry'!Y42='Data Entry'!$D42,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!K42="","",IF('Data Entry'!K42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="L42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!L42="","",IF('Data Entry'!L42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="M42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!M42="","",IF('Data Entry'!M42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="N42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!N42="","",IF('Data Entry'!N42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="O42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!O42="","",IF('Data Entry'!O42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="P42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!P42="","",IF('Data Entry'!P42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Q42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Q42="","",IF('Data Entry'!Q42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="R42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!R42="","",IF('Data Entry'!R42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="S42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!S42="","",IF('Data Entry'!S42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="T42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!T42="","",IF('Data Entry'!T42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="U42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!U42="","",IF('Data Entry'!U42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="V42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!V42="","",IF('Data Entry'!V42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="W42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!W42="","",IF('Data Entry'!W42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="X42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!X42="","",IF('Data Entry'!X42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="Y42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Y42="","",IF('Data Entry'!Y42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="Z42" s="49" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!Z42="","",IF('Data Entry'!Z42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AA42" s="46" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AA42="","",IF('Data Entry'!AA42='Data Entry'!$D42,1,0)))</f>
-        <v/>
-      </c>
-      <c r="AB42" s="47" t="str">
-        <f aca="false">IF($Z$11="","",IF('Data Entry'!AB42="","",IF('Data Entry'!AB42='Data Entry'!$D42,1,0)))</f>
+        <f aca="false">IF($H$11="","",IF('Data Entry'!Z42="","",IF('Data Entry'!Z42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AA42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AA42="","",IF('Data Entry'!AA42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
+        <v/>
+      </c>
+      <c r="AB42" s="49" t="str">
+        <f aca="false">IF($H$11="","",IF('Data Entry'!AB42="","",IF('Data Entry'!AB42='Data Entry'!$D42,1,IF('Data Entry'!$D42="GOOD",0,-1))))</f>
         <v/>
       </c>
       <c r="AC42" s="99" t="str">
@@ -30626,7 +30626,7 @@
   </sheetPr>
   <dimension ref="A1:DA989"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIX: correção na planilha, no calculo
</commit_message>
<xml_diff>
--- a/storage/app/public/GRR_BASICO.xlsx
+++ b/storage/app/public/GRR_BASICO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" state="visible" r:id="rId3"/>
@@ -617,20 +617,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="13">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="&quot;&gt; &quot;0.0%;&quot;Invalid, Invalid, Invalid&quot;"/>
-    <numFmt numFmtId="174" formatCode="&quot;&lt; &quot;0.0%;&quot;Invalid, Invalid, Invalid&quot;"/>
-    <numFmt numFmtId="175" formatCode="&quot;&lt; &quot;0.00;&quot;Invalid, Invalid, Invalid&quot;"/>
-    <numFmt numFmtId="176" formatCode="&quot;&gt; &quot;0.00;&quot;Invalid, Invalid, Invalid&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="&quot;&gt; &quot;0.0%;&quot;Invalid, Invalid, Invalid&quot;"/>
+    <numFmt numFmtId="173" formatCode="&quot;&lt; &quot;0.0%;&quot;Invalid, Invalid, Invalid&quot;"/>
+    <numFmt numFmtId="174" formatCode="&quot;&lt; &quot;0.00;&quot;Invalid, Invalid, Invalid&quot;"/>
+    <numFmt numFmtId="175" formatCode="&quot;&gt; &quot;0.00;&quot;Invalid, Invalid, Invalid&quot;"/>
   </numFmts>
   <fonts count="42">
     <font>
@@ -1510,11 +1509,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1526,7 +1525,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1550,11 +1549,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1670,7 +1669,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1706,11 +1705,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1718,7 +1717,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1738,11 +1737,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1750,7 +1749,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1770,15 +1769,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1786,7 +1785,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1826,7 +1825,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1834,7 +1833,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1850,15 +1849,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1910,7 +1909,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1978,7 +1977,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2018,19 +2017,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2038,39 +2037,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2078,19 +2077,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2098,7 +2097,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2106,11 +2105,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2118,11 +2117,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2166,15 +2165,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2182,11 +2181,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2198,15 +2197,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="34" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="34" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2222,7 +2221,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2230,7 +2229,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2246,7 +2245,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2254,19 +2253,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2274,7 +2273,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2286,7 +2285,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2294,11 +2293,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2306,15 +2305,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2322,15 +2321,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2378,15 +2377,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2394,23 +2393,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2418,39 +2417,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="174" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="40" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="175" fontId="40" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2458,7 +2457,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4210,8 +4209,8 @@
   </sheetPr>
   <dimension ref="A1:AO930"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16137,7 +16136,7 @@
       <formula>"NO GOOD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:AB20 K22:AB42 K21:AB21 E13:J42">
+  <conditionalFormatting sqref="K13:AB20 K22:AB42 K21:AB21 F13:J42 E13 E15:E42">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"GOOD"</formula>
     </cfRule>
@@ -16151,6 +16150,14 @@
     </cfRule>
     <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"GOOD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"GOOD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"NO GOOD"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -16180,8 +16187,8 @@
   </sheetPr>
   <dimension ref="A1:AN930"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM1" activeCellId="0" sqref="AM1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30545,8 +30552,8 @@
   </sheetPr>
   <dimension ref="A1:DA989"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31624,11 +31631,11 @@
         <v>68</v>
       </c>
       <c r="C10" s="139" t="n">
-        <f aca="false">E10+G10+I10+K10+S10</f>
+        <f aca="false">E10+G10+I10+K10+M10+O10+Q10+S10</f>
         <v>0</v>
       </c>
       <c r="D10" s="140" t="n">
-        <f aca="false">F10+H10+J10+L10+T10</f>
+        <f aca="false">F10+H10+J10+L10+N10+P10+R10+T10</f>
         <v>0</v>
       </c>
       <c r="E10" s="141" t="n">

</xml_diff>

<commit_message>
FIX: correção no campo de part number
</commit_message>
<xml_diff>
--- a/storage/app/public/GRR_BASICO.xlsx
+++ b/storage/app/public/GRR_BASICO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" state="visible" r:id="rId3"/>
@@ -1460,7 +1460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="259">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1951,6 +1951,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4209,7 +4213,7 @@
   </sheetPr>
   <dimension ref="A1:AO930"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -30552,8 +30556,8 @@
   </sheetPr>
   <dimension ref="A1:DA989"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31021,12 +31025,12 @@
       <c r="F5" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="121" t="str">
+      <c r="G5" s="123" t="str">
         <f aca="false">IF('Data Entry'!$I$7="","",'Data Entry'!$I$7)</f>
         <v>GP32H</v>
       </c>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="116"/>
       <c r="K5" s="116"/>
       <c r="L5" s="116"/>
@@ -31128,11 +31132,11 @@
       <c r="B6" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="123" t="str">
+      <c r="C6" s="124" t="str">
         <f aca="false">IF('Data Entry'!$I$6="","",'Data Entry'!$I$6)</f>
         <v>Apenas um grande teste</v>
       </c>
-      <c r="D6" s="123"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="116"/>
       <c r="F6" s="122" t="s">
         <v>58</v>
@@ -31346,54 +31350,54 @@
       <c r="DA7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="124"/>
-      <c r="B8" s="125" t="s">
+      <c r="A8" s="125"/>
+      <c r="B8" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="126" t="s">
+      <c r="C8" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="126"/>
-      <c r="E8" s="127" t="str">
+      <c r="D8" s="127"/>
+      <c r="E8" s="128" t="str">
         <f aca="false">'Data Entry'!E$11</f>
         <v>No user</v>
       </c>
-      <c r="F8" s="127"/>
-      <c r="G8" s="128" t="str">
+      <c r="F8" s="128"/>
+      <c r="G8" s="129" t="str">
         <f aca="false">'Data Entry'!H$11</f>
         <v>No user</v>
       </c>
-      <c r="H8" s="128"/>
-      <c r="I8" s="128" t="str">
+      <c r="H8" s="129"/>
+      <c r="I8" s="129" t="str">
         <f aca="false">'Data Entry'!K$11</f>
         <v>No user</v>
       </c>
-      <c r="J8" s="128"/>
-      <c r="K8" s="128" t="str">
+      <c r="J8" s="129"/>
+      <c r="K8" s="129" t="str">
         <f aca="false">'Data Entry'!N$11</f>
         <v>No user</v>
       </c>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128" t="str">
+      <c r="L8" s="129"/>
+      <c r="M8" s="129" t="str">
         <f aca="false">'Data Entry'!Q$11</f>
         <v>No user</v>
       </c>
-      <c r="N8" s="128"/>
-      <c r="O8" s="128" t="str">
+      <c r="N8" s="129"/>
+      <c r="O8" s="129" t="str">
         <f aca="false">'Data Entry'!T$11</f>
         <v>No user</v>
       </c>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="128" t="str">
+      <c r="P8" s="129"/>
+      <c r="Q8" s="129" t="str">
         <f aca="false">'Data Entry'!W$11</f>
         <v>No user</v>
       </c>
-      <c r="R8" s="128"/>
-      <c r="S8" s="129" t="str">
+      <c r="R8" s="129"/>
+      <c r="S8" s="130" t="str">
         <f aca="false">'Data Entry'!Z$11</f>
         <v>No user</v>
       </c>
-      <c r="T8" s="129"/>
+      <c r="T8" s="130"/>
       <c r="U8" s="3"/>
       <c r="V8" s="2"/>
       <c r="W8" s="3"/>
@@ -31482,133 +31486,133 @@
     </row>
     <row r="9" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="85"/>
-      <c r="B9" s="130" t="s">
+      <c r="B9" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="133" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="133" t="s">
+      <c r="E9" s="134" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="134" t="s">
+      <c r="F9" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="136" t="s">
+      <c r="H9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="135" t="s">
+      <c r="I9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="136" t="s">
+      <c r="J9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="135" t="s">
+      <c r="K9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="136" t="s">
+      <c r="L9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="M9" s="135" t="s">
+      <c r="M9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="136" t="s">
+      <c r="N9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="135" t="s">
+      <c r="O9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="136" t="s">
+      <c r="P9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="Q9" s="135" t="s">
+      <c r="Q9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="R9" s="136" t="s">
+      <c r="R9" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="S9" s="135" t="s">
+      <c r="S9" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="T9" s="137" t="s">
+      <c r="T9" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="U9" s="138"/>
-      <c r="V9" s="138"/>
-      <c r="W9" s="138"/>
-      <c r="X9" s="138"/>
-      <c r="Y9" s="138"/>
-      <c r="Z9" s="138"/>
-      <c r="AA9" s="138"/>
-      <c r="AB9" s="138"/>
-      <c r="AC9" s="138"/>
-      <c r="AD9" s="138"/>
-      <c r="AE9" s="138"/>
-      <c r="AF9" s="138"/>
-      <c r="AG9" s="138"/>
-      <c r="AH9" s="138"/>
-      <c r="AI9" s="138"/>
-      <c r="AJ9" s="138"/>
-      <c r="AK9" s="138"/>
-      <c r="AL9" s="138"/>
-      <c r="AM9" s="138"/>
-      <c r="AN9" s="138"/>
-      <c r="AO9" s="138"/>
-      <c r="AP9" s="138"/>
-      <c r="AQ9" s="138"/>
-      <c r="AR9" s="138"/>
-      <c r="AS9" s="138"/>
-      <c r="AT9" s="138"/>
-      <c r="AU9" s="138"/>
-      <c r="AV9" s="138"/>
-      <c r="AW9" s="138"/>
-      <c r="AX9" s="138"/>
-      <c r="AY9" s="138"/>
-      <c r="AZ9" s="138"/>
-      <c r="BA9" s="138"/>
-      <c r="BB9" s="138"/>
-      <c r="BC9" s="138"/>
-      <c r="BD9" s="138"/>
-      <c r="BE9" s="138"/>
-      <c r="BF9" s="138"/>
-      <c r="BG9" s="138"/>
-      <c r="BH9" s="138"/>
-      <c r="BI9" s="138"/>
-      <c r="BJ9" s="138"/>
-      <c r="BK9" s="138"/>
-      <c r="BL9" s="138"/>
-      <c r="BM9" s="138"/>
-      <c r="BN9" s="138"/>
-      <c r="BO9" s="138"/>
-      <c r="BP9" s="138"/>
-      <c r="BQ9" s="138"/>
-      <c r="BR9" s="138"/>
-      <c r="BS9" s="138"/>
-      <c r="BT9" s="138"/>
-      <c r="BU9" s="138"/>
-      <c r="BV9" s="138"/>
-      <c r="BW9" s="138"/>
-      <c r="BX9" s="138"/>
-      <c r="BY9" s="138"/>
-      <c r="BZ9" s="138"/>
-      <c r="CA9" s="138"/>
-      <c r="CB9" s="138"/>
-      <c r="CC9" s="138"/>
-      <c r="CD9" s="138"/>
-      <c r="CE9" s="138"/>
-      <c r="CF9" s="138"/>
-      <c r="CG9" s="138"/>
-      <c r="CH9" s="138"/>
-      <c r="CI9" s="138"/>
-      <c r="CJ9" s="138"/>
-      <c r="CK9" s="138"/>
-      <c r="CL9" s="138"/>
+      <c r="U9" s="139"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="139"/>
+      <c r="X9" s="139"/>
+      <c r="Y9" s="139"/>
+      <c r="Z9" s="139"/>
+      <c r="AA9" s="139"/>
+      <c r="AB9" s="139"/>
+      <c r="AC9" s="139"/>
+      <c r="AD9" s="139"/>
+      <c r="AE9" s="139"/>
+      <c r="AF9" s="139"/>
+      <c r="AG9" s="139"/>
+      <c r="AH9" s="139"/>
+      <c r="AI9" s="139"/>
+      <c r="AJ9" s="139"/>
+      <c r="AK9" s="139"/>
+      <c r="AL9" s="139"/>
+      <c r="AM9" s="139"/>
+      <c r="AN9" s="139"/>
+      <c r="AO9" s="139"/>
+      <c r="AP9" s="139"/>
+      <c r="AQ9" s="139"/>
+      <c r="AR9" s="139"/>
+      <c r="AS9" s="139"/>
+      <c r="AT9" s="139"/>
+      <c r="AU9" s="139"/>
+      <c r="AV9" s="139"/>
+      <c r="AW9" s="139"/>
+      <c r="AX9" s="139"/>
+      <c r="AY9" s="139"/>
+      <c r="AZ9" s="139"/>
+      <c r="BA9" s="139"/>
+      <c r="BB9" s="139"/>
+      <c r="BC9" s="139"/>
+      <c r="BD9" s="139"/>
+      <c r="BE9" s="139"/>
+      <c r="BF9" s="139"/>
+      <c r="BG9" s="139"/>
+      <c r="BH9" s="139"/>
+      <c r="BI9" s="139"/>
+      <c r="BJ9" s="139"/>
+      <c r="BK9" s="139"/>
+      <c r="BL9" s="139"/>
+      <c r="BM9" s="139"/>
+      <c r="BN9" s="139"/>
+      <c r="BO9" s="139"/>
+      <c r="BP9" s="139"/>
+      <c r="BQ9" s="139"/>
+      <c r="BR9" s="139"/>
+      <c r="BS9" s="139"/>
+      <c r="BT9" s="139"/>
+      <c r="BU9" s="139"/>
+      <c r="BV9" s="139"/>
+      <c r="BW9" s="139"/>
+      <c r="BX9" s="139"/>
+      <c r="BY9" s="139"/>
+      <c r="BZ9" s="139"/>
+      <c r="CA9" s="139"/>
+      <c r="CB9" s="139"/>
+      <c r="CC9" s="139"/>
+      <c r="CD9" s="139"/>
+      <c r="CE9" s="139"/>
+      <c r="CF9" s="139"/>
+      <c r="CG9" s="139"/>
+      <c r="CH9" s="139"/>
+      <c r="CI9" s="139"/>
+      <c r="CJ9" s="139"/>
+      <c r="CK9" s="139"/>
+      <c r="CL9" s="139"/>
       <c r="CM9" s="2"/>
       <c r="CN9" s="2"/>
       <c r="CO9" s="2"/>
@@ -31627,151 +31631,151 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="85"/>
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="139" t="n">
+      <c r="C10" s="140" t="n">
         <f aca="false">E10+G10+I10+K10+M10+O10+Q10+S10</f>
         <v>0</v>
       </c>
-      <c r="D10" s="140" t="n">
+      <c r="D10" s="141" t="n">
         <f aca="false">F10+H10+J10+L10+N10+P10+R10+T10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="141" t="n">
+      <c r="E10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!E13:G42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="F10" s="140" t="n">
+      <c r="F10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!E13:G42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="G10" s="141" t="n">
+      <c r="G10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!H13:J42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="H10" s="140" t="n">
+      <c r="H10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!H13:J42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="I10" s="141" t="n">
+      <c r="I10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!K13:M42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="J10" s="140" t="n">
+      <c r="J10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!K13:M42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="K10" s="141" t="n">
+      <c r="K10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!N13:P42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="L10" s="140" t="n">
+      <c r="L10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!N13:P42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="M10" s="141" t="n">
+      <c r="M10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!Q13:S42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="N10" s="140" t="n">
+      <c r="N10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!Q13:S42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="O10" s="141" t="n">
+      <c r="O10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!T13:V42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="P10" s="140" t="n">
+      <c r="P10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!T13:V42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="141" t="n">
+      <c r="Q10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!W13:Y42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="R10" s="140" t="n">
+      <c r="R10" s="141" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!W13:Y42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="S10" s="141" t="n">
+      <c r="S10" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!Z13:AB42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="T10" s="142" t="n">
+      <c r="T10" s="143" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!Z13:AB42,"&gt;=-1"))</f>
         <v>0</v>
       </c>
-      <c r="U10" s="143"/>
-      <c r="V10" s="143"/>
-      <c r="W10" s="143"/>
-      <c r="X10" s="143"/>
-      <c r="Y10" s="143"/>
-      <c r="Z10" s="143"/>
-      <c r="AA10" s="143"/>
-      <c r="AB10" s="143"/>
-      <c r="AC10" s="143"/>
-      <c r="AD10" s="143"/>
-      <c r="AE10" s="143"/>
-      <c r="AF10" s="143"/>
-      <c r="AG10" s="143"/>
-      <c r="AH10" s="143"/>
-      <c r="AI10" s="143"/>
-      <c r="AJ10" s="143"/>
-      <c r="AK10" s="143"/>
-      <c r="AL10" s="143"/>
-      <c r="AM10" s="143"/>
-      <c r="AN10" s="143"/>
-      <c r="AO10" s="143"/>
-      <c r="AP10" s="143"/>
-      <c r="AQ10" s="143"/>
-      <c r="AR10" s="143"/>
-      <c r="AS10" s="143"/>
-      <c r="AT10" s="143"/>
-      <c r="AU10" s="143"/>
-      <c r="AV10" s="143"/>
-      <c r="AW10" s="143"/>
-      <c r="AX10" s="143"/>
-      <c r="AY10" s="143"/>
-      <c r="AZ10" s="143"/>
-      <c r="BA10" s="143"/>
-      <c r="BB10" s="143"/>
-      <c r="BC10" s="143"/>
-      <c r="BD10" s="143"/>
-      <c r="BE10" s="143"/>
-      <c r="BF10" s="143"/>
-      <c r="BG10" s="143"/>
-      <c r="BH10" s="143"/>
-      <c r="BI10" s="143"/>
-      <c r="BJ10" s="143"/>
-      <c r="BK10" s="143"/>
-      <c r="BL10" s="143"/>
-      <c r="BM10" s="143"/>
-      <c r="BN10" s="143"/>
-      <c r="BO10" s="143"/>
-      <c r="BP10" s="143"/>
-      <c r="BQ10" s="143"/>
-      <c r="BR10" s="143"/>
-      <c r="BS10" s="143"/>
-      <c r="BT10" s="143"/>
-      <c r="BU10" s="143"/>
-      <c r="BV10" s="143"/>
-      <c r="BW10" s="143"/>
-      <c r="BX10" s="143"/>
-      <c r="BY10" s="143"/>
-      <c r="BZ10" s="143"/>
-      <c r="CA10" s="143"/>
-      <c r="CB10" s="143"/>
-      <c r="CC10" s="143"/>
-      <c r="CD10" s="143"/>
-      <c r="CE10" s="143"/>
-      <c r="CF10" s="143"/>
-      <c r="CG10" s="143"/>
-      <c r="CH10" s="143"/>
-      <c r="CI10" s="143"/>
-      <c r="CJ10" s="143"/>
-      <c r="CK10" s="143"/>
-      <c r="CL10" s="143"/>
+      <c r="U10" s="144"/>
+      <c r="V10" s="144"/>
+      <c r="W10" s="144"/>
+      <c r="X10" s="144"/>
+      <c r="Y10" s="144"/>
+      <c r="Z10" s="144"/>
+      <c r="AA10" s="144"/>
+      <c r="AB10" s="144"/>
+      <c r="AC10" s="144"/>
+      <c r="AD10" s="144"/>
+      <c r="AE10" s="144"/>
+      <c r="AF10" s="144"/>
+      <c r="AG10" s="144"/>
+      <c r="AH10" s="144"/>
+      <c r="AI10" s="144"/>
+      <c r="AJ10" s="144"/>
+      <c r="AK10" s="144"/>
+      <c r="AL10" s="144"/>
+      <c r="AM10" s="144"/>
+      <c r="AN10" s="144"/>
+      <c r="AO10" s="144"/>
+      <c r="AP10" s="144"/>
+      <c r="AQ10" s="144"/>
+      <c r="AR10" s="144"/>
+      <c r="AS10" s="144"/>
+      <c r="AT10" s="144"/>
+      <c r="AU10" s="144"/>
+      <c r="AV10" s="144"/>
+      <c r="AW10" s="144"/>
+      <c r="AX10" s="144"/>
+      <c r="AY10" s="144"/>
+      <c r="AZ10" s="144"/>
+      <c r="BA10" s="144"/>
+      <c r="BB10" s="144"/>
+      <c r="BC10" s="144"/>
+      <c r="BD10" s="144"/>
+      <c r="BE10" s="144"/>
+      <c r="BF10" s="144"/>
+      <c r="BG10" s="144"/>
+      <c r="BH10" s="144"/>
+      <c r="BI10" s="144"/>
+      <c r="BJ10" s="144"/>
+      <c r="BK10" s="144"/>
+      <c r="BL10" s="144"/>
+      <c r="BM10" s="144"/>
+      <c r="BN10" s="144"/>
+      <c r="BO10" s="144"/>
+      <c r="BP10" s="144"/>
+      <c r="BQ10" s="144"/>
+      <c r="BR10" s="144"/>
+      <c r="BS10" s="144"/>
+      <c r="BT10" s="144"/>
+      <c r="BU10" s="144"/>
+      <c r="BV10" s="144"/>
+      <c r="BW10" s="144"/>
+      <c r="BX10" s="144"/>
+      <c r="BY10" s="144"/>
+      <c r="BZ10" s="144"/>
+      <c r="CA10" s="144"/>
+      <c r="CB10" s="144"/>
+      <c r="CC10" s="144"/>
+      <c r="CD10" s="144"/>
+      <c r="CE10" s="144"/>
+      <c r="CF10" s="144"/>
+      <c r="CG10" s="144"/>
+      <c r="CH10" s="144"/>
+      <c r="CI10" s="144"/>
+      <c r="CJ10" s="144"/>
+      <c r="CK10" s="144"/>
+      <c r="CL10" s="144"/>
       <c r="CM10" s="2"/>
       <c r="CN10" s="2"/>
       <c r="CO10" s="2"/>
@@ -31790,151 +31794,151 @@
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="85"/>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="144" t="n">
+      <c r="C11" s="145" t="n">
         <f aca="false">E11+G11+I11+K11+M11+O11+Q11+S11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="145" t="n">
+      <c r="D11" s="146" t="n">
         <f aca="false">F11+H11+J11+L11+N11+P11+R11+T11</f>
         <v>0</v>
       </c>
-      <c r="E11" s="146" t="n">
+      <c r="E11" s="147" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!E13:G42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="145" t="n">
+      <c r="F11" s="146" t="n">
         <f aca="false">IF(F8="No user",0,COUNTIF(Calculation!E13:G42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="146" t="n">
+      <c r="G11" s="147" t="n">
         <f aca="false">IF(G8="No user",0,COUNTIF(Calculation!H13:J42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="H11" s="145" t="n">
+      <c r="H11" s="146" t="n">
         <f aca="false">IF(H8="No user",0,COUNTIF(Calculation!H13:J42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="I11" s="146" t="n">
+      <c r="I11" s="147" t="n">
         <f aca="false">IF(I8="No user",0,COUNTIF(Calculation!K13:M42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="J11" s="145" t="n">
+      <c r="J11" s="146" t="n">
         <f aca="false">IF(J8="No user",0,COUNTIF(Calculation!K13:M42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="K11" s="146" t="n">
+      <c r="K11" s="147" t="n">
         <f aca="false">IF(K8="No user",0,COUNTIF(Calculation!N13:P42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="L11" s="145" t="n">
+      <c r="L11" s="146" t="n">
         <f aca="false">IF(L8="No user",0,COUNTIF(Calculation!N13:P42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="M11" s="146" t="n">
+      <c r="M11" s="147" t="n">
         <f aca="false">IF(M8="No user",0,COUNTIF(Calculation!Q13:S42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="N11" s="145" t="n">
+      <c r="N11" s="146" t="n">
         <f aca="false">IF(N8="No user",0,COUNTIF(Calculation!Q13:S42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="O11" s="146" t="n">
+      <c r="O11" s="147" t="n">
         <f aca="false">IF(O8="No user",0,COUNTIF(Calculation!T13:V42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="P11" s="145" t="n">
+      <c r="P11" s="146" t="n">
         <f aca="false">IF(P8="No user",0,COUNTIF(Calculation!T13:V42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="146" t="n">
+      <c r="Q11" s="147" t="n">
         <f aca="false">IF(Q8="No user",0,COUNTIF(Calculation!W13:Y42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="R11" s="145" t="n">
+      <c r="R11" s="146" t="n">
         <f aca="false">IF(R8="No user",0,COUNTIF(Calculation!W13:Y42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="S11" s="146" t="n">
+      <c r="S11" s="147" t="n">
         <f aca="false">IF(S8="No user",0,COUNTIF(Calculation!Z13:AB42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="T11" s="147" t="n">
+      <c r="T11" s="148" t="n">
         <f aca="false">IF(T8="No user",0,COUNTIF(Calculation!Z13:AB42,"=1"))</f>
         <v>0</v>
       </c>
-      <c r="U11" s="143"/>
-      <c r="V11" s="143"/>
-      <c r="W11" s="143"/>
-      <c r="X11" s="143"/>
-      <c r="Y11" s="143"/>
-      <c r="Z11" s="143"/>
-      <c r="AA11" s="143"/>
-      <c r="AB11" s="143"/>
-      <c r="AC11" s="143"/>
-      <c r="AD11" s="143"/>
-      <c r="AE11" s="143"/>
-      <c r="AF11" s="143"/>
-      <c r="AG11" s="143"/>
-      <c r="AH11" s="143"/>
-      <c r="AI11" s="143"/>
-      <c r="AJ11" s="143"/>
-      <c r="AK11" s="143"/>
-      <c r="AL11" s="143"/>
-      <c r="AM11" s="143"/>
-      <c r="AN11" s="143"/>
-      <c r="AO11" s="143"/>
-      <c r="AP11" s="143"/>
-      <c r="AQ11" s="143"/>
-      <c r="AR11" s="143"/>
-      <c r="AS11" s="143"/>
-      <c r="AT11" s="143"/>
-      <c r="AU11" s="143"/>
-      <c r="AV11" s="143"/>
-      <c r="AW11" s="143"/>
-      <c r="AX11" s="143"/>
-      <c r="AY11" s="143"/>
-      <c r="AZ11" s="143"/>
-      <c r="BA11" s="143"/>
-      <c r="BB11" s="143"/>
-      <c r="BC11" s="143"/>
-      <c r="BD11" s="143"/>
-      <c r="BE11" s="143"/>
-      <c r="BF11" s="143"/>
-      <c r="BG11" s="143"/>
-      <c r="BH11" s="143"/>
-      <c r="BI11" s="143"/>
-      <c r="BJ11" s="143"/>
-      <c r="BK11" s="143"/>
-      <c r="BL11" s="143"/>
-      <c r="BM11" s="143"/>
-      <c r="BN11" s="143"/>
-      <c r="BO11" s="143"/>
-      <c r="BP11" s="143"/>
-      <c r="BQ11" s="143"/>
-      <c r="BR11" s="143"/>
-      <c r="BS11" s="143"/>
-      <c r="BT11" s="143"/>
-      <c r="BU11" s="143"/>
-      <c r="BV11" s="143"/>
-      <c r="BW11" s="143"/>
-      <c r="BX11" s="143"/>
-      <c r="BY11" s="143"/>
-      <c r="BZ11" s="143"/>
-      <c r="CA11" s="143"/>
-      <c r="CB11" s="143"/>
-      <c r="CC11" s="143"/>
-      <c r="CD11" s="143"/>
-      <c r="CE11" s="143"/>
-      <c r="CF11" s="143"/>
-      <c r="CG11" s="143"/>
-      <c r="CH11" s="143"/>
-      <c r="CI11" s="143"/>
-      <c r="CJ11" s="143"/>
-      <c r="CK11" s="143"/>
-      <c r="CL11" s="143"/>
+      <c r="U11" s="144"/>
+      <c r="V11" s="144"/>
+      <c r="W11" s="144"/>
+      <c r="X11" s="144"/>
+      <c r="Y11" s="144"/>
+      <c r="Z11" s="144"/>
+      <c r="AA11" s="144"/>
+      <c r="AB11" s="144"/>
+      <c r="AC11" s="144"/>
+      <c r="AD11" s="144"/>
+      <c r="AE11" s="144"/>
+      <c r="AF11" s="144"/>
+      <c r="AG11" s="144"/>
+      <c r="AH11" s="144"/>
+      <c r="AI11" s="144"/>
+      <c r="AJ11" s="144"/>
+      <c r="AK11" s="144"/>
+      <c r="AL11" s="144"/>
+      <c r="AM11" s="144"/>
+      <c r="AN11" s="144"/>
+      <c r="AO11" s="144"/>
+      <c r="AP11" s="144"/>
+      <c r="AQ11" s="144"/>
+      <c r="AR11" s="144"/>
+      <c r="AS11" s="144"/>
+      <c r="AT11" s="144"/>
+      <c r="AU11" s="144"/>
+      <c r="AV11" s="144"/>
+      <c r="AW11" s="144"/>
+      <c r="AX11" s="144"/>
+      <c r="AY11" s="144"/>
+      <c r="AZ11" s="144"/>
+      <c r="BA11" s="144"/>
+      <c r="BB11" s="144"/>
+      <c r="BC11" s="144"/>
+      <c r="BD11" s="144"/>
+      <c r="BE11" s="144"/>
+      <c r="BF11" s="144"/>
+      <c r="BG11" s="144"/>
+      <c r="BH11" s="144"/>
+      <c r="BI11" s="144"/>
+      <c r="BJ11" s="144"/>
+      <c r="BK11" s="144"/>
+      <c r="BL11" s="144"/>
+      <c r="BM11" s="144"/>
+      <c r="BN11" s="144"/>
+      <c r="BO11" s="144"/>
+      <c r="BP11" s="144"/>
+      <c r="BQ11" s="144"/>
+      <c r="BR11" s="144"/>
+      <c r="BS11" s="144"/>
+      <c r="BT11" s="144"/>
+      <c r="BU11" s="144"/>
+      <c r="BV11" s="144"/>
+      <c r="BW11" s="144"/>
+      <c r="BX11" s="144"/>
+      <c r="BY11" s="144"/>
+      <c r="BZ11" s="144"/>
+      <c r="CA11" s="144"/>
+      <c r="CB11" s="144"/>
+      <c r="CC11" s="144"/>
+      <c r="CD11" s="144"/>
+      <c r="CE11" s="144"/>
+      <c r="CF11" s="144"/>
+      <c r="CG11" s="144"/>
+      <c r="CH11" s="144"/>
+      <c r="CI11" s="144"/>
+      <c r="CJ11" s="144"/>
+      <c r="CK11" s="144"/>
+      <c r="CL11" s="144"/>
       <c r="CM11" s="2"/>
       <c r="CN11" s="2"/>
       <c r="CO11" s="2"/>
@@ -31953,100 +31957,100 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="85"/>
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="148" t="n">
+      <c r="C12" s="149" t="n">
         <f aca="false">'Data Entry'!D43</f>
         <v>0</v>
       </c>
-      <c r="D12" s="149"/>
-      <c r="E12" s="150"/>
-      <c r="F12" s="149"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="150"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="150"/>
-      <c r="L12" s="149"/>
-      <c r="M12" s="150"/>
-      <c r="N12" s="149"/>
-      <c r="O12" s="150"/>
-      <c r="P12" s="149"/>
-      <c r="Q12" s="150"/>
-      <c r="R12" s="149"/>
-      <c r="S12" s="150"/>
-      <c r="T12" s="151"/>
-      <c r="U12" s="152"/>
-      <c r="V12" s="152"/>
-      <c r="W12" s="152"/>
-      <c r="X12" s="152"/>
-      <c r="Y12" s="152"/>
-      <c r="Z12" s="152"/>
-      <c r="AA12" s="152"/>
-      <c r="AB12" s="152"/>
-      <c r="AC12" s="152"/>
-      <c r="AD12" s="152"/>
-      <c r="AE12" s="152"/>
-      <c r="AF12" s="152"/>
-      <c r="AG12" s="152"/>
-      <c r="AH12" s="152"/>
-      <c r="AI12" s="152"/>
-      <c r="AJ12" s="152"/>
-      <c r="AK12" s="152"/>
-      <c r="AL12" s="152"/>
-      <c r="AM12" s="152"/>
-      <c r="AN12" s="152"/>
-      <c r="AO12" s="152"/>
-      <c r="AP12" s="152"/>
-      <c r="AQ12" s="152"/>
-      <c r="AR12" s="152"/>
-      <c r="AS12" s="152"/>
-      <c r="AT12" s="152"/>
-      <c r="AU12" s="152"/>
-      <c r="AV12" s="152"/>
-      <c r="AW12" s="152"/>
-      <c r="AX12" s="152"/>
-      <c r="AY12" s="152"/>
-      <c r="AZ12" s="152"/>
-      <c r="BA12" s="152"/>
-      <c r="BB12" s="152"/>
-      <c r="BC12" s="152"/>
-      <c r="BD12" s="152"/>
-      <c r="BE12" s="152"/>
-      <c r="BF12" s="152"/>
-      <c r="BG12" s="152"/>
-      <c r="BH12" s="152"/>
-      <c r="BI12" s="152"/>
-      <c r="BJ12" s="152"/>
-      <c r="BK12" s="152"/>
-      <c r="BL12" s="152"/>
-      <c r="BM12" s="152"/>
-      <c r="BN12" s="152"/>
-      <c r="BO12" s="152"/>
-      <c r="BP12" s="152"/>
-      <c r="BQ12" s="152"/>
-      <c r="BR12" s="152"/>
-      <c r="BS12" s="152"/>
-      <c r="BT12" s="152"/>
-      <c r="BU12" s="152"/>
-      <c r="BV12" s="152"/>
-      <c r="BW12" s="152"/>
-      <c r="BX12" s="152"/>
-      <c r="BY12" s="152"/>
-      <c r="BZ12" s="152"/>
-      <c r="CA12" s="152"/>
-      <c r="CB12" s="152"/>
-      <c r="CC12" s="152"/>
-      <c r="CD12" s="152"/>
-      <c r="CE12" s="152"/>
-      <c r="CF12" s="152"/>
-      <c r="CG12" s="152"/>
-      <c r="CH12" s="152"/>
-      <c r="CI12" s="152"/>
-      <c r="CJ12" s="152"/>
-      <c r="CK12" s="152"/>
-      <c r="CL12" s="152"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="151"/>
+      <c r="L12" s="150"/>
+      <c r="M12" s="151"/>
+      <c r="N12" s="150"/>
+      <c r="O12" s="151"/>
+      <c r="P12" s="150"/>
+      <c r="Q12" s="151"/>
+      <c r="R12" s="150"/>
+      <c r="S12" s="151"/>
+      <c r="T12" s="152"/>
+      <c r="U12" s="153"/>
+      <c r="V12" s="153"/>
+      <c r="W12" s="153"/>
+      <c r="X12" s="153"/>
+      <c r="Y12" s="153"/>
+      <c r="Z12" s="153"/>
+      <c r="AA12" s="153"/>
+      <c r="AB12" s="153"/>
+      <c r="AC12" s="153"/>
+      <c r="AD12" s="153"/>
+      <c r="AE12" s="153"/>
+      <c r="AF12" s="153"/>
+      <c r="AG12" s="153"/>
+      <c r="AH12" s="153"/>
+      <c r="AI12" s="153"/>
+      <c r="AJ12" s="153"/>
+      <c r="AK12" s="153"/>
+      <c r="AL12" s="153"/>
+      <c r="AM12" s="153"/>
+      <c r="AN12" s="153"/>
+      <c r="AO12" s="153"/>
+      <c r="AP12" s="153"/>
+      <c r="AQ12" s="153"/>
+      <c r="AR12" s="153"/>
+      <c r="AS12" s="153"/>
+      <c r="AT12" s="153"/>
+      <c r="AU12" s="153"/>
+      <c r="AV12" s="153"/>
+      <c r="AW12" s="153"/>
+      <c r="AX12" s="153"/>
+      <c r="AY12" s="153"/>
+      <c r="AZ12" s="153"/>
+      <c r="BA12" s="153"/>
+      <c r="BB12" s="153"/>
+      <c r="BC12" s="153"/>
+      <c r="BD12" s="153"/>
+      <c r="BE12" s="153"/>
+      <c r="BF12" s="153"/>
+      <c r="BG12" s="153"/>
+      <c r="BH12" s="153"/>
+      <c r="BI12" s="153"/>
+      <c r="BJ12" s="153"/>
+      <c r="BK12" s="153"/>
+      <c r="BL12" s="153"/>
+      <c r="BM12" s="153"/>
+      <c r="BN12" s="153"/>
+      <c r="BO12" s="153"/>
+      <c r="BP12" s="153"/>
+      <c r="BQ12" s="153"/>
+      <c r="BR12" s="153"/>
+      <c r="BS12" s="153"/>
+      <c r="BT12" s="153"/>
+      <c r="BU12" s="153"/>
+      <c r="BV12" s="153"/>
+      <c r="BW12" s="153"/>
+      <c r="BX12" s="153"/>
+      <c r="BY12" s="153"/>
+      <c r="BZ12" s="153"/>
+      <c r="CA12" s="153"/>
+      <c r="CB12" s="153"/>
+      <c r="CC12" s="153"/>
+      <c r="CD12" s="153"/>
+      <c r="CE12" s="153"/>
+      <c r="CF12" s="153"/>
+      <c r="CG12" s="153"/>
+      <c r="CH12" s="153"/>
+      <c r="CI12" s="153"/>
+      <c r="CJ12" s="153"/>
+      <c r="CK12" s="153"/>
+      <c r="CL12" s="153"/>
       <c r="CM12" s="2"/>
       <c r="CN12" s="2"/>
       <c r="CO12" s="2"/>
@@ -32064,152 +32068,152 @@
       <c r="DA12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="124"/>
-      <c r="B13" s="153" t="s">
+      <c r="A13" s="125"/>
+      <c r="B13" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="154" t="str">
+      <c r="C13" s="155" t="str">
         <f aca="false">IF(C10=0,"",C11/C10)</f>
         <v/>
       </c>
-      <c r="D13" s="155" t="str">
+      <c r="D13" s="156" t="str">
         <f aca="false">IF(D10=0,"",D11/D10)</f>
         <v/>
       </c>
-      <c r="E13" s="156" t="str">
+      <c r="E13" s="157" t="str">
         <f aca="false">IF(OR(E8="No user", E11=0), "", E11/E10)</f>
         <v/>
       </c>
-      <c r="F13" s="156" t="str">
+      <c r="F13" s="157" t="str">
         <f aca="false">IF(OR(F8="No user", F11=0), "", F11/F10)</f>
         <v/>
       </c>
-      <c r="G13" s="156" t="str">
+      <c r="G13" s="157" t="str">
         <f aca="false">IF(OR(G8="No user", G11=0), "", G11/G10)</f>
         <v/>
       </c>
-      <c r="H13" s="156" t="str">
+      <c r="H13" s="157" t="str">
         <f aca="false">IF(OR(H8="No user", H11=0), "", H11/H10)</f>
         <v/>
       </c>
-      <c r="I13" s="156" t="str">
+      <c r="I13" s="157" t="str">
         <f aca="false">IF(OR(I8="No user", I11=0), "", I11/I10)</f>
         <v/>
       </c>
-      <c r="J13" s="156" t="str">
+      <c r="J13" s="157" t="str">
         <f aca="false">IF(OR(I8="No user", J11=0), "", J11/J10)</f>
         <v/>
       </c>
-      <c r="K13" s="156" t="str">
+      <c r="K13" s="157" t="str">
         <f aca="false">IF(OR(K8="No user", K11=0), "", K11/K10)</f>
         <v/>
       </c>
-      <c r="L13" s="156" t="str">
+      <c r="L13" s="157" t="str">
         <f aca="false">IF(OR(K8="No user", L11=0), "", L11/L10)</f>
         <v/>
       </c>
-      <c r="M13" s="156" t="str">
+      <c r="M13" s="157" t="str">
         <f aca="false">IF(OR(M8="No user", M11=0), "", M11/M10)</f>
         <v/>
       </c>
-      <c r="N13" s="156" t="str">
+      <c r="N13" s="157" t="str">
         <f aca="false">IF(OR(M8="No user", N11=0), "", N11/N10)</f>
         <v/>
       </c>
-      <c r="O13" s="156" t="str">
+      <c r="O13" s="157" t="str">
         <f aca="false">IF(OR(O8="No user", O11=0), "", O11/O10)</f>
         <v/>
       </c>
-      <c r="P13" s="156" t="str">
+      <c r="P13" s="157" t="str">
         <f aca="false">IF(OR(O8="No user", P11=0), "", P11/P10)</f>
         <v/>
       </c>
-      <c r="Q13" s="156" t="str">
+      <c r="Q13" s="157" t="str">
         <f aca="false">IF(OR(Q8="No user", Q11=0), "", Q11/Q10)</f>
         <v/>
       </c>
-      <c r="R13" s="156" t="str">
+      <c r="R13" s="157" t="str">
         <f aca="false">IF(OR(Q8="No user", R11=0), "", R11/R10)</f>
         <v/>
       </c>
-      <c r="S13" s="156" t="str">
+      <c r="S13" s="157" t="str">
         <f aca="false">IF(OR(S8="No user", S11=0), "", S11/S10)</f>
         <v/>
       </c>
-      <c r="T13" s="156" t="str">
+      <c r="T13" s="157" t="str">
         <f aca="false">IF(OR(S8="No user", T11=0), "", T11/T10)</f>
         <v/>
       </c>
-      <c r="U13" s="157"/>
-      <c r="V13" s="157"/>
-      <c r="W13" s="157"/>
-      <c r="X13" s="157"/>
-      <c r="Y13" s="157"/>
-      <c r="Z13" s="157"/>
-      <c r="AA13" s="157"/>
-      <c r="AB13" s="157"/>
-      <c r="AC13" s="157"/>
-      <c r="AD13" s="157"/>
-      <c r="AE13" s="157"/>
-      <c r="AF13" s="157"/>
-      <c r="AG13" s="157"/>
-      <c r="AH13" s="157"/>
-      <c r="AI13" s="157"/>
-      <c r="AJ13" s="157"/>
-      <c r="AK13" s="157"/>
-      <c r="AL13" s="157"/>
-      <c r="AM13" s="157"/>
-      <c r="AN13" s="157"/>
-      <c r="AO13" s="157"/>
-      <c r="AP13" s="157"/>
-      <c r="AQ13" s="157"/>
-      <c r="AR13" s="157"/>
-      <c r="AS13" s="157"/>
-      <c r="AT13" s="157"/>
-      <c r="AU13" s="157"/>
-      <c r="AV13" s="157"/>
-      <c r="AW13" s="157"/>
-      <c r="AX13" s="157"/>
-      <c r="AY13" s="157"/>
-      <c r="AZ13" s="157"/>
-      <c r="BA13" s="157"/>
-      <c r="BB13" s="157"/>
-      <c r="BC13" s="157"/>
-      <c r="BD13" s="157"/>
-      <c r="BE13" s="157"/>
-      <c r="BF13" s="157"/>
-      <c r="BG13" s="157"/>
-      <c r="BH13" s="157"/>
-      <c r="BI13" s="157"/>
-      <c r="BJ13" s="157"/>
-      <c r="BK13" s="157"/>
-      <c r="BL13" s="157"/>
-      <c r="BM13" s="157"/>
-      <c r="BN13" s="157"/>
-      <c r="BO13" s="157"/>
-      <c r="BP13" s="157"/>
-      <c r="BQ13" s="157"/>
-      <c r="BR13" s="157"/>
-      <c r="BS13" s="157"/>
-      <c r="BT13" s="157"/>
-      <c r="BU13" s="157"/>
-      <c r="BV13" s="157"/>
-      <c r="BW13" s="157"/>
-      <c r="BX13" s="157"/>
-      <c r="BY13" s="157"/>
-      <c r="BZ13" s="157"/>
-      <c r="CA13" s="157"/>
-      <c r="CB13" s="157"/>
-      <c r="CC13" s="157"/>
-      <c r="CD13" s="157"/>
-      <c r="CE13" s="157"/>
-      <c r="CF13" s="157"/>
-      <c r="CG13" s="157"/>
-      <c r="CH13" s="157"/>
-      <c r="CI13" s="157"/>
-      <c r="CJ13" s="157"/>
-      <c r="CK13" s="157"/>
-      <c r="CL13" s="157"/>
+      <c r="U13" s="158"/>
+      <c r="V13" s="158"/>
+      <c r="W13" s="158"/>
+      <c r="X13" s="158"/>
+      <c r="Y13" s="158"/>
+      <c r="Z13" s="158"/>
+      <c r="AA13" s="158"/>
+      <c r="AB13" s="158"/>
+      <c r="AC13" s="158"/>
+      <c r="AD13" s="158"/>
+      <c r="AE13" s="158"/>
+      <c r="AF13" s="158"/>
+      <c r="AG13" s="158"/>
+      <c r="AH13" s="158"/>
+      <c r="AI13" s="158"/>
+      <c r="AJ13" s="158"/>
+      <c r="AK13" s="158"/>
+      <c r="AL13" s="158"/>
+      <c r="AM13" s="158"/>
+      <c r="AN13" s="158"/>
+      <c r="AO13" s="158"/>
+      <c r="AP13" s="158"/>
+      <c r="AQ13" s="158"/>
+      <c r="AR13" s="158"/>
+      <c r="AS13" s="158"/>
+      <c r="AT13" s="158"/>
+      <c r="AU13" s="158"/>
+      <c r="AV13" s="158"/>
+      <c r="AW13" s="158"/>
+      <c r="AX13" s="158"/>
+      <c r="AY13" s="158"/>
+      <c r="AZ13" s="158"/>
+      <c r="BA13" s="158"/>
+      <c r="BB13" s="158"/>
+      <c r="BC13" s="158"/>
+      <c r="BD13" s="158"/>
+      <c r="BE13" s="158"/>
+      <c r="BF13" s="158"/>
+      <c r="BG13" s="158"/>
+      <c r="BH13" s="158"/>
+      <c r="BI13" s="158"/>
+      <c r="BJ13" s="158"/>
+      <c r="BK13" s="158"/>
+      <c r="BL13" s="158"/>
+      <c r="BM13" s="158"/>
+      <c r="BN13" s="158"/>
+      <c r="BO13" s="158"/>
+      <c r="BP13" s="158"/>
+      <c r="BQ13" s="158"/>
+      <c r="BR13" s="158"/>
+      <c r="BS13" s="158"/>
+      <c r="BT13" s="158"/>
+      <c r="BU13" s="158"/>
+      <c r="BV13" s="158"/>
+      <c r="BW13" s="158"/>
+      <c r="BX13" s="158"/>
+      <c r="BY13" s="158"/>
+      <c r="BZ13" s="158"/>
+      <c r="CA13" s="158"/>
+      <c r="CB13" s="158"/>
+      <c r="CC13" s="158"/>
+      <c r="CD13" s="158"/>
+      <c r="CE13" s="158"/>
+      <c r="CF13" s="158"/>
+      <c r="CG13" s="158"/>
+      <c r="CH13" s="158"/>
+      <c r="CI13" s="158"/>
+      <c r="CJ13" s="158"/>
+      <c r="CK13" s="158"/>
+      <c r="CL13" s="158"/>
       <c r="CM13" s="2"/>
       <c r="CN13" s="2"/>
       <c r="CO13" s="2"/>
@@ -32228,100 +32232,100 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="85"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="159" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="159" t="e">
+      <c r="C14" s="159"/>
+      <c r="D14" s="160" t="e">
         <f aca="false">_xlfn.STDEV.S(E13,G13,I13,K13,M13,O13,Q13,S13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E14" s="156"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="156"/>
-      <c r="H14" s="156"/>
-      <c r="I14" s="156"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="156"/>
-      <c r="M14" s="156"/>
-      <c r="N14" s="156"/>
-      <c r="O14" s="156"/>
-      <c r="P14" s="156"/>
-      <c r="Q14" s="156"/>
-      <c r="R14" s="156"/>
-      <c r="S14" s="156"/>
-      <c r="T14" s="156"/>
-      <c r="U14" s="152"/>
-      <c r="V14" s="152"/>
-      <c r="W14" s="152"/>
-      <c r="X14" s="152"/>
-      <c r="Y14" s="152"/>
-      <c r="Z14" s="152"/>
-      <c r="AA14" s="152"/>
-      <c r="AB14" s="152"/>
-      <c r="AC14" s="152"/>
-      <c r="AD14" s="152"/>
-      <c r="AE14" s="152"/>
-      <c r="AF14" s="152"/>
-      <c r="AG14" s="152"/>
-      <c r="AH14" s="152"/>
-      <c r="AI14" s="152"/>
-      <c r="AJ14" s="152"/>
-      <c r="AK14" s="152"/>
-      <c r="AL14" s="152"/>
-      <c r="AM14" s="152"/>
-      <c r="AN14" s="152"/>
-      <c r="AO14" s="152"/>
-      <c r="AP14" s="152"/>
-      <c r="AQ14" s="152"/>
-      <c r="AR14" s="152"/>
-      <c r="AS14" s="152"/>
-      <c r="AT14" s="152"/>
-      <c r="AU14" s="152"/>
-      <c r="AV14" s="152"/>
-      <c r="AW14" s="152"/>
-      <c r="AX14" s="152"/>
-      <c r="AY14" s="152"/>
-      <c r="AZ14" s="152"/>
-      <c r="BA14" s="152"/>
-      <c r="BB14" s="152"/>
-      <c r="BC14" s="152"/>
-      <c r="BD14" s="152"/>
-      <c r="BE14" s="152"/>
-      <c r="BF14" s="152"/>
-      <c r="BG14" s="152"/>
-      <c r="BH14" s="152"/>
-      <c r="BI14" s="152"/>
-      <c r="BJ14" s="152"/>
-      <c r="BK14" s="152"/>
-      <c r="BL14" s="152"/>
-      <c r="BM14" s="152"/>
-      <c r="BN14" s="152"/>
-      <c r="BO14" s="152"/>
-      <c r="BP14" s="152"/>
-      <c r="BQ14" s="152"/>
-      <c r="BR14" s="152"/>
-      <c r="BS14" s="152"/>
-      <c r="BT14" s="152"/>
-      <c r="BU14" s="152"/>
-      <c r="BV14" s="152"/>
-      <c r="BW14" s="152"/>
-      <c r="BX14" s="152"/>
-      <c r="BY14" s="152"/>
-      <c r="BZ14" s="152"/>
-      <c r="CA14" s="152"/>
-      <c r="CB14" s="152"/>
-      <c r="CC14" s="152"/>
-      <c r="CD14" s="152"/>
-      <c r="CE14" s="152"/>
-      <c r="CF14" s="152"/>
-      <c r="CG14" s="152"/>
-      <c r="CH14" s="152"/>
-      <c r="CI14" s="152"/>
-      <c r="CJ14" s="152"/>
-      <c r="CK14" s="152"/>
-      <c r="CL14" s="152"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="157"/>
+      <c r="K14" s="157"/>
+      <c r="L14" s="157"/>
+      <c r="M14" s="157"/>
+      <c r="N14" s="157"/>
+      <c r="O14" s="157"/>
+      <c r="P14" s="157"/>
+      <c r="Q14" s="157"/>
+      <c r="R14" s="157"/>
+      <c r="S14" s="157"/>
+      <c r="T14" s="157"/>
+      <c r="U14" s="153"/>
+      <c r="V14" s="153"/>
+      <c r="W14" s="153"/>
+      <c r="X14" s="153"/>
+      <c r="Y14" s="153"/>
+      <c r="Z14" s="153"/>
+      <c r="AA14" s="153"/>
+      <c r="AB14" s="153"/>
+      <c r="AC14" s="153"/>
+      <c r="AD14" s="153"/>
+      <c r="AE14" s="153"/>
+      <c r="AF14" s="153"/>
+      <c r="AG14" s="153"/>
+      <c r="AH14" s="153"/>
+      <c r="AI14" s="153"/>
+      <c r="AJ14" s="153"/>
+      <c r="AK14" s="153"/>
+      <c r="AL14" s="153"/>
+      <c r="AM14" s="153"/>
+      <c r="AN14" s="153"/>
+      <c r="AO14" s="153"/>
+      <c r="AP14" s="153"/>
+      <c r="AQ14" s="153"/>
+      <c r="AR14" s="153"/>
+      <c r="AS14" s="153"/>
+      <c r="AT14" s="153"/>
+      <c r="AU14" s="153"/>
+      <c r="AV14" s="153"/>
+      <c r="AW14" s="153"/>
+      <c r="AX14" s="153"/>
+      <c r="AY14" s="153"/>
+      <c r="AZ14" s="153"/>
+      <c r="BA14" s="153"/>
+      <c r="BB14" s="153"/>
+      <c r="BC14" s="153"/>
+      <c r="BD14" s="153"/>
+      <c r="BE14" s="153"/>
+      <c r="BF14" s="153"/>
+      <c r="BG14" s="153"/>
+      <c r="BH14" s="153"/>
+      <c r="BI14" s="153"/>
+      <c r="BJ14" s="153"/>
+      <c r="BK14" s="153"/>
+      <c r="BL14" s="153"/>
+      <c r="BM14" s="153"/>
+      <c r="BN14" s="153"/>
+      <c r="BO14" s="153"/>
+      <c r="BP14" s="153"/>
+      <c r="BQ14" s="153"/>
+      <c r="BR14" s="153"/>
+      <c r="BS14" s="153"/>
+      <c r="BT14" s="153"/>
+      <c r="BU14" s="153"/>
+      <c r="BV14" s="153"/>
+      <c r="BW14" s="153"/>
+      <c r="BX14" s="153"/>
+      <c r="BY14" s="153"/>
+      <c r="BZ14" s="153"/>
+      <c r="CA14" s="153"/>
+      <c r="CB14" s="153"/>
+      <c r="CC14" s="153"/>
+      <c r="CD14" s="153"/>
+      <c r="CE14" s="153"/>
+      <c r="CF14" s="153"/>
+      <c r="CG14" s="153"/>
+      <c r="CH14" s="153"/>
+      <c r="CI14" s="153"/>
+      <c r="CJ14" s="153"/>
+      <c r="CK14" s="153"/>
+      <c r="CL14" s="153"/>
       <c r="CM14" s="2"/>
       <c r="CN14" s="2"/>
       <c r="CO14" s="2"/>
@@ -32339,152 +32343,152 @@
       <c r="DA14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="124"/>
-      <c r="B15" s="160" t="s">
+      <c r="A15" s="125"/>
+      <c r="B15" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="154" t="str">
+      <c r="C15" s="155" t="str">
         <f aca="false">IF(C13="","",IF(C13&lt;$C$40,$C$37,IF(C13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="D15" s="155" t="str">
+      <c r="D15" s="156" t="str">
         <f aca="false">IF(D13="","",IF(D13&lt;$C$40,$C$37,IF(D13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="E15" s="155" t="str">
+      <c r="E15" s="156" t="str">
         <f aca="false">IF(E13="","",IF(E13&lt;$C$40,$C$37,IF(E13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="F15" s="155" t="str">
+      <c r="F15" s="156" t="str">
         <f aca="false">IF(F13="","",IF(F13&lt;$C$40,$C$37,IF(F13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="G15" s="161" t="str">
+      <c r="G15" s="162" t="str">
         <f aca="false">IF(G13="","",IF(G13&lt;$C$40,$C$37,IF(G13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="H15" s="155" t="str">
+      <c r="H15" s="156" t="str">
         <f aca="false">IF(H13="","",IF(H13&lt;$C$40,$C$37,IF(H13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="I15" s="161" t="str">
+      <c r="I15" s="162" t="str">
         <f aca="false">IF(I13="","",IF(I13&lt;$C$40,$C$37,IF(I13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="J15" s="155" t="str">
+      <c r="J15" s="156" t="str">
         <f aca="false">IF(J13="","",IF(J13&lt;$C$40,$C$37,IF(J13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="K15" s="161" t="str">
+      <c r="K15" s="162" t="str">
         <f aca="false">IF(K13="","",IF(K13&lt;$C$40,$C$37,IF(K13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="L15" s="155" t="str">
+      <c r="L15" s="156" t="str">
         <f aca="false">IF(L13="","",IF(L13&lt;$C$40,$C$37,IF(L13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="M15" s="161" t="str">
+      <c r="M15" s="162" t="str">
         <f aca="false">IF(M13="","",IF(M13&lt;$C$40,$C$37,IF(M13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="N15" s="155" t="str">
+      <c r="N15" s="156" t="str">
         <f aca="false">IF(N13="","",IF(N13&lt;$C$40,$C$37,IF(N13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="O15" s="161" t="str">
+      <c r="O15" s="162" t="str">
         <f aca="false">IF(O13="","",IF(O13&lt;$C$40,$C$37,IF(O13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="P15" s="155" t="str">
+      <c r="P15" s="156" t="str">
         <f aca="false">IF(P13="","",IF(P13&lt;$C$40,$C$37,IF(P13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="Q15" s="161" t="str">
+      <c r="Q15" s="162" t="str">
         <f aca="false">IF(Q13="","",IF(Q13&lt;$C$40,$C$37,IF(Q13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="R15" s="155" t="str">
+      <c r="R15" s="156" t="str">
         <f aca="false">IF(R13="","",IF(R13&lt;$C$40,$C$37,IF(R13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="S15" s="161" t="str">
+      <c r="S15" s="162" t="str">
         <f aca="false">IF(S13="","",IF(S13&lt;$C$40,$C$37,IF(S13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="T15" s="162" t="str">
+      <c r="T15" s="163" t="str">
         <f aca="false">IF(T13="","",IF(T13&lt;$C$40,$C$37,IF(T13&gt;=$E$40,$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="U15" s="157"/>
-      <c r="V15" s="157"/>
-      <c r="W15" s="157"/>
-      <c r="X15" s="157"/>
-      <c r="Y15" s="157"/>
-      <c r="Z15" s="157"/>
-      <c r="AA15" s="157"/>
-      <c r="AB15" s="157"/>
-      <c r="AC15" s="157"/>
-      <c r="AD15" s="157"/>
-      <c r="AE15" s="157"/>
-      <c r="AF15" s="157"/>
-      <c r="AG15" s="157"/>
-      <c r="AH15" s="157"/>
-      <c r="AI15" s="157"/>
-      <c r="AJ15" s="157"/>
-      <c r="AK15" s="157"/>
-      <c r="AL15" s="157"/>
-      <c r="AM15" s="157"/>
-      <c r="AN15" s="157"/>
-      <c r="AO15" s="157"/>
-      <c r="AP15" s="157"/>
-      <c r="AQ15" s="157"/>
-      <c r="AR15" s="157"/>
-      <c r="AS15" s="157"/>
-      <c r="AT15" s="157"/>
-      <c r="AU15" s="157"/>
-      <c r="AV15" s="157"/>
-      <c r="AW15" s="157"/>
-      <c r="AX15" s="157"/>
-      <c r="AY15" s="157"/>
-      <c r="AZ15" s="157"/>
-      <c r="BA15" s="157"/>
-      <c r="BB15" s="157"/>
-      <c r="BC15" s="157"/>
-      <c r="BD15" s="157"/>
-      <c r="BE15" s="157"/>
-      <c r="BF15" s="157"/>
-      <c r="BG15" s="157"/>
-      <c r="BH15" s="157"/>
-      <c r="BI15" s="157"/>
-      <c r="BJ15" s="157"/>
-      <c r="BK15" s="157"/>
-      <c r="BL15" s="157"/>
-      <c r="BM15" s="157"/>
-      <c r="BN15" s="157"/>
-      <c r="BO15" s="157"/>
-      <c r="BP15" s="157"/>
-      <c r="BQ15" s="157"/>
-      <c r="BR15" s="157"/>
-      <c r="BS15" s="157"/>
-      <c r="BT15" s="157"/>
-      <c r="BU15" s="157"/>
-      <c r="BV15" s="157"/>
-      <c r="BW15" s="157"/>
-      <c r="BX15" s="157"/>
-      <c r="BY15" s="157"/>
-      <c r="BZ15" s="157"/>
-      <c r="CA15" s="157"/>
-      <c r="CB15" s="157"/>
-      <c r="CC15" s="157"/>
-      <c r="CD15" s="157"/>
-      <c r="CE15" s="157"/>
-      <c r="CF15" s="157"/>
-      <c r="CG15" s="157"/>
-      <c r="CH15" s="157"/>
-      <c r="CI15" s="157"/>
-      <c r="CJ15" s="157"/>
-      <c r="CK15" s="157"/>
-      <c r="CL15" s="157"/>
+      <c r="U15" s="158"/>
+      <c r="V15" s="158"/>
+      <c r="W15" s="158"/>
+      <c r="X15" s="158"/>
+      <c r="Y15" s="158"/>
+      <c r="Z15" s="158"/>
+      <c r="AA15" s="158"/>
+      <c r="AB15" s="158"/>
+      <c r="AC15" s="158"/>
+      <c r="AD15" s="158"/>
+      <c r="AE15" s="158"/>
+      <c r="AF15" s="158"/>
+      <c r="AG15" s="158"/>
+      <c r="AH15" s="158"/>
+      <c r="AI15" s="158"/>
+      <c r="AJ15" s="158"/>
+      <c r="AK15" s="158"/>
+      <c r="AL15" s="158"/>
+      <c r="AM15" s="158"/>
+      <c r="AN15" s="158"/>
+      <c r="AO15" s="158"/>
+      <c r="AP15" s="158"/>
+      <c r="AQ15" s="158"/>
+      <c r="AR15" s="158"/>
+      <c r="AS15" s="158"/>
+      <c r="AT15" s="158"/>
+      <c r="AU15" s="158"/>
+      <c r="AV15" s="158"/>
+      <c r="AW15" s="158"/>
+      <c r="AX15" s="158"/>
+      <c r="AY15" s="158"/>
+      <c r="AZ15" s="158"/>
+      <c r="BA15" s="158"/>
+      <c r="BB15" s="158"/>
+      <c r="BC15" s="158"/>
+      <c r="BD15" s="158"/>
+      <c r="BE15" s="158"/>
+      <c r="BF15" s="158"/>
+      <c r="BG15" s="158"/>
+      <c r="BH15" s="158"/>
+      <c r="BI15" s="158"/>
+      <c r="BJ15" s="158"/>
+      <c r="BK15" s="158"/>
+      <c r="BL15" s="158"/>
+      <c r="BM15" s="158"/>
+      <c r="BN15" s="158"/>
+      <c r="BO15" s="158"/>
+      <c r="BP15" s="158"/>
+      <c r="BQ15" s="158"/>
+      <c r="BR15" s="158"/>
+      <c r="BS15" s="158"/>
+      <c r="BT15" s="158"/>
+      <c r="BU15" s="158"/>
+      <c r="BV15" s="158"/>
+      <c r="BW15" s="158"/>
+      <c r="BX15" s="158"/>
+      <c r="BY15" s="158"/>
+      <c r="BZ15" s="158"/>
+      <c r="CA15" s="158"/>
+      <c r="CB15" s="158"/>
+      <c r="CC15" s="158"/>
+      <c r="CD15" s="158"/>
+      <c r="CE15" s="158"/>
+      <c r="CF15" s="158"/>
+      <c r="CG15" s="158"/>
+      <c r="CH15" s="158"/>
+      <c r="CI15" s="158"/>
+      <c r="CJ15" s="158"/>
+      <c r="CK15" s="158"/>
+      <c r="CL15" s="158"/>
       <c r="CM15" s="2"/>
       <c r="CN15" s="2"/>
       <c r="CO15" s="2"/>
@@ -32502,25 +32506,25 @@
       <c r="DA15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="124"/>
-      <c r="B16" s="163"/>
-      <c r="C16" s="164"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="164"/>
-      <c r="G16" s="166"/>
+      <c r="A16" s="125"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="167"/>
       <c r="H16" s="116"/>
-      <c r="I16" s="166"/>
+      <c r="I16" s="167"/>
       <c r="J16" s="116"/>
-      <c r="K16" s="166"/>
+      <c r="K16" s="167"/>
       <c r="L16" s="116"/>
-      <c r="M16" s="166"/>
+      <c r="M16" s="167"/>
       <c r="N16" s="116"/>
-      <c r="O16" s="166"/>
+      <c r="O16" s="167"/>
       <c r="P16" s="116"/>
-      <c r="Q16" s="166"/>
+      <c r="Q16" s="167"/>
       <c r="R16" s="116"/>
-      <c r="S16" s="166"/>
+      <c r="S16" s="167"/>
       <c r="T16" s="118"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
@@ -32609,130 +32613,130 @@
       <c r="DA16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="167"/>
-      <c r="B17" s="168" t="s">
+      <c r="A17" s="168"/>
+      <c r="B17" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="168"/>
-      <c r="D17" s="168"/>
-      <c r="E17" s="169" t="s">
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="170" t="s">
+      <c r="F17" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="171" t="s">
+      <c r="G17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="172" t="s">
+      <c r="H17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="171" t="s">
+      <c r="I17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="172" t="s">
+      <c r="J17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="K17" s="171" t="s">
+      <c r="K17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="172" t="s">
+      <c r="L17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="M17" s="171" t="s">
+      <c r="M17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="172" t="s">
+      <c r="N17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="O17" s="171" t="s">
+      <c r="O17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="P17" s="172" t="s">
+      <c r="P17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="Q17" s="171" t="s">
+      <c r="Q17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="R17" s="172" t="s">
+      <c r="R17" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="S17" s="171" t="s">
+      <c r="S17" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="T17" s="173" t="s">
+      <c r="T17" s="174" t="s">
         <v>76</v>
       </c>
-      <c r="U17" s="138"/>
-      <c r="V17" s="138"/>
-      <c r="W17" s="138"/>
-      <c r="X17" s="138"/>
-      <c r="Y17" s="138"/>
-      <c r="Z17" s="138"/>
-      <c r="AA17" s="138"/>
-      <c r="AB17" s="138"/>
-      <c r="AC17" s="138"/>
-      <c r="AD17" s="138"/>
-      <c r="AE17" s="138"/>
-      <c r="AF17" s="138"/>
-      <c r="AG17" s="138"/>
-      <c r="AH17" s="138"/>
-      <c r="AI17" s="138"/>
-      <c r="AJ17" s="138"/>
-      <c r="AK17" s="138"/>
-      <c r="AL17" s="138"/>
-      <c r="AM17" s="138"/>
-      <c r="AN17" s="138"/>
-      <c r="AO17" s="138"/>
-      <c r="AP17" s="138"/>
-      <c r="AQ17" s="138"/>
-      <c r="AR17" s="138"/>
-      <c r="AS17" s="138"/>
-      <c r="AT17" s="138"/>
-      <c r="AU17" s="138"/>
-      <c r="AV17" s="138"/>
-      <c r="AW17" s="138"/>
-      <c r="AX17" s="138"/>
-      <c r="AY17" s="138"/>
-      <c r="AZ17" s="138"/>
-      <c r="BA17" s="138"/>
-      <c r="BB17" s="138"/>
-      <c r="BC17" s="138"/>
-      <c r="BD17" s="138"/>
-      <c r="BE17" s="138"/>
-      <c r="BF17" s="138"/>
-      <c r="BG17" s="138"/>
-      <c r="BH17" s="138"/>
-      <c r="BI17" s="138"/>
-      <c r="BJ17" s="138"/>
-      <c r="BK17" s="138"/>
-      <c r="BL17" s="138"/>
-      <c r="BM17" s="138"/>
-      <c r="BN17" s="138"/>
-      <c r="BO17" s="138"/>
-      <c r="BP17" s="138"/>
-      <c r="BQ17" s="138"/>
-      <c r="BR17" s="138"/>
-      <c r="BS17" s="138"/>
-      <c r="BT17" s="138"/>
-      <c r="BU17" s="138"/>
-      <c r="BV17" s="138"/>
-      <c r="BW17" s="138"/>
-      <c r="BX17" s="138"/>
-      <c r="BY17" s="138"/>
-      <c r="BZ17" s="138"/>
-      <c r="CA17" s="138"/>
-      <c r="CB17" s="138"/>
-      <c r="CC17" s="138"/>
-      <c r="CD17" s="138"/>
-      <c r="CE17" s="138"/>
-      <c r="CF17" s="138"/>
-      <c r="CG17" s="138"/>
-      <c r="CH17" s="138"/>
-      <c r="CI17" s="138"/>
-      <c r="CJ17" s="138"/>
-      <c r="CK17" s="138"/>
-      <c r="CL17" s="138"/>
+      <c r="U17" s="139"/>
+      <c r="V17" s="139"/>
+      <c r="W17" s="139"/>
+      <c r="X17" s="139"/>
+      <c r="Y17" s="139"/>
+      <c r="Z17" s="139"/>
+      <c r="AA17" s="139"/>
+      <c r="AB17" s="139"/>
+      <c r="AC17" s="139"/>
+      <c r="AD17" s="139"/>
+      <c r="AE17" s="139"/>
+      <c r="AF17" s="139"/>
+      <c r="AG17" s="139"/>
+      <c r="AH17" s="139"/>
+      <c r="AI17" s="139"/>
+      <c r="AJ17" s="139"/>
+      <c r="AK17" s="139"/>
+      <c r="AL17" s="139"/>
+      <c r="AM17" s="139"/>
+      <c r="AN17" s="139"/>
+      <c r="AO17" s="139"/>
+      <c r="AP17" s="139"/>
+      <c r="AQ17" s="139"/>
+      <c r="AR17" s="139"/>
+      <c r="AS17" s="139"/>
+      <c r="AT17" s="139"/>
+      <c r="AU17" s="139"/>
+      <c r="AV17" s="139"/>
+      <c r="AW17" s="139"/>
+      <c r="AX17" s="139"/>
+      <c r="AY17" s="139"/>
+      <c r="AZ17" s="139"/>
+      <c r="BA17" s="139"/>
+      <c r="BB17" s="139"/>
+      <c r="BC17" s="139"/>
+      <c r="BD17" s="139"/>
+      <c r="BE17" s="139"/>
+      <c r="BF17" s="139"/>
+      <c r="BG17" s="139"/>
+      <c r="BH17" s="139"/>
+      <c r="BI17" s="139"/>
+      <c r="BJ17" s="139"/>
+      <c r="BK17" s="139"/>
+      <c r="BL17" s="139"/>
+      <c r="BM17" s="139"/>
+      <c r="BN17" s="139"/>
+      <c r="BO17" s="139"/>
+      <c r="BP17" s="139"/>
+      <c r="BQ17" s="139"/>
+      <c r="BR17" s="139"/>
+      <c r="BS17" s="139"/>
+      <c r="BT17" s="139"/>
+      <c r="BU17" s="139"/>
+      <c r="BV17" s="139"/>
+      <c r="BW17" s="139"/>
+      <c r="BX17" s="139"/>
+      <c r="BY17" s="139"/>
+      <c r="BZ17" s="139"/>
+      <c r="CA17" s="139"/>
+      <c r="CB17" s="139"/>
+      <c r="CC17" s="139"/>
+      <c r="CD17" s="139"/>
+      <c r="CE17" s="139"/>
+      <c r="CF17" s="139"/>
+      <c r="CG17" s="139"/>
+      <c r="CH17" s="139"/>
+      <c r="CI17" s="139"/>
+      <c r="CJ17" s="139"/>
+      <c r="CK17" s="139"/>
+      <c r="CL17" s="139"/>
       <c r="CM17" s="2"/>
       <c r="CN17" s="2"/>
       <c r="CO17" s="2"/>
@@ -32750,146 +32754,146 @@
       <c r="DA17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="174"/>
-      <c r="B18" s="175" t="s">
+      <c r="A18" s="175"/>
+      <c r="B18" s="176" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="175"/>
-      <c r="D18" s="175"/>
-      <c r="E18" s="141" t="n">
+      <c r="C18" s="176"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="142" t="n">
         <f aca="false">IF(E8="No user",0,COUNTIF(Calculation!E13:G42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="F18" s="176" t="str">
+      <c r="F18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",E18/$G$29)</f>
         <v/>
       </c>
-      <c r="G18" s="141" t="n">
+      <c r="G18" s="142" t="n">
         <f aca="false">IF(G8="No user",0,COUNTIF(Calculation!H13:J42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="H18" s="176" t="str">
+      <c r="H18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",G18/$G$29)</f>
         <v/>
       </c>
-      <c r="I18" s="141" t="n">
+      <c r="I18" s="142" t="n">
         <f aca="false">IF(I8="No user",0,COUNTIF(Calculation!K13:M42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="J18" s="176" t="str">
+      <c r="J18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",I18/$G$29)</f>
         <v/>
       </c>
-      <c r="K18" s="141" t="n">
+      <c r="K18" s="142" t="n">
         <f aca="false">IF(K8="No user",0,COUNTIF(Calculation!N13:P42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="L18" s="176" t="str">
+      <c r="L18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",K18/$G$29)</f>
         <v/>
       </c>
-      <c r="M18" s="141" t="n">
+      <c r="M18" s="142" t="n">
         <f aca="false">IF(M8="No user",0,COUNTIF(Calculation!Q13:S42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="N18" s="176" t="str">
+      <c r="N18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",M18/$G$29)</f>
         <v/>
       </c>
-      <c r="O18" s="141" t="n">
+      <c r="O18" s="142" t="n">
         <f aca="false">IF(O8="No user",0,COUNTIF(Calculation!T13:V42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="P18" s="176" t="str">
+      <c r="P18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",O18/$G$29)</f>
         <v/>
       </c>
-      <c r="Q18" s="141" t="n">
+      <c r="Q18" s="142" t="n">
         <f aca="false">IF(Q8="No user",0,COUNTIF(Calculation!W13:Y42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="R18" s="176" t="str">
+      <c r="R18" s="177" t="str">
         <f aca="false">IF($G$29=0,"",Q18/$G$29)</f>
         <v/>
       </c>
-      <c r="S18" s="141" t="n">
+      <c r="S18" s="142" t="n">
         <f aca="false">IF(S8="No user",0,COUNTIF(Calculation!Z13:AB42,"=0"))</f>
         <v>0</v>
       </c>
-      <c r="T18" s="177" t="str">
+      <c r="T18" s="178" t="str">
         <f aca="false">IF($G$29=0,"",S18/$G$29)</f>
         <v/>
       </c>
-      <c r="U18" s="143"/>
-      <c r="V18" s="178"/>
-      <c r="W18" s="143"/>
-      <c r="X18" s="178"/>
-      <c r="Y18" s="143"/>
-      <c r="Z18" s="178"/>
-      <c r="AA18" s="143"/>
-      <c r="AB18" s="178"/>
-      <c r="AC18" s="143"/>
-      <c r="AD18" s="178"/>
-      <c r="AE18" s="143"/>
-      <c r="AF18" s="178"/>
-      <c r="AG18" s="143"/>
-      <c r="AH18" s="178"/>
-      <c r="AI18" s="143"/>
-      <c r="AJ18" s="178"/>
-      <c r="AK18" s="143"/>
-      <c r="AL18" s="178"/>
-      <c r="AM18" s="143"/>
-      <c r="AN18" s="178"/>
-      <c r="AO18" s="143"/>
-      <c r="AP18" s="178"/>
-      <c r="AQ18" s="143"/>
-      <c r="AR18" s="178"/>
-      <c r="AS18" s="143"/>
-      <c r="AT18" s="178"/>
-      <c r="AU18" s="143"/>
-      <c r="AV18" s="178"/>
-      <c r="AW18" s="143"/>
-      <c r="AX18" s="178"/>
-      <c r="AY18" s="143"/>
-      <c r="AZ18" s="178"/>
-      <c r="BA18" s="143"/>
-      <c r="BB18" s="178"/>
-      <c r="BC18" s="143"/>
-      <c r="BD18" s="178"/>
-      <c r="BE18" s="143"/>
-      <c r="BF18" s="178"/>
-      <c r="BG18" s="143"/>
-      <c r="BH18" s="178"/>
-      <c r="BI18" s="143"/>
-      <c r="BJ18" s="178"/>
-      <c r="BK18" s="143"/>
-      <c r="BL18" s="178"/>
-      <c r="BM18" s="143"/>
-      <c r="BN18" s="178"/>
-      <c r="BO18" s="143"/>
-      <c r="BP18" s="178"/>
-      <c r="BQ18" s="143"/>
-      <c r="BR18" s="178"/>
-      <c r="BS18" s="143"/>
-      <c r="BT18" s="178"/>
-      <c r="BU18" s="143"/>
-      <c r="BV18" s="178"/>
-      <c r="BW18" s="143"/>
-      <c r="BX18" s="178"/>
-      <c r="BY18" s="143"/>
-      <c r="BZ18" s="178"/>
-      <c r="CA18" s="143"/>
-      <c r="CB18" s="178"/>
-      <c r="CC18" s="143"/>
-      <c r="CD18" s="178"/>
-      <c r="CE18" s="143"/>
-      <c r="CF18" s="178"/>
-      <c r="CG18" s="143"/>
-      <c r="CH18" s="178"/>
-      <c r="CI18" s="143"/>
-      <c r="CJ18" s="178"/>
-      <c r="CK18" s="143"/>
-      <c r="CL18" s="178"/>
+      <c r="U18" s="144"/>
+      <c r="V18" s="179"/>
+      <c r="W18" s="144"/>
+      <c r="X18" s="179"/>
+      <c r="Y18" s="144"/>
+      <c r="Z18" s="179"/>
+      <c r="AA18" s="144"/>
+      <c r="AB18" s="179"/>
+      <c r="AC18" s="144"/>
+      <c r="AD18" s="179"/>
+      <c r="AE18" s="144"/>
+      <c r="AF18" s="179"/>
+      <c r="AG18" s="144"/>
+      <c r="AH18" s="179"/>
+      <c r="AI18" s="144"/>
+      <c r="AJ18" s="179"/>
+      <c r="AK18" s="144"/>
+      <c r="AL18" s="179"/>
+      <c r="AM18" s="144"/>
+      <c r="AN18" s="179"/>
+      <c r="AO18" s="144"/>
+      <c r="AP18" s="179"/>
+      <c r="AQ18" s="144"/>
+      <c r="AR18" s="179"/>
+      <c r="AS18" s="144"/>
+      <c r="AT18" s="179"/>
+      <c r="AU18" s="144"/>
+      <c r="AV18" s="179"/>
+      <c r="AW18" s="144"/>
+      <c r="AX18" s="179"/>
+      <c r="AY18" s="144"/>
+      <c r="AZ18" s="179"/>
+      <c r="BA18" s="144"/>
+      <c r="BB18" s="179"/>
+      <c r="BC18" s="144"/>
+      <c r="BD18" s="179"/>
+      <c r="BE18" s="144"/>
+      <c r="BF18" s="179"/>
+      <c r="BG18" s="144"/>
+      <c r="BH18" s="179"/>
+      <c r="BI18" s="144"/>
+      <c r="BJ18" s="179"/>
+      <c r="BK18" s="144"/>
+      <c r="BL18" s="179"/>
+      <c r="BM18" s="144"/>
+      <c r="BN18" s="179"/>
+      <c r="BO18" s="144"/>
+      <c r="BP18" s="179"/>
+      <c r="BQ18" s="144"/>
+      <c r="BR18" s="179"/>
+      <c r="BS18" s="144"/>
+      <c r="BT18" s="179"/>
+      <c r="BU18" s="144"/>
+      <c r="BV18" s="179"/>
+      <c r="BW18" s="144"/>
+      <c r="BX18" s="179"/>
+      <c r="BY18" s="144"/>
+      <c r="BZ18" s="179"/>
+      <c r="CA18" s="144"/>
+      <c r="CB18" s="179"/>
+      <c r="CC18" s="144"/>
+      <c r="CD18" s="179"/>
+      <c r="CE18" s="144"/>
+      <c r="CF18" s="179"/>
+      <c r="CG18" s="144"/>
+      <c r="CH18" s="179"/>
+      <c r="CI18" s="144"/>
+      <c r="CJ18" s="179"/>
+      <c r="CK18" s="144"/>
+      <c r="CL18" s="179"/>
       <c r="CM18" s="2"/>
       <c r="CN18" s="2"/>
       <c r="CO18" s="2"/>
@@ -32908,145 +32912,145 @@
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="85"/>
-      <c r="B19" s="179" t="s">
+      <c r="B19" s="180" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="179"/>
-      <c r="D19" s="179"/>
-      <c r="E19" s="141" t="n">
+      <c r="C19" s="180"/>
+      <c r="D19" s="180"/>
+      <c r="E19" s="142" t="n">
         <f aca="false">IF(E9="No user",0,COUNTIF(Calculation!E14:G43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="F19" s="176" t="str">
+      <c r="F19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",E19/$G$29)</f>
         <v/>
       </c>
-      <c r="G19" s="141" t="n">
+      <c r="G19" s="142" t="n">
         <f aca="false">IF(G9="No user",0,COUNTIF(Calculation!H14:J43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="H19" s="176" t="str">
+      <c r="H19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",G19/$G$29)</f>
         <v/>
       </c>
-      <c r="I19" s="141" t="n">
+      <c r="I19" s="142" t="n">
         <f aca="false">IF(I9="No user",0,COUNTIF(Calculation!K14:M43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="J19" s="176" t="str">
+      <c r="J19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",I19/$G$29)</f>
         <v/>
       </c>
-      <c r="K19" s="141" t="n">
+      <c r="K19" s="142" t="n">
         <f aca="false">IF(K9="No user",0,COUNTIF(Calculation!N14:P43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="L19" s="176" t="str">
+      <c r="L19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",K19/$G$29)</f>
         <v/>
       </c>
-      <c r="M19" s="141" t="n">
+      <c r="M19" s="142" t="n">
         <f aca="false">IF(M9="No user",0,COUNTIF(Calculation!Q14:S43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="N19" s="176" t="str">
+      <c r="N19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",M19/$G$29)</f>
         <v/>
       </c>
-      <c r="O19" s="141" t="n">
+      <c r="O19" s="142" t="n">
         <f aca="false">IF(O9="No user",0,COUNTIF(Calculation!T14:V43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="P19" s="176" t="str">
+      <c r="P19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",O19/$G$29)</f>
         <v/>
       </c>
-      <c r="Q19" s="141" t="n">
+      <c r="Q19" s="142" t="n">
         <f aca="false">IF(Q9="No user",0,COUNTIF(Calculation!W14:Y43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="R19" s="176" t="str">
+      <c r="R19" s="177" t="str">
         <f aca="false">IF($G$29=0,"",Q19/$G$29)</f>
         <v/>
       </c>
-      <c r="S19" s="141" t="n">
+      <c r="S19" s="142" t="n">
         <f aca="false">IF(S9="No user",0,COUNTIF(Calculation!Z14:AB43,"=-1"))</f>
         <v>0</v>
       </c>
-      <c r="T19" s="177" t="str">
+      <c r="T19" s="178" t="str">
         <f aca="false">IF($G$29=0,"",S19/$G$29)</f>
         <v/>
       </c>
-      <c r="U19" s="143"/>
-      <c r="V19" s="178"/>
-      <c r="W19" s="143"/>
-      <c r="X19" s="178"/>
-      <c r="Y19" s="143"/>
-      <c r="Z19" s="178"/>
-      <c r="AA19" s="143"/>
-      <c r="AB19" s="178"/>
-      <c r="AC19" s="143"/>
-      <c r="AD19" s="178"/>
-      <c r="AE19" s="143"/>
-      <c r="AF19" s="178"/>
-      <c r="AG19" s="143"/>
-      <c r="AH19" s="178"/>
-      <c r="AI19" s="143"/>
-      <c r="AJ19" s="178"/>
-      <c r="AK19" s="143"/>
-      <c r="AL19" s="178"/>
-      <c r="AM19" s="143"/>
-      <c r="AN19" s="178"/>
-      <c r="AO19" s="143"/>
-      <c r="AP19" s="178"/>
-      <c r="AQ19" s="143"/>
-      <c r="AR19" s="178"/>
-      <c r="AS19" s="143"/>
-      <c r="AT19" s="178"/>
-      <c r="AU19" s="143"/>
-      <c r="AV19" s="178"/>
-      <c r="AW19" s="143"/>
-      <c r="AX19" s="178"/>
-      <c r="AY19" s="143"/>
-      <c r="AZ19" s="178"/>
-      <c r="BA19" s="143"/>
-      <c r="BB19" s="178"/>
-      <c r="BC19" s="143"/>
-      <c r="BD19" s="178"/>
-      <c r="BE19" s="143"/>
-      <c r="BF19" s="178"/>
-      <c r="BG19" s="143"/>
-      <c r="BH19" s="178"/>
-      <c r="BI19" s="143"/>
-      <c r="BJ19" s="178"/>
-      <c r="BK19" s="143"/>
-      <c r="BL19" s="178"/>
-      <c r="BM19" s="143"/>
-      <c r="BN19" s="178"/>
-      <c r="BO19" s="143"/>
-      <c r="BP19" s="178"/>
-      <c r="BQ19" s="143"/>
-      <c r="BR19" s="178"/>
-      <c r="BS19" s="143"/>
-      <c r="BT19" s="178"/>
-      <c r="BU19" s="143"/>
-      <c r="BV19" s="178"/>
-      <c r="BW19" s="143"/>
-      <c r="BX19" s="178"/>
-      <c r="BY19" s="143"/>
-      <c r="BZ19" s="178"/>
-      <c r="CA19" s="143"/>
-      <c r="CB19" s="178"/>
-      <c r="CC19" s="143"/>
-      <c r="CD19" s="178"/>
-      <c r="CE19" s="143"/>
-      <c r="CF19" s="178"/>
-      <c r="CG19" s="143"/>
-      <c r="CH19" s="178"/>
-      <c r="CI19" s="143"/>
-      <c r="CJ19" s="178"/>
-      <c r="CK19" s="143"/>
-      <c r="CL19" s="178"/>
+      <c r="U19" s="144"/>
+      <c r="V19" s="179"/>
+      <c r="W19" s="144"/>
+      <c r="X19" s="179"/>
+      <c r="Y19" s="144"/>
+      <c r="Z19" s="179"/>
+      <c r="AA19" s="144"/>
+      <c r="AB19" s="179"/>
+      <c r="AC19" s="144"/>
+      <c r="AD19" s="179"/>
+      <c r="AE19" s="144"/>
+      <c r="AF19" s="179"/>
+      <c r="AG19" s="144"/>
+      <c r="AH19" s="179"/>
+      <c r="AI19" s="144"/>
+      <c r="AJ19" s="179"/>
+      <c r="AK19" s="144"/>
+      <c r="AL19" s="179"/>
+      <c r="AM19" s="144"/>
+      <c r="AN19" s="179"/>
+      <c r="AO19" s="144"/>
+      <c r="AP19" s="179"/>
+      <c r="AQ19" s="144"/>
+      <c r="AR19" s="179"/>
+      <c r="AS19" s="144"/>
+      <c r="AT19" s="179"/>
+      <c r="AU19" s="144"/>
+      <c r="AV19" s="179"/>
+      <c r="AW19" s="144"/>
+      <c r="AX19" s="179"/>
+      <c r="AY19" s="144"/>
+      <c r="AZ19" s="179"/>
+      <c r="BA19" s="144"/>
+      <c r="BB19" s="179"/>
+      <c r="BC19" s="144"/>
+      <c r="BD19" s="179"/>
+      <c r="BE19" s="144"/>
+      <c r="BF19" s="179"/>
+      <c r="BG19" s="144"/>
+      <c r="BH19" s="179"/>
+      <c r="BI19" s="144"/>
+      <c r="BJ19" s="179"/>
+      <c r="BK19" s="144"/>
+      <c r="BL19" s="179"/>
+      <c r="BM19" s="144"/>
+      <c r="BN19" s="179"/>
+      <c r="BO19" s="144"/>
+      <c r="BP19" s="179"/>
+      <c r="BQ19" s="144"/>
+      <c r="BR19" s="179"/>
+      <c r="BS19" s="144"/>
+      <c r="BT19" s="179"/>
+      <c r="BU19" s="144"/>
+      <c r="BV19" s="179"/>
+      <c r="BW19" s="144"/>
+      <c r="BX19" s="179"/>
+      <c r="BY19" s="144"/>
+      <c r="BZ19" s="179"/>
+      <c r="CA19" s="144"/>
+      <c r="CB19" s="179"/>
+      <c r="CC19" s="144"/>
+      <c r="CD19" s="179"/>
+      <c r="CE19" s="144"/>
+      <c r="CF19" s="179"/>
+      <c r="CG19" s="144"/>
+      <c r="CH19" s="179"/>
+      <c r="CI19" s="144"/>
+      <c r="CJ19" s="179"/>
+      <c r="CK19" s="144"/>
+      <c r="CL19" s="179"/>
       <c r="CM19" s="2"/>
       <c r="CN19" s="2"/>
       <c r="CO19" s="2"/>
@@ -33065,145 +33069,145 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="85"/>
-      <c r="B20" s="179" t="s">
+      <c r="B20" s="180" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="179"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="146" t="n">
+      <c r="C20" s="180"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="147" t="n">
         <f aca="false">SUM(E18:E19)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="180" t="str">
+      <c r="F20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",E20/$G$29)</f>
         <v/>
       </c>
-      <c r="G20" s="146" t="n">
+      <c r="G20" s="147" t="n">
         <f aca="false">SUM(G18:G19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="180" t="str">
+      <c r="H20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",G20/$G$29)</f>
         <v/>
       </c>
-      <c r="I20" s="146" t="n">
+      <c r="I20" s="147" t="n">
         <f aca="false">SUM(I18:I19)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="180" t="str">
+      <c r="J20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",I20/$G$29)</f>
         <v/>
       </c>
-      <c r="K20" s="146" t="n">
+      <c r="K20" s="147" t="n">
         <f aca="false">SUM(K18:K19)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="180" t="str">
+      <c r="L20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",K20/$G$29)</f>
         <v/>
       </c>
-      <c r="M20" s="146" t="n">
+      <c r="M20" s="147" t="n">
         <f aca="false">SUM(M18:M19)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="180" t="str">
+      <c r="N20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",M20/$G$29)</f>
         <v/>
       </c>
-      <c r="O20" s="146" t="n">
+      <c r="O20" s="147" t="n">
         <f aca="false">SUM(O18:O19)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="180" t="str">
+      <c r="P20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",O20/$G$29)</f>
         <v/>
       </c>
-      <c r="Q20" s="146" t="n">
+      <c r="Q20" s="147" t="n">
         <f aca="false">SUM(Q18:Q19)</f>
         <v>0</v>
       </c>
-      <c r="R20" s="180" t="str">
+      <c r="R20" s="181" t="str">
         <f aca="false">IF($G$29=0,"",Q20/$G$29)</f>
         <v/>
       </c>
-      <c r="S20" s="146" t="n">
+      <c r="S20" s="147" t="n">
         <f aca="false">SUM(S18:S19)</f>
         <v>0</v>
       </c>
-      <c r="T20" s="181" t="str">
+      <c r="T20" s="182" t="str">
         <f aca="false">IF($G$29=0,"",S20/$G$29)</f>
         <v/>
       </c>
-      <c r="U20" s="143"/>
-      <c r="V20" s="178"/>
-      <c r="W20" s="143"/>
-      <c r="X20" s="178"/>
-      <c r="Y20" s="143"/>
-      <c r="Z20" s="178"/>
-      <c r="AA20" s="143"/>
-      <c r="AB20" s="178"/>
-      <c r="AC20" s="143"/>
-      <c r="AD20" s="178"/>
-      <c r="AE20" s="143"/>
-      <c r="AF20" s="178"/>
-      <c r="AG20" s="143"/>
-      <c r="AH20" s="178"/>
-      <c r="AI20" s="143"/>
-      <c r="AJ20" s="178"/>
-      <c r="AK20" s="143"/>
-      <c r="AL20" s="178"/>
-      <c r="AM20" s="143"/>
-      <c r="AN20" s="178"/>
-      <c r="AO20" s="143"/>
-      <c r="AP20" s="178"/>
-      <c r="AQ20" s="143"/>
-      <c r="AR20" s="178"/>
-      <c r="AS20" s="143"/>
-      <c r="AT20" s="178"/>
-      <c r="AU20" s="143"/>
-      <c r="AV20" s="178"/>
-      <c r="AW20" s="143"/>
-      <c r="AX20" s="178"/>
-      <c r="AY20" s="143"/>
-      <c r="AZ20" s="178"/>
-      <c r="BA20" s="143"/>
-      <c r="BB20" s="178"/>
-      <c r="BC20" s="143"/>
-      <c r="BD20" s="178"/>
-      <c r="BE20" s="143"/>
-      <c r="BF20" s="178"/>
-      <c r="BG20" s="143"/>
-      <c r="BH20" s="178"/>
-      <c r="BI20" s="143"/>
-      <c r="BJ20" s="178"/>
-      <c r="BK20" s="143"/>
-      <c r="BL20" s="178"/>
-      <c r="BM20" s="143"/>
-      <c r="BN20" s="178"/>
-      <c r="BO20" s="143"/>
-      <c r="BP20" s="178"/>
-      <c r="BQ20" s="143"/>
-      <c r="BR20" s="178"/>
-      <c r="BS20" s="143"/>
-      <c r="BT20" s="178"/>
-      <c r="BU20" s="143"/>
-      <c r="BV20" s="178"/>
-      <c r="BW20" s="143"/>
-      <c r="BX20" s="178"/>
-      <c r="BY20" s="143"/>
-      <c r="BZ20" s="178"/>
-      <c r="CA20" s="143"/>
-      <c r="CB20" s="178"/>
-      <c r="CC20" s="143"/>
-      <c r="CD20" s="178"/>
-      <c r="CE20" s="143"/>
-      <c r="CF20" s="178"/>
-      <c r="CG20" s="143"/>
-      <c r="CH20" s="178"/>
-      <c r="CI20" s="143"/>
-      <c r="CJ20" s="178"/>
-      <c r="CK20" s="143"/>
-      <c r="CL20" s="178"/>
+      <c r="U20" s="144"/>
+      <c r="V20" s="179"/>
+      <c r="W20" s="144"/>
+      <c r="X20" s="179"/>
+      <c r="Y20" s="144"/>
+      <c r="Z20" s="179"/>
+      <c r="AA20" s="144"/>
+      <c r="AB20" s="179"/>
+      <c r="AC20" s="144"/>
+      <c r="AD20" s="179"/>
+      <c r="AE20" s="144"/>
+      <c r="AF20" s="179"/>
+      <c r="AG20" s="144"/>
+      <c r="AH20" s="179"/>
+      <c r="AI20" s="144"/>
+      <c r="AJ20" s="179"/>
+      <c r="AK20" s="144"/>
+      <c r="AL20" s="179"/>
+      <c r="AM20" s="144"/>
+      <c r="AN20" s="179"/>
+      <c r="AO20" s="144"/>
+      <c r="AP20" s="179"/>
+      <c r="AQ20" s="144"/>
+      <c r="AR20" s="179"/>
+      <c r="AS20" s="144"/>
+      <c r="AT20" s="179"/>
+      <c r="AU20" s="144"/>
+      <c r="AV20" s="179"/>
+      <c r="AW20" s="144"/>
+      <c r="AX20" s="179"/>
+      <c r="AY20" s="144"/>
+      <c r="AZ20" s="179"/>
+      <c r="BA20" s="144"/>
+      <c r="BB20" s="179"/>
+      <c r="BC20" s="144"/>
+      <c r="BD20" s="179"/>
+      <c r="BE20" s="144"/>
+      <c r="BF20" s="179"/>
+      <c r="BG20" s="144"/>
+      <c r="BH20" s="179"/>
+      <c r="BI20" s="144"/>
+      <c r="BJ20" s="179"/>
+      <c r="BK20" s="144"/>
+      <c r="BL20" s="179"/>
+      <c r="BM20" s="144"/>
+      <c r="BN20" s="179"/>
+      <c r="BO20" s="144"/>
+      <c r="BP20" s="179"/>
+      <c r="BQ20" s="144"/>
+      <c r="BR20" s="179"/>
+      <c r="BS20" s="144"/>
+      <c r="BT20" s="179"/>
+      <c r="BU20" s="144"/>
+      <c r="BV20" s="179"/>
+      <c r="BW20" s="144"/>
+      <c r="BX20" s="179"/>
+      <c r="BY20" s="144"/>
+      <c r="BZ20" s="179"/>
+      <c r="CA20" s="144"/>
+      <c r="CB20" s="179"/>
+      <c r="CC20" s="144"/>
+      <c r="CD20" s="179"/>
+      <c r="CE20" s="144"/>
+      <c r="CF20" s="179"/>
+      <c r="CG20" s="144"/>
+      <c r="CH20" s="179"/>
+      <c r="CI20" s="144"/>
+      <c r="CJ20" s="179"/>
+      <c r="CK20" s="144"/>
+      <c r="CL20" s="179"/>
       <c r="CM20" s="2"/>
       <c r="CN20" s="2"/>
       <c r="CO20" s="2"/>
@@ -33221,122 +33225,122 @@
       <c r="DA20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="124"/>
-      <c r="B21" s="182" t="s">
+      <c r="A21" s="125"/>
+      <c r="B21" s="183" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="182"/>
-      <c r="D21" s="182"/>
-      <c r="E21" s="183"/>
-      <c r="F21" s="184" t="str">
+      <c r="C21" s="183"/>
+      <c r="D21" s="183"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="185" t="str">
         <f aca="false">IF(OR(F18="",F19=""),"",IF(OR(F18&gt;C38,F19&gt;C39),C37,IF(AND(F18&lt;=E38,F19&lt;=E39),E37,D37)))</f>
         <v/>
       </c>
-      <c r="G21" s="183"/>
-      <c r="H21" s="185" t="str">
+      <c r="G21" s="184"/>
+      <c r="H21" s="186" t="str">
         <f aca="false">IF(OR(H18="",H19=""),"",IF(OR(H18&gt;$C$38,H19&gt;$C$39),$C$37,IF(AND(H18&lt;=$E$38,H19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="I21" s="183"/>
-      <c r="J21" s="185" t="str">
+      <c r="I21" s="184"/>
+      <c r="J21" s="186" t="str">
         <f aca="false">IF(OR(J18="",J19=""),"",IF(OR(J18&gt;$C$38,J19&gt;$C$39),$C$37,IF(AND(J18&lt;=$E$38,J19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="K21" s="183"/>
-      <c r="L21" s="185" t="str">
+      <c r="K21" s="184"/>
+      <c r="L21" s="186" t="str">
         <f aca="false">IF(OR(L18="",L19=""),"",IF(OR(L18&gt;$C$38,L19&gt;$C$39),$C$37,IF(AND(L18&lt;=$E$38,L19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="M21" s="183"/>
-      <c r="N21" s="185" t="str">
+      <c r="M21" s="184"/>
+      <c r="N21" s="186" t="str">
         <f aca="false">IF(OR(N18="",N19=""),"",IF(OR(N18&gt;$C$38,N19&gt;$C$39),$C$37,IF(AND(N18&lt;=$E$38,N19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="O21" s="183"/>
-      <c r="P21" s="185" t="str">
+      <c r="O21" s="184"/>
+      <c r="P21" s="186" t="str">
         <f aca="false">IF(OR(P18="",P19=""),"",IF(OR(P18&gt;$C$38,P19&gt;$C$39),$C$37,IF(AND(P18&lt;=$E$38,P19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="Q21" s="183"/>
-      <c r="R21" s="185" t="str">
+      <c r="Q21" s="184"/>
+      <c r="R21" s="186" t="str">
         <f aca="false">IF(OR(R18="",R19=""),"",IF(OR(R18&gt;$C$38,R19&gt;$C$39),$C$37,IF(AND(R18&lt;=$E$38,R19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
-      <c r="S21" s="183"/>
-      <c r="T21" s="186" t="str">
+      <c r="S21" s="184"/>
+      <c r="T21" s="187" t="str">
         <f aca="false">IF(OR(T18="",T19=""),"",IF(OR(T18&gt;$C$38,T19&gt;$C$39),$C$37,IF(AND(T18&lt;=$E$38,T19&lt;=$E$39),$E$37,$D$37)))</f>
         <v/>
       </c>
       <c r="U21" s="2"/>
-      <c r="V21" s="157"/>
+      <c r="V21" s="158"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="157"/>
+      <c r="X21" s="158"/>
       <c r="Y21" s="2"/>
-      <c r="Z21" s="157"/>
+      <c r="Z21" s="158"/>
       <c r="AA21" s="2"/>
-      <c r="AB21" s="157"/>
+      <c r="AB21" s="158"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="157"/>
+      <c r="AD21" s="158"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="157"/>
+      <c r="AF21" s="158"/>
       <c r="AG21" s="2"/>
-      <c r="AH21" s="157"/>
+      <c r="AH21" s="158"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="157"/>
+      <c r="AJ21" s="158"/>
       <c r="AK21" s="2"/>
-      <c r="AL21" s="157"/>
+      <c r="AL21" s="158"/>
       <c r="AM21" s="2"/>
-      <c r="AN21" s="157"/>
+      <c r="AN21" s="158"/>
       <c r="AO21" s="2"/>
-      <c r="AP21" s="157"/>
+      <c r="AP21" s="158"/>
       <c r="AQ21" s="2"/>
-      <c r="AR21" s="157"/>
+      <c r="AR21" s="158"/>
       <c r="AS21" s="2"/>
-      <c r="AT21" s="157"/>
+      <c r="AT21" s="158"/>
       <c r="AU21" s="2"/>
-      <c r="AV21" s="157"/>
+      <c r="AV21" s="158"/>
       <c r="AW21" s="2"/>
-      <c r="AX21" s="157"/>
+      <c r="AX21" s="158"/>
       <c r="AY21" s="2"/>
-      <c r="AZ21" s="157"/>
+      <c r="AZ21" s="158"/>
       <c r="BA21" s="2"/>
-      <c r="BB21" s="157"/>
+      <c r="BB21" s="158"/>
       <c r="BC21" s="2"/>
-      <c r="BD21" s="157"/>
+      <c r="BD21" s="158"/>
       <c r="BE21" s="2"/>
-      <c r="BF21" s="157"/>
+      <c r="BF21" s="158"/>
       <c r="BG21" s="2"/>
-      <c r="BH21" s="157"/>
+      <c r="BH21" s="158"/>
       <c r="BI21" s="2"/>
-      <c r="BJ21" s="157"/>
+      <c r="BJ21" s="158"/>
       <c r="BK21" s="2"/>
-      <c r="BL21" s="157"/>
+      <c r="BL21" s="158"/>
       <c r="BM21" s="2"/>
-      <c r="BN21" s="157"/>
+      <c r="BN21" s="158"/>
       <c r="BO21" s="2"/>
-      <c r="BP21" s="157"/>
+      <c r="BP21" s="158"/>
       <c r="BQ21" s="2"/>
-      <c r="BR21" s="157"/>
+      <c r="BR21" s="158"/>
       <c r="BS21" s="2"/>
-      <c r="BT21" s="157"/>
+      <c r="BT21" s="158"/>
       <c r="BU21" s="2"/>
-      <c r="BV21" s="157"/>
+      <c r="BV21" s="158"/>
       <c r="BW21" s="2"/>
-      <c r="BX21" s="157"/>
+      <c r="BX21" s="158"/>
       <c r="BY21" s="2"/>
-      <c r="BZ21" s="157"/>
+      <c r="BZ21" s="158"/>
       <c r="CA21" s="2"/>
-      <c r="CB21" s="157"/>
+      <c r="CB21" s="158"/>
       <c r="CC21" s="2"/>
-      <c r="CD21" s="157"/>
+      <c r="CD21" s="158"/>
       <c r="CE21" s="2"/>
-      <c r="CF21" s="157"/>
+      <c r="CF21" s="158"/>
       <c r="CG21" s="2"/>
-      <c r="CH21" s="157"/>
+      <c r="CH21" s="158"/>
       <c r="CI21" s="2"/>
-      <c r="CJ21" s="157"/>
+      <c r="CJ21" s="158"/>
       <c r="CK21" s="2"/>
-      <c r="CL21" s="157"/>
+      <c r="CL21" s="158"/>
       <c r="CM21" s="2"/>
       <c r="CN21" s="2"/>
       <c r="CO21" s="2"/>
@@ -33355,7 +33359,7 @@
     </row>
     <row r="22" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="85"/>
-      <c r="B22" s="187"/>
+      <c r="B22" s="188"/>
       <c r="C22" s="116"/>
       <c r="D22" s="116"/>
       <c r="E22" s="116"/>
@@ -33462,14 +33466,14 @@
     </row>
     <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="85"/>
-      <c r="B23" s="188" t="s">
+      <c r="B23" s="189" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="188"/>
-      <c r="D23" s="188"/>
-      <c r="E23" s="188"/>
-      <c r="F23" s="188"/>
-      <c r="G23" s="188"/>
+      <c r="C23" s="189"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="189"/>
+      <c r="F23" s="189"/>
+      <c r="G23" s="189"/>
       <c r="H23" s="116"/>
       <c r="I23" s="116"/>
       <c r="J23" s="116"/>
@@ -33532,65 +33536,65 @@
       <c r="BV23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="124"/>
-      <c r="B24" s="189" t="s">
+      <c r="A24" s="125"/>
+      <c r="B24" s="190" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="190" t="e">
+      <c r="C24" s="191" t="e">
         <f aca="false">LARGE(E13:T13,1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D24" s="191" t="s">
+      <c r="D24" s="192" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="191"/>
-      <c r="F24" s="191"/>
-      <c r="G24" s="192" t="n">
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="193" t="n">
         <f aca="false">INDEX(Calculation!C13:C42, MATCH(MAX(Calculation!AE13:AE42), Calculation!AE13:AE42, 0))</f>
         <v>1</v>
       </c>
-      <c r="H24" s="148"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="148"/>
-      <c r="K24" s="148"/>
-      <c r="L24" s="148"/>
-      <c r="M24" s="148"/>
-      <c r="N24" s="148"/>
-      <c r="O24" s="148"/>
-      <c r="P24" s="148"/>
-      <c r="Q24" s="148"/>
-      <c r="R24" s="148"/>
-      <c r="S24" s="148"/>
-      <c r="T24" s="193"/>
-      <c r="U24" s="194"/>
-      <c r="V24" s="194"/>
-      <c r="W24" s="194"/>
-      <c r="X24" s="194"/>
-      <c r="Y24" s="194"/>
-      <c r="Z24" s="194"/>
-      <c r="AA24" s="194"/>
-      <c r="AB24" s="194"/>
-      <c r="AC24" s="194"/>
-      <c r="AD24" s="194"/>
-      <c r="AE24" s="194"/>
-      <c r="AF24" s="194"/>
-      <c r="AG24" s="194"/>
-      <c r="AH24" s="194"/>
-      <c r="AI24" s="194"/>
-      <c r="AJ24" s="194"/>
-      <c r="AK24" s="194"/>
-      <c r="AL24" s="194"/>
-      <c r="AM24" s="194"/>
-      <c r="AN24" s="194"/>
-      <c r="AO24" s="194"/>
-      <c r="AP24" s="194"/>
-      <c r="AQ24" s="194"/>
-      <c r="AR24" s="194"/>
-      <c r="AS24" s="194"/>
-      <c r="AT24" s="194"/>
-      <c r="AU24" s="194"/>
-      <c r="AV24" s="194"/>
-      <c r="AW24" s="194"/>
+      <c r="H24" s="149"/>
+      <c r="I24" s="149"/>
+      <c r="J24" s="149"/>
+      <c r="K24" s="149"/>
+      <c r="L24" s="149"/>
+      <c r="M24" s="149"/>
+      <c r="N24" s="149"/>
+      <c r="O24" s="149"/>
+      <c r="P24" s="149"/>
+      <c r="Q24" s="149"/>
+      <c r="R24" s="149"/>
+      <c r="S24" s="149"/>
+      <c r="T24" s="194"/>
+      <c r="U24" s="195"/>
+      <c r="V24" s="195"/>
+      <c r="W24" s="195"/>
+      <c r="X24" s="195"/>
+      <c r="Y24" s="195"/>
+      <c r="Z24" s="195"/>
+      <c r="AA24" s="195"/>
+      <c r="AB24" s="195"/>
+      <c r="AC24" s="195"/>
+      <c r="AD24" s="195"/>
+      <c r="AE24" s="195"/>
+      <c r="AF24" s="195"/>
+      <c r="AG24" s="195"/>
+      <c r="AH24" s="195"/>
+      <c r="AI24" s="195"/>
+      <c r="AJ24" s="195"/>
+      <c r="AK24" s="195"/>
+      <c r="AL24" s="195"/>
+      <c r="AM24" s="195"/>
+      <c r="AN24" s="195"/>
+      <c r="AO24" s="195"/>
+      <c r="AP24" s="195"/>
+      <c r="AQ24" s="195"/>
+      <c r="AR24" s="195"/>
+      <c r="AS24" s="195"/>
+      <c r="AT24" s="195"/>
+      <c r="AU24" s="195"/>
+      <c r="AV24" s="195"/>
+      <c r="AW24" s="195"/>
       <c r="BD24" s="2"/>
       <c r="BE24" s="2"/>
       <c r="BF24" s="2"/>
@@ -33609,59 +33613,59 @@
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="85"/>
-      <c r="B25" s="195" t="s">
+      <c r="B25" s="196" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="196" t="e">
+      <c r="C25" s="197" t="e">
         <f aca="false">SMALL(E13:T13,1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D25" s="197"/>
-      <c r="E25" s="197"/>
-      <c r="F25" s="197"/>
-      <c r="G25" s="198"/>
-      <c r="H25" s="199"/>
-      <c r="I25" s="199"/>
-      <c r="J25" s="199"/>
-      <c r="K25" s="199"/>
-      <c r="L25" s="199"/>
-      <c r="M25" s="199"/>
-      <c r="N25" s="199"/>
-      <c r="O25" s="199"/>
-      <c r="P25" s="199"/>
-      <c r="Q25" s="199"/>
-      <c r="R25" s="199"/>
-      <c r="S25" s="199"/>
-      <c r="T25" s="200"/>
-      <c r="U25" s="201"/>
-      <c r="V25" s="201"/>
-      <c r="W25" s="201"/>
-      <c r="X25" s="201"/>
-      <c r="Y25" s="201"/>
-      <c r="Z25" s="201"/>
-      <c r="AA25" s="201"/>
-      <c r="AB25" s="201"/>
-      <c r="AC25" s="201"/>
-      <c r="AD25" s="201"/>
-      <c r="AE25" s="201"/>
-      <c r="AF25" s="201"/>
-      <c r="AG25" s="201"/>
-      <c r="AH25" s="201"/>
-      <c r="AI25" s="201"/>
-      <c r="AJ25" s="201"/>
-      <c r="AK25" s="201"/>
-      <c r="AL25" s="201"/>
-      <c r="AM25" s="201"/>
-      <c r="AN25" s="201"/>
-      <c r="AO25" s="201"/>
-      <c r="AP25" s="201"/>
-      <c r="AQ25" s="201"/>
-      <c r="AR25" s="201"/>
-      <c r="AS25" s="201"/>
-      <c r="AT25" s="201"/>
-      <c r="AU25" s="201"/>
-      <c r="AV25" s="201"/>
-      <c r="AW25" s="201"/>
+      <c r="D25" s="198"/>
+      <c r="E25" s="198"/>
+      <c r="F25" s="198"/>
+      <c r="G25" s="199"/>
+      <c r="H25" s="200"/>
+      <c r="I25" s="200"/>
+      <c r="J25" s="200"/>
+      <c r="K25" s="200"/>
+      <c r="L25" s="200"/>
+      <c r="M25" s="200"/>
+      <c r="N25" s="200"/>
+      <c r="O25" s="200"/>
+      <c r="P25" s="200"/>
+      <c r="Q25" s="200"/>
+      <c r="R25" s="200"/>
+      <c r="S25" s="200"/>
+      <c r="T25" s="201"/>
+      <c r="U25" s="202"/>
+      <c r="V25" s="202"/>
+      <c r="W25" s="202"/>
+      <c r="X25" s="202"/>
+      <c r="Y25" s="202"/>
+      <c r="Z25" s="202"/>
+      <c r="AA25" s="202"/>
+      <c r="AB25" s="202"/>
+      <c r="AC25" s="202"/>
+      <c r="AD25" s="202"/>
+      <c r="AE25" s="202"/>
+      <c r="AF25" s="202"/>
+      <c r="AG25" s="202"/>
+      <c r="AH25" s="202"/>
+      <c r="AI25" s="202"/>
+      <c r="AJ25" s="202"/>
+      <c r="AK25" s="202"/>
+      <c r="AL25" s="202"/>
+      <c r="AM25" s="202"/>
+      <c r="AN25" s="202"/>
+      <c r="AO25" s="202"/>
+      <c r="AP25" s="202"/>
+      <c r="AQ25" s="202"/>
+      <c r="AR25" s="202"/>
+      <c r="AS25" s="202"/>
+      <c r="AT25" s="202"/>
+      <c r="AU25" s="202"/>
+      <c r="AV25" s="202"/>
+      <c r="AW25" s="202"/>
       <c r="BD25" s="2"/>
       <c r="BE25" s="2"/>
       <c r="BF25" s="2"/>
@@ -33679,60 +33683,60 @@
       <c r="BR25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="124"/>
-      <c r="B26" s="202" t="s">
+      <c r="A26" s="125"/>
+      <c r="B26" s="203" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="203" t="n">
+      <c r="C26" s="204" t="n">
         <f aca="false">SUM(Calculation!AD13:AD42)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="197"/>
-      <c r="E26" s="197"/>
-      <c r="F26" s="197"/>
-      <c r="G26" s="198"/>
-      <c r="H26" s="199"/>
-      <c r="I26" s="199"/>
-      <c r="J26" s="204"/>
-      <c r="K26" s="204"/>
-      <c r="L26" s="205"/>
-      <c r="M26" s="199"/>
-      <c r="N26" s="199"/>
-      <c r="O26" s="199"/>
-      <c r="P26" s="199"/>
-      <c r="Q26" s="199"/>
-      <c r="R26" s="199"/>
-      <c r="S26" s="199"/>
-      <c r="T26" s="200"/>
-      <c r="U26" s="201"/>
-      <c r="V26" s="201"/>
-      <c r="W26" s="201"/>
-      <c r="X26" s="201"/>
-      <c r="Y26" s="201"/>
-      <c r="Z26" s="201"/>
-      <c r="AA26" s="201"/>
-      <c r="AB26" s="201"/>
-      <c r="AC26" s="201"/>
-      <c r="AD26" s="201"/>
-      <c r="AE26" s="201"/>
-      <c r="AF26" s="201"/>
-      <c r="AG26" s="201"/>
-      <c r="AH26" s="201"/>
-      <c r="AI26" s="201"/>
-      <c r="AJ26" s="201"/>
-      <c r="AK26" s="201"/>
-      <c r="AL26" s="201"/>
-      <c r="AM26" s="201"/>
-      <c r="AN26" s="201"/>
-      <c r="AO26" s="201"/>
-      <c r="AP26" s="201"/>
-      <c r="AQ26" s="201"/>
-      <c r="AR26" s="201"/>
-      <c r="AS26" s="201"/>
-      <c r="AT26" s="201"/>
-      <c r="AU26" s="201"/>
-      <c r="AV26" s="201"/>
-      <c r="AW26" s="201"/>
+      <c r="D26" s="198"/>
+      <c r="E26" s="198"/>
+      <c r="F26" s="198"/>
+      <c r="G26" s="199"/>
+      <c r="H26" s="200"/>
+      <c r="I26" s="200"/>
+      <c r="J26" s="205"/>
+      <c r="K26" s="205"/>
+      <c r="L26" s="206"/>
+      <c r="M26" s="200"/>
+      <c r="N26" s="200"/>
+      <c r="O26" s="200"/>
+      <c r="P26" s="200"/>
+      <c r="Q26" s="200"/>
+      <c r="R26" s="200"/>
+      <c r="S26" s="200"/>
+      <c r="T26" s="201"/>
+      <c r="U26" s="202"/>
+      <c r="V26" s="202"/>
+      <c r="W26" s="202"/>
+      <c r="X26" s="202"/>
+      <c r="Y26" s="202"/>
+      <c r="Z26" s="202"/>
+      <c r="AA26" s="202"/>
+      <c r="AB26" s="202"/>
+      <c r="AC26" s="202"/>
+      <c r="AD26" s="202"/>
+      <c r="AE26" s="202"/>
+      <c r="AF26" s="202"/>
+      <c r="AG26" s="202"/>
+      <c r="AH26" s="202"/>
+      <c r="AI26" s="202"/>
+      <c r="AJ26" s="202"/>
+      <c r="AK26" s="202"/>
+      <c r="AL26" s="202"/>
+      <c r="AM26" s="202"/>
+      <c r="AN26" s="202"/>
+      <c r="AO26" s="202"/>
+      <c r="AP26" s="202"/>
+      <c r="AQ26" s="202"/>
+      <c r="AR26" s="202"/>
+      <c r="AS26" s="202"/>
+      <c r="AT26" s="202"/>
+      <c r="AU26" s="202"/>
+      <c r="AV26" s="202"/>
+      <c r="AW26" s="202"/>
       <c r="BD26" s="2"/>
       <c r="BE26" s="2"/>
       <c r="BF26" s="2"/>
@@ -33751,59 +33755,59 @@
     </row>
     <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="85"/>
-      <c r="B27" s="202" t="s">
+      <c r="B27" s="203" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="206" t="n">
+      <c r="C27" s="207" t="n">
         <f aca="false">SUM(Calculation!AC13:AC42)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="197"/>
-      <c r="E27" s="197"/>
-      <c r="F27" s="197"/>
-      <c r="G27" s="198"/>
-      <c r="H27" s="199"/>
-      <c r="I27" s="199"/>
-      <c r="J27" s="204"/>
-      <c r="K27" s="204"/>
-      <c r="L27" s="205"/>
-      <c r="M27" s="199"/>
-      <c r="N27" s="199"/>
-      <c r="O27" s="199"/>
-      <c r="P27" s="199"/>
-      <c r="Q27" s="199"/>
-      <c r="R27" s="199"/>
-      <c r="S27" s="199"/>
-      <c r="T27" s="200"/>
-      <c r="U27" s="201"/>
-      <c r="V27" s="201"/>
-      <c r="W27" s="201"/>
-      <c r="X27" s="201"/>
-      <c r="Y27" s="201"/>
-      <c r="Z27" s="201"/>
-      <c r="AA27" s="201"/>
-      <c r="AB27" s="201"/>
-      <c r="AC27" s="201"/>
-      <c r="AD27" s="201"/>
-      <c r="AE27" s="201"/>
-      <c r="AF27" s="201"/>
-      <c r="AG27" s="201"/>
-      <c r="AH27" s="201"/>
-      <c r="AI27" s="201"/>
-      <c r="AJ27" s="201"/>
-      <c r="AK27" s="201"/>
-      <c r="AL27" s="201"/>
-      <c r="AM27" s="201"/>
-      <c r="AN27" s="201"/>
-      <c r="AO27" s="201"/>
-      <c r="AP27" s="201"/>
-      <c r="AQ27" s="201"/>
-      <c r="AR27" s="201"/>
-      <c r="AS27" s="201"/>
-      <c r="AT27" s="201"/>
-      <c r="AU27" s="201"/>
-      <c r="AV27" s="201"/>
-      <c r="AW27" s="201"/>
+      <c r="D27" s="198"/>
+      <c r="E27" s="198"/>
+      <c r="F27" s="198"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="200"/>
+      <c r="I27" s="200"/>
+      <c r="J27" s="205"/>
+      <c r="K27" s="205"/>
+      <c r="L27" s="206"/>
+      <c r="M27" s="200"/>
+      <c r="N27" s="200"/>
+      <c r="O27" s="200"/>
+      <c r="P27" s="200"/>
+      <c r="Q27" s="200"/>
+      <c r="R27" s="200"/>
+      <c r="S27" s="200"/>
+      <c r="T27" s="201"/>
+      <c r="U27" s="202"/>
+      <c r="V27" s="202"/>
+      <c r="W27" s="202"/>
+      <c r="X27" s="202"/>
+      <c r="Y27" s="202"/>
+      <c r="Z27" s="202"/>
+      <c r="AA27" s="202"/>
+      <c r="AB27" s="202"/>
+      <c r="AC27" s="202"/>
+      <c r="AD27" s="202"/>
+      <c r="AE27" s="202"/>
+      <c r="AF27" s="202"/>
+      <c r="AG27" s="202"/>
+      <c r="AH27" s="202"/>
+      <c r="AI27" s="202"/>
+      <c r="AJ27" s="202"/>
+      <c r="AK27" s="202"/>
+      <c r="AL27" s="202"/>
+      <c r="AM27" s="202"/>
+      <c r="AN27" s="202"/>
+      <c r="AO27" s="202"/>
+      <c r="AP27" s="202"/>
+      <c r="AQ27" s="202"/>
+      <c r="AR27" s="202"/>
+      <c r="AS27" s="202"/>
+      <c r="AT27" s="202"/>
+      <c r="AU27" s="202"/>
+      <c r="AV27" s="202"/>
+      <c r="AW27" s="202"/>
       <c r="BD27" s="2"/>
       <c r="BE27" s="2"/>
       <c r="BF27" s="2"/>
@@ -33822,26 +33826,26 @@
     </row>
     <row r="28" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="85"/>
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="208" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="207"/>
-      <c r="D28" s="207"/>
-      <c r="E28" s="208" t="str">
+      <c r="C28" s="208"/>
+      <c r="D28" s="208"/>
+      <c r="E28" s="209" t="str">
         <f aca="false">'Data Entry'!$D$7</f>
         <v>GOOD</v>
       </c>
-      <c r="F28" s="209" t="str">
+      <c r="F28" s="210" t="str">
         <f aca="false">'Data Entry'!$D$8</f>
         <v>NO GOOD</v>
       </c>
-      <c r="G28" s="210" t="s">
+      <c r="G28" s="211" t="s">
         <v>87</v>
       </c>
       <c r="H28" s="116"/>
       <c r="I28" s="116"/>
-      <c r="J28" s="204"/>
-      <c r="K28" s="204"/>
+      <c r="J28" s="205"/>
+      <c r="K28" s="205"/>
       <c r="L28" s="116"/>
       <c r="M28" s="116"/>
       <c r="N28" s="116"/>
@@ -33937,25 +33941,25 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="85"/>
-      <c r="B29" s="207"/>
-      <c r="C29" s="207"/>
-      <c r="D29" s="207"/>
-      <c r="E29" s="211" t="n">
+      <c r="B29" s="208"/>
+      <c r="C29" s="208"/>
+      <c r="D29" s="208"/>
+      <c r="E29" s="212" t="n">
         <f aca="false">COUNTIF('Data Entry'!E13:AB42,'Statistical Report'!E28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="212" t="n">
+      <c r="F29" s="213" t="n">
         <f aca="false">COUNTIF('Data Entry'!E13:AB42,'Statistical Report'!F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="213" t="n">
+      <c r="G29" s="214" t="n">
         <f aca="false">E29+F29</f>
         <v>0</v>
       </c>
       <c r="H29" s="116"/>
       <c r="I29" s="116"/>
-      <c r="J29" s="204"/>
-      <c r="K29" s="204"/>
+      <c r="J29" s="205"/>
+      <c r="K29" s="205"/>
       <c r="L29" s="116"/>
       <c r="M29" s="116"/>
       <c r="N29" s="116"/>
@@ -34053,18 +34057,18 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="85"/>
-      <c r="B30" s="214"/>
-      <c r="C30" s="204"/>
-      <c r="D30" s="204"/>
-      <c r="E30" s="204"/>
+      <c r="B30" s="215"/>
+      <c r="C30" s="205"/>
+      <c r="D30" s="205"/>
+      <c r="E30" s="205"/>
       <c r="F30" s="116"/>
       <c r="G30" s="116"/>
       <c r="H30" s="116"/>
       <c r="I30" s="116"/>
       <c r="J30" s="116"/>
-      <c r="K30" s="204"/>
-      <c r="L30" s="204"/>
-      <c r="M30" s="204"/>
+      <c r="K30" s="205"/>
+      <c r="L30" s="205"/>
+      <c r="M30" s="205"/>
       <c r="N30" s="116"/>
       <c r="O30" s="116"/>
       <c r="P30" s="116"/>
@@ -34160,7 +34164,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="85"/>
-      <c r="B31" s="187"/>
+      <c r="B31" s="188"/>
       <c r="C31" s="116"/>
       <c r="D31" s="116"/>
       <c r="E31" s="116"/>
@@ -34169,9 +34173,9 @@
       <c r="H31" s="116"/>
       <c r="I31" s="116"/>
       <c r="J31" s="116"/>
-      <c r="K31" s="204"/>
-      <c r="L31" s="204"/>
-      <c r="M31" s="204"/>
+      <c r="K31" s="205"/>
+      <c r="L31" s="205"/>
+      <c r="M31" s="205"/>
       <c r="N31" s="116"/>
       <c r="O31" s="116"/>
       <c r="P31" s="116"/>
@@ -34267,16 +34271,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="85"/>
-      <c r="B32" s="163"/>
-      <c r="C32" s="215"/>
-      <c r="D32" s="215"/>
-      <c r="E32" s="215"/>
+      <c r="B32" s="164"/>
+      <c r="C32" s="216"/>
+      <c r="D32" s="216"/>
+      <c r="E32" s="216"/>
       <c r="F32" s="116"/>
       <c r="G32" s="116"/>
       <c r="H32" s="116"/>
       <c r="I32" s="116"/>
       <c r="J32" s="116"/>
-      <c r="K32" s="204"/>
+      <c r="K32" s="205"/>
       <c r="L32" s="116"/>
       <c r="M32" s="116"/>
       <c r="N32" s="116"/>
@@ -34374,16 +34378,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="85"/>
-      <c r="B33" s="163"/>
-      <c r="C33" s="216"/>
-      <c r="D33" s="216"/>
-      <c r="E33" s="216"/>
+      <c r="B33" s="164"/>
+      <c r="C33" s="217"/>
+      <c r="D33" s="217"/>
+      <c r="E33" s="217"/>
       <c r="F33" s="116"/>
       <c r="G33" s="116"/>
       <c r="H33" s="116"/>
       <c r="I33" s="116"/>
       <c r="J33" s="116"/>
-      <c r="K33" s="204"/>
+      <c r="K33" s="205"/>
       <c r="L33" s="116"/>
       <c r="M33" s="116"/>
       <c r="N33" s="116"/>
@@ -34481,16 +34485,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="85"/>
-      <c r="B34" s="187"/>
-      <c r="C34" s="217"/>
-      <c r="D34" s="217"/>
-      <c r="E34" s="217"/>
+      <c r="B34" s="188"/>
+      <c r="C34" s="218"/>
+      <c r="D34" s="218"/>
+      <c r="E34" s="218"/>
       <c r="F34" s="116"/>
       <c r="G34" s="116"/>
       <c r="H34" s="116"/>
       <c r="I34" s="116"/>
       <c r="J34" s="116"/>
-      <c r="K34" s="204"/>
+      <c r="K34" s="205"/>
       <c r="L34" s="116"/>
       <c r="M34" s="116"/>
       <c r="N34" s="116"/>
@@ -34588,7 +34592,7 @@
     </row>
     <row r="35" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="85"/>
-      <c r="B35" s="187"/>
+      <c r="B35" s="188"/>
       <c r="C35" s="116"/>
       <c r="D35" s="116"/>
       <c r="E35" s="116"/>
@@ -34597,15 +34601,15 @@
       <c r="H35" s="116"/>
       <c r="I35" s="116"/>
       <c r="J35" s="116"/>
-      <c r="K35" s="204"/>
+      <c r="K35" s="205"/>
       <c r="L35" s="116"/>
       <c r="M35" s="116"/>
       <c r="N35" s="116"/>
       <c r="O35" s="116"/>
-      <c r="P35" s="204"/>
-      <c r="Q35" s="204"/>
-      <c r="R35" s="204"/>
-      <c r="S35" s="204"/>
+      <c r="P35" s="205"/>
+      <c r="Q35" s="205"/>
+      <c r="R35" s="205"/>
+      <c r="S35" s="205"/>
       <c r="T35" s="118"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
@@ -34694,29 +34698,29 @@
       <c r="DA35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="218"/>
-      <c r="B36" s="219" t="s">
+      <c r="A36" s="219"/>
+      <c r="B36" s="220" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="220"/>
-      <c r="D36" s="220"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="221" t="s">
+      <c r="C36" s="221"/>
+      <c r="D36" s="221"/>
+      <c r="E36" s="221"/>
+      <c r="F36" s="222" t="s">
         <v>89</v>
       </c>
       <c r="G36" s="109"/>
       <c r="H36" s="109"/>
       <c r="I36" s="109"/>
       <c r="J36" s="113"/>
-      <c r="K36" s="204"/>
-      <c r="L36" s="204"/>
-      <c r="M36" s="204"/>
-      <c r="N36" s="204"/>
-      <c r="O36" s="204"/>
-      <c r="P36" s="204"/>
-      <c r="Q36" s="204"/>
-      <c r="R36" s="204"/>
-      <c r="S36" s="204"/>
+      <c r="K36" s="205"/>
+      <c r="L36" s="205"/>
+      <c r="M36" s="205"/>
+      <c r="N36" s="205"/>
+      <c r="O36" s="205"/>
+      <c r="P36" s="205"/>
+      <c r="Q36" s="205"/>
+      <c r="R36" s="205"/>
+      <c r="S36" s="205"/>
       <c r="T36" s="118"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
@@ -34806,32 +34810,32 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="85"/>
-      <c r="B37" s="222"/>
-      <c r="C37" s="223" t="s">
+      <c r="B37" s="223"/>
+      <c r="C37" s="224" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="224" t="s">
+      <c r="D37" s="225" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="225" t="s">
+      <c r="E37" s="226" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="226" t="s">
+      <c r="F37" s="227" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="227"/>
+      <c r="G37" s="228"/>
       <c r="H37" s="116"/>
       <c r="I37" s="116"/>
       <c r="J37" s="118"/>
-      <c r="K37" s="204"/>
-      <c r="L37" s="204"/>
-      <c r="M37" s="204"/>
-      <c r="N37" s="204"/>
-      <c r="O37" s="204"/>
-      <c r="P37" s="204"/>
-      <c r="Q37" s="204"/>
-      <c r="R37" s="204"/>
-      <c r="S37" s="204"/>
+      <c r="K37" s="205"/>
+      <c r="L37" s="205"/>
+      <c r="M37" s="205"/>
+      <c r="N37" s="205"/>
+      <c r="O37" s="205"/>
+      <c r="P37" s="205"/>
+      <c r="Q37" s="205"/>
+      <c r="R37" s="205"/>
+      <c r="S37" s="205"/>
       <c r="T37" s="118"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
@@ -34921,35 +34925,35 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="85"/>
-      <c r="B38" s="228" t="s">
+      <c r="B38" s="229" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="229" t="n">
+      <c r="C38" s="230" t="n">
         <v>0.1</v>
       </c>
-      <c r="D38" s="230" t="str">
+      <c r="D38" s="231" t="str">
         <f aca="false">E38*100&amp;"% - "&amp;C38*100&amp;"%"</f>
         <v>5% - 10%</v>
       </c>
-      <c r="E38" s="231" t="n">
+      <c r="E38" s="232" t="n">
         <v>0.05</v>
       </c>
-      <c r="F38" s="232" t="s">
+      <c r="F38" s="233" t="s">
         <v>95</v>
       </c>
-      <c r="G38" s="227"/>
+      <c r="G38" s="228"/>
       <c r="H38" s="116"/>
       <c r="I38" s="116"/>
       <c r="J38" s="118"/>
-      <c r="K38" s="204"/>
-      <c r="L38" s="204"/>
-      <c r="M38" s="204"/>
-      <c r="N38" s="204"/>
-      <c r="O38" s="204"/>
-      <c r="P38" s="204"/>
-      <c r="Q38" s="204"/>
-      <c r="R38" s="204"/>
-      <c r="S38" s="204"/>
+      <c r="K38" s="205"/>
+      <c r="L38" s="205"/>
+      <c r="M38" s="205"/>
+      <c r="N38" s="205"/>
+      <c r="O38" s="205"/>
+      <c r="P38" s="205"/>
+      <c r="Q38" s="205"/>
+      <c r="R38" s="205"/>
+      <c r="S38" s="205"/>
       <c r="T38" s="118"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
@@ -35039,35 +35043,35 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="85"/>
-      <c r="B39" s="179" t="s">
+      <c r="B39" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="229" t="n">
+      <c r="C39" s="230" t="n">
         <v>0.05</v>
       </c>
-      <c r="D39" s="230" t="str">
+      <c r="D39" s="231" t="str">
         <f aca="false">E39*100&amp;"% - "&amp;C39*100&amp;"%"</f>
         <v>2% - 5%</v>
       </c>
-      <c r="E39" s="231" t="n">
+      <c r="E39" s="232" t="n">
         <v>0.02</v>
       </c>
-      <c r="F39" s="232" t="s">
+      <c r="F39" s="233" t="s">
         <v>97</v>
       </c>
-      <c r="G39" s="227"/>
+      <c r="G39" s="228"/>
       <c r="H39" s="116"/>
       <c r="I39" s="116"/>
       <c r="J39" s="118"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="204"/>
-      <c r="M39" s="204"/>
-      <c r="N39" s="204"/>
-      <c r="O39" s="204"/>
-      <c r="P39" s="204"/>
-      <c r="Q39" s="204"/>
-      <c r="R39" s="204"/>
-      <c r="S39" s="204"/>
+      <c r="K39" s="205"/>
+      <c r="L39" s="205"/>
+      <c r="M39" s="205"/>
+      <c r="N39" s="205"/>
+      <c r="O39" s="205"/>
+      <c r="P39" s="205"/>
+      <c r="Q39" s="205"/>
+      <c r="R39" s="205"/>
+      <c r="S39" s="205"/>
       <c r="T39" s="118"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
@@ -35157,31 +35161,31 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="85"/>
-      <c r="B40" s="179" t="s">
+      <c r="B40" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="233" t="n">
+      <c r="C40" s="234" t="n">
         <v>0.8</v>
       </c>
-      <c r="D40" s="230" t="str">
+      <c r="D40" s="231" t="str">
         <f aca="false">C40*100&amp;"% - "&amp;E40*100&amp;"%"</f>
         <v>80% - 90%</v>
       </c>
-      <c r="E40" s="234" t="n">
+      <c r="E40" s="235" t="n">
         <v>0.9</v>
       </c>
-      <c r="F40" s="235" t="s">
+      <c r="F40" s="236" t="s">
         <v>99</v>
       </c>
-      <c r="G40" s="236"/>
-      <c r="H40" s="236"/>
-      <c r="I40" s="236"/>
-      <c r="J40" s="237"/>
-      <c r="K40" s="204"/>
-      <c r="L40" s="204"/>
-      <c r="M40" s="204"/>
-      <c r="N40" s="204"/>
-      <c r="O40" s="204"/>
+      <c r="G40" s="237"/>
+      <c r="H40" s="237"/>
+      <c r="I40" s="237"/>
+      <c r="J40" s="238"/>
+      <c r="K40" s="205"/>
+      <c r="L40" s="205"/>
+      <c r="M40" s="205"/>
+      <c r="N40" s="205"/>
+      <c r="O40" s="205"/>
       <c r="P40" s="116"/>
       <c r="Q40" s="116"/>
       <c r="R40" s="116"/>
@@ -35275,29 +35279,29 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="85"/>
-      <c r="B41" s="238" t="s">
+      <c r="B41" s="239" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="239" t="n">
+      <c r="C41" s="240" t="n">
         <v>0.4</v>
       </c>
-      <c r="D41" s="240" t="str">
+      <c r="D41" s="241" t="str">
         <f aca="false">C41&amp;" - "&amp;E41</f>
         <v>0,4 - 0,75</v>
       </c>
-      <c r="E41" s="241" t="n">
+      <c r="E41" s="242" t="n">
         <v>0.75</v>
       </c>
-      <c r="F41" s="242"/>
-      <c r="G41" s="243"/>
-      <c r="H41" s="243"/>
-      <c r="I41" s="243"/>
-      <c r="J41" s="244"/>
-      <c r="K41" s="204"/>
-      <c r="L41" s="204"/>
-      <c r="M41" s="204"/>
-      <c r="N41" s="204"/>
-      <c r="O41" s="204"/>
+      <c r="F41" s="243"/>
+      <c r="G41" s="244"/>
+      <c r="H41" s="244"/>
+      <c r="I41" s="244"/>
+      <c r="J41" s="245"/>
+      <c r="K41" s="205"/>
+      <c r="L41" s="205"/>
+      <c r="M41" s="205"/>
+      <c r="N41" s="205"/>
+      <c r="O41" s="205"/>
       <c r="P41" s="116"/>
       <c r="Q41" s="116"/>
       <c r="R41" s="116"/>
@@ -35390,17 +35394,17 @@
       <c r="DA41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="245"/>
-      <c r="B42" s="246" t="s">
+      <c r="A42" s="246"/>
+      <c r="B42" s="247" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="247"/>
-      <c r="D42" s="247"/>
-      <c r="E42" s="247"/>
-      <c r="F42" s="248"/>
-      <c r="G42" s="248"/>
-      <c r="H42" s="248"/>
-      <c r="I42" s="248"/>
+      <c r="C42" s="248"/>
+      <c r="D42" s="248"/>
+      <c r="E42" s="248"/>
+      <c r="F42" s="249"/>
+      <c r="G42" s="249"/>
+      <c r="H42" s="249"/>
+      <c r="I42" s="249"/>
       <c r="J42" s="116"/>
       <c r="K42" s="116"/>
       <c r="L42" s="116"/>
@@ -35500,7 +35504,7 @@
     </row>
     <row r="43" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="85"/>
-      <c r="B43" s="187"/>
+      <c r="B43" s="188"/>
       <c r="C43" s="116"/>
       <c r="D43" s="116"/>
       <c r="E43" s="116"/>
@@ -35606,21 +35610,21 @@
       <c r="DA43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="218"/>
-      <c r="B44" s="219" t="s">
+      <c r="A44" s="219"/>
+      <c r="B44" s="220" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="249" t="str">
+      <c r="C44" s="250" t="str">
         <f aca="false">IF(COUNTIF(C15:CL21,C37)&gt;0,C37,IF(COUNTIF(C15:CL21,D37)&gt;0,D37,E37))</f>
         <v>Accept</v>
       </c>
-      <c r="D44" s="249"/>
-      <c r="E44" s="220"/>
-      <c r="F44" s="220"/>
-      <c r="G44" s="220"/>
-      <c r="H44" s="220"/>
-      <c r="I44" s="220"/>
-      <c r="J44" s="250"/>
+      <c r="D44" s="250"/>
+      <c r="E44" s="221"/>
+      <c r="F44" s="221"/>
+      <c r="G44" s="221"/>
+      <c r="H44" s="221"/>
+      <c r="I44" s="221"/>
+      <c r="J44" s="251"/>
       <c r="K44" s="116"/>
       <c r="L44" s="116"/>
       <c r="M44" s="116"/>
@@ -35718,8 +35722,8 @@
       <c r="DA44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="124"/>
-      <c r="B45" s="251" t="s">
+      <c r="A45" s="125"/>
+      <c r="B45" s="252" t="s">
         <v>103</v>
       </c>
       <c r="C45" s="109"/>
@@ -35828,7 +35832,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="85"/>
-      <c r="B46" s="187"/>
+      <c r="B46" s="188"/>
       <c r="C46" s="116"/>
       <c r="D46" s="116"/>
       <c r="E46" s="116"/>
@@ -35935,7 +35939,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="85"/>
-      <c r="B47" s="187"/>
+      <c r="B47" s="188"/>
       <c r="C47" s="116"/>
       <c r="D47" s="116"/>
       <c r="E47" s="116"/>
@@ -36042,7 +36046,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="85"/>
-      <c r="B48" s="187"/>
+      <c r="B48" s="188"/>
       <c r="C48" s="116"/>
       <c r="D48" s="116"/>
       <c r="E48" s="116"/>
@@ -36149,7 +36153,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="85"/>
-      <c r="B49" s="187"/>
+      <c r="B49" s="188"/>
       <c r="C49" s="116"/>
       <c r="D49" s="116"/>
       <c r="E49" s="116"/>
@@ -36256,17 +36260,17 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="85"/>
-      <c r="B50" s="252" t="s">
+      <c r="B50" s="253" t="s">
         <v>104</v>
       </c>
       <c r="C50" s="109"/>
       <c r="D50" s="113"/>
-      <c r="E50" s="252" t="s">
+      <c r="E50" s="253" t="s">
         <v>105</v>
       </c>
       <c r="F50" s="109"/>
       <c r="G50" s="113"/>
-      <c r="H50" s="252" t="s">
+      <c r="H50" s="253" t="s">
         <v>106</v>
       </c>
       <c r="I50" s="109"/>
@@ -36369,13 +36373,13 @@
     </row>
     <row r="51" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="85"/>
-      <c r="B51" s="187"/>
+      <c r="B51" s="188"/>
       <c r="C51" s="116"/>
       <c r="D51" s="118"/>
-      <c r="E51" s="187"/>
+      <c r="E51" s="188"/>
       <c r="F51" s="116"/>
       <c r="G51" s="118"/>
-      <c r="H51" s="187"/>
+      <c r="H51" s="188"/>
       <c r="I51" s="116"/>
       <c r="J51" s="118"/>
       <c r="K51" s="116"/>
@@ -36476,13 +36480,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="85"/>
-      <c r="B52" s="187"/>
+      <c r="B52" s="188"/>
       <c r="C52" s="116"/>
       <c r="D52" s="118"/>
-      <c r="E52" s="187"/>
+      <c r="E52" s="188"/>
       <c r="F52" s="116"/>
       <c r="G52" s="118"/>
-      <c r="H52" s="187"/>
+      <c r="H52" s="188"/>
       <c r="I52" s="116"/>
       <c r="J52" s="118"/>
       <c r="K52" s="116"/>
@@ -36583,37 +36587,37 @@
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="85"/>
-      <c r="B53" s="253" t="s">
+      <c r="B53" s="254" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="254"/>
-      <c r="D53" s="255" t="s">
+      <c r="C53" s="255"/>
+      <c r="D53" s="256" t="s">
         <v>108</v>
       </c>
-      <c r="E53" s="253" t="s">
+      <c r="E53" s="254" t="s">
         <v>107</v>
       </c>
-      <c r="F53" s="254"/>
-      <c r="G53" s="255" t="s">
+      <c r="F53" s="255"/>
+      <c r="G53" s="256" t="s">
         <v>108</v>
       </c>
-      <c r="H53" s="253" t="s">
+      <c r="H53" s="254" t="s">
         <v>107</v>
       </c>
-      <c r="I53" s="254"/>
-      <c r="J53" s="255" t="s">
+      <c r="I53" s="255"/>
+      <c r="J53" s="256" t="s">
         <v>108</v>
       </c>
-      <c r="K53" s="256"/>
-      <c r="L53" s="256"/>
-      <c r="M53" s="256"/>
-      <c r="N53" s="256"/>
-      <c r="O53" s="256"/>
-      <c r="P53" s="256"/>
-      <c r="Q53" s="256"/>
-      <c r="R53" s="256"/>
-      <c r="S53" s="256"/>
-      <c r="T53" s="257"/>
+      <c r="K53" s="257"/>
+      <c r="L53" s="257"/>
+      <c r="M53" s="257"/>
+      <c r="N53" s="257"/>
+      <c r="O53" s="257"/>
+      <c r="P53" s="257"/>
+      <c r="Q53" s="257"/>
+      <c r="R53" s="257"/>
+      <c r="S53" s="257"/>
+      <c r="T53" s="258"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>

</xml_diff>